<commit_message>
perbaikan data & judul NERS
</commit_message>
<xml_diff>
--- a/Ners/2023-2024/Transkip Nilai Ners 2023-2024.xlsx
+++ b/Ners/2023-2024/Transkip Nilai Ners 2023-2024.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Nando\Documents\Stikes\Transkip Nilai 2025\Ners\2023-2024\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{655A8221-F51A-4E3C-BA56-4293B80A89E9}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1EEBA472-A362-4A85-A11C-A08D86520544}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{435B60B8-694F-4DDA-ADD2-15262503367A}"/>
+    <workbookView xWindow="-98" yWindow="-98" windowWidth="21795" windowHeight="12975" xr2:uid="{435B60B8-694F-4DDA-ADD2-15262503367A}"/>
   </bookViews>
   <sheets>
     <sheet name="Transkip" sheetId="1" r:id="rId1"/>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="400" uniqueCount="243">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="401" uniqueCount="244">
   <si>
     <t>NO</t>
   </si>
@@ -480,9 +480,6 @@
     <t>Kuala Tungkal</t>
   </si>
   <si>
-    <t>22 Februari 1986</t>
-  </si>
-  <si>
     <t>30 Januari 1981</t>
   </si>
   <si>
@@ -591,9 +588,6 @@
     <t>Asuhan Keperawatan Ketidakstabilan Kadar Glukosa Darah Pada Ny. J Dengan Diabetes Mellitus Dan Penerapan Terapi Dzikir Di Ruang Zaal Wanita Rsud Dabo Tahun 2023</t>
   </si>
   <si>
-    <t>Asuhan Keperawatan Gangguan Tumbuh Kembang Pada Keluarga Tn.C Dengan Stunting Dan Penerapan Pijat Tui Na Di Rt 01 Rw 02 Kelurahan Raya Kecamatan Singkep Barat Tahun 2024</t>
-  </si>
-  <si>
     <t>Asuhan Keperawatan Nyeri Akut Pada Nn. J Asdengan Post Appendictomy Dan Penerapan Relaksasi Benson Di Rsud Dabo Tahun 2023</t>
   </si>
   <si>
@@ -762,14 +756,44 @@
     <t>ASUHAN KEPERAWATAN HALUSINASI PADA NN.L DENGAN SKIZOFRENIA PARANOID DAN PENERAPAN STRATEGI PELAKSANAAN HALUSINASI DI WILAYAH DAIK LINGGA TAHUN 2024</t>
   </si>
   <si>
-    <t>Asuhan Keperawatan Gangguan Integeritas Kulit Pada An.A Dengan Luka Bakar Dan Penerapan Aloevera Di Paviliun Cindai Rsud Encik Maryam Kabupatern Lingga</t>
+    <t>22 Februari 1985</t>
+  </si>
+  <si>
+    <t>ASUHAN KEPERAWATAN GANGGUAN TUMBUH KEMBANG AN.ER DENGAN STUNTING PADA KELUARGA TN.C DAN PENERAPAN PIJAT TUI NA DI RT 01 RW 02 KELURAHAN RAYA KECAMATAN SINGKEP BARAT TAHUN 2024</t>
+  </si>
+  <si>
+    <t>Asuhan Keperawatan Gangguan Integeritas Kulit Pada An.A Dengan Luka Bakar Dan Penerapan Aloevera Di Paviliun Cindai Rsud Encik Maryam Kabupaten Lingga</t>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">Asuhan Keperawatan Bersihan Jalan Nafas Tidak Efektif Pada Tn. R Dengan Penerapan Batuk Efektif &amp; Teknik Pernafasan </t>
+    </r>
+    <r>
+      <rPr>
+        <i/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+      </rPr>
+      <t>Pursed Lips Breathing</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+      </rPr>
+      <t xml:space="preserve"> di Ruang Rawat Inap RSUD Palmatak</t>
+    </r>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="14" x14ac:knownFonts="1">
+  <fonts count="15" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -855,6 +879,13 @@
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
+    </font>
+    <font>
+      <i/>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Arial"/>
+      <family val="2"/>
     </font>
   </fonts>
   <fills count="15">
@@ -974,7 +1005,7 @@
       <alignment vertical="center"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="114">
+  <cellXfs count="115">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="10" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -1262,28 +1293,19 @@
     <xf numFmtId="0" fontId="7" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="9" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="10" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="1" fillId="11" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="12" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="13" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="5" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -1298,20 +1320,32 @@
     <xf numFmtId="0" fontId="1" fillId="8" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="49" fontId="1" fillId="2" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="1" fillId="9" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="10" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="12" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="13" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="14" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="1" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="11" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="12" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
+    <xf numFmtId="49" fontId="1" fillId="2" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="3">
@@ -1632,137 +1666,137 @@
   <dimension ref="A1:BW47"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <pane xSplit="2" ySplit="2" topLeftCell="AZ33" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="2" ySplit="2" topLeftCell="AN13" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="C1" sqref="C1"/>
       <selection pane="bottomLeft" activeCell="A3" sqref="A3"/>
-      <selection pane="bottomRight" activeCell="BW41" sqref="BW41"/>
+      <selection pane="bottomRight" activeCell="BW20" sqref="BW20"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
   <cols>
     <col min="1" max="1" width="8" customWidth="1"/>
-    <col min="2" max="2" width="30.140625" customWidth="1"/>
+    <col min="2" max="2" width="30.1328125" customWidth="1"/>
     <col min="3" max="3" width="18" customWidth="1"/>
-    <col min="4" max="4" width="20.28515625" customWidth="1"/>
-    <col min="5" max="5" width="20.28515625" style="74" customWidth="1"/>
-    <col min="6" max="6" width="24.42578125" style="77" customWidth="1"/>
-    <col min="7" max="7" width="20.28515625" style="76" customWidth="1"/>
-    <col min="8" max="8" width="20.28515625" customWidth="1"/>
-    <col min="9" max="46" width="6.7109375" customWidth="1"/>
+    <col min="4" max="4" width="20.265625" customWidth="1"/>
+    <col min="5" max="5" width="20.265625" style="74" customWidth="1"/>
+    <col min="6" max="6" width="24.3984375" style="77" customWidth="1"/>
+    <col min="7" max="7" width="20.265625" style="76" customWidth="1"/>
+    <col min="8" max="8" width="20.265625" customWidth="1"/>
+    <col min="9" max="46" width="6.73046875" customWidth="1"/>
     <col min="47" max="47" width="8" customWidth="1"/>
-    <col min="48" max="48" width="6.7109375" customWidth="1"/>
-    <col min="49" max="49" width="8.140625" customWidth="1"/>
-    <col min="50" max="53" width="6.7109375" customWidth="1"/>
-    <col min="54" max="54" width="8.28515625" customWidth="1"/>
-    <col min="55" max="63" width="6.7109375" customWidth="1"/>
-    <col min="64" max="64" width="8.140625" customWidth="1"/>
-    <col min="65" max="65" width="6.7109375" customWidth="1"/>
-    <col min="66" max="66" width="8.28515625" customWidth="1"/>
-    <col min="68" max="68" width="6.7109375" customWidth="1"/>
-    <col min="69" max="69" width="8.85546875" customWidth="1"/>
-    <col min="70" max="70" width="11.140625" customWidth="1"/>
+    <col min="48" max="48" width="6.73046875" customWidth="1"/>
+    <col min="49" max="49" width="8.1328125" customWidth="1"/>
+    <col min="50" max="53" width="6.73046875" customWidth="1"/>
+    <col min="54" max="54" width="8.265625" customWidth="1"/>
+    <col min="55" max="63" width="6.73046875" customWidth="1"/>
+    <col min="64" max="64" width="8.1328125" customWidth="1"/>
+    <col min="65" max="65" width="6.73046875" customWidth="1"/>
+    <col min="66" max="66" width="8.265625" customWidth="1"/>
+    <col min="68" max="68" width="6.73046875" customWidth="1"/>
+    <col min="69" max="69" width="8.86328125" customWidth="1"/>
+    <col min="70" max="70" width="11.1328125" customWidth="1"/>
     <col min="71" max="71" width="10" customWidth="1"/>
-    <col min="72" max="72" width="13.42578125" customWidth="1"/>
-    <col min="73" max="73" width="18.140625" customWidth="1"/>
-    <col min="74" max="74" width="17.85546875" customWidth="1"/>
-    <col min="75" max="75" width="27.28515625" customWidth="1"/>
+    <col min="72" max="72" width="13.3984375" customWidth="1"/>
+    <col min="73" max="73" width="18.1328125" customWidth="1"/>
+    <col min="74" max="74" width="17.86328125" customWidth="1"/>
+    <col min="75" max="75" width="27.265625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:75" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A1" s="98" t="s">
+    <row r="1" spans="1:75" ht="15" x14ac:dyDescent="0.45">
+      <c r="A1" s="100" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="98" t="s">
+      <c r="B1" s="100" t="s">
         <v>1</v>
       </c>
-      <c r="C1" s="98" t="s">
+      <c r="C1" s="100" t="s">
         <v>2</v>
       </c>
-      <c r="D1" s="98" t="s">
-        <v>3</v>
-      </c>
-      <c r="E1" s="98" t="s">
+      <c r="D1" s="100" t="s">
+        <v>3</v>
+      </c>
+      <c r="E1" s="100" t="s">
         <v>73</v>
       </c>
-      <c r="F1" s="109" t="s">
+      <c r="F1" s="113" t="s">
         <v>74</v>
       </c>
-      <c r="G1" s="109" t="s">
+      <c r="G1" s="113" t="s">
         <v>75</v>
       </c>
-      <c r="H1" s="98" t="s">
+      <c r="H1" s="100" t="s">
         <v>76</v>
       </c>
-      <c r="I1" s="99" t="s">
-        <v>4</v>
-      </c>
-      <c r="J1" s="99"/>
-      <c r="K1" s="99"/>
-      <c r="L1" s="99"/>
-      <c r="M1" s="99"/>
-      <c r="N1" s="97" t="s">
+      <c r="I1" s="112" t="s">
+        <v>4</v>
+      </c>
+      <c r="J1" s="112"/>
+      <c r="K1" s="112"/>
+      <c r="L1" s="112"/>
+      <c r="M1" s="112"/>
+      <c r="N1" s="111" t="s">
         <v>5</v>
       </c>
-      <c r="O1" s="97"/>
-      <c r="P1" s="97"/>
-      <c r="Q1" s="97"/>
-      <c r="R1" s="97"/>
-      <c r="S1" s="105" t="s">
+      <c r="O1" s="111"/>
+      <c r="P1" s="111"/>
+      <c r="Q1" s="111"/>
+      <c r="R1" s="111"/>
+      <c r="S1" s="102" t="s">
         <v>6</v>
       </c>
-      <c r="T1" s="105"/>
-      <c r="U1" s="105"/>
-      <c r="V1" s="105"/>
-      <c r="W1" s="105"/>
-      <c r="X1" s="106" t="s">
+      <c r="T1" s="102"/>
+      <c r="U1" s="102"/>
+      <c r="V1" s="102"/>
+      <c r="W1" s="102"/>
+      <c r="X1" s="103" t="s">
         <v>7</v>
       </c>
-      <c r="Y1" s="106"/>
-      <c r="Z1" s="106"/>
-      <c r="AA1" s="106"/>
-      <c r="AB1" s="106"/>
-      <c r="AC1" s="107" t="s">
+      <c r="Y1" s="103"/>
+      <c r="Z1" s="103"/>
+      <c r="AA1" s="103"/>
+      <c r="AB1" s="103"/>
+      <c r="AC1" s="104" t="s">
         <v>8</v>
       </c>
-      <c r="AD1" s="107"/>
-      <c r="AE1" s="107"/>
-      <c r="AF1" s="107"/>
-      <c r="AG1" s="107"/>
-      <c r="AH1" s="108" t="s">
+      <c r="AD1" s="104"/>
+      <c r="AE1" s="104"/>
+      <c r="AF1" s="104"/>
+      <c r="AG1" s="104"/>
+      <c r="AH1" s="105" t="s">
         <v>9</v>
       </c>
-      <c r="AI1" s="108"/>
-      <c r="AJ1" s="108"/>
-      <c r="AK1" s="108"/>
-      <c r="AL1" s="108"/>
-      <c r="AM1" s="101" t="s">
+      <c r="AI1" s="105"/>
+      <c r="AJ1" s="105"/>
+      <c r="AK1" s="105"/>
+      <c r="AL1" s="105"/>
+      <c r="AM1" s="107" t="s">
         <v>13</v>
       </c>
-      <c r="AN1" s="101"/>
-      <c r="AO1" s="101"/>
-      <c r="AP1" s="101"/>
-      <c r="AQ1" s="101"/>
-      <c r="AR1" s="102" t="s">
+      <c r="AN1" s="107"/>
+      <c r="AO1" s="107"/>
+      <c r="AP1" s="107"/>
+      <c r="AQ1" s="107"/>
+      <c r="AR1" s="101" t="s">
         <v>14</v>
       </c>
-      <c r="AS1" s="102"/>
-      <c r="AT1" s="102"/>
-      <c r="AU1" s="102"/>
-      <c r="AV1" s="102"/>
-      <c r="AW1" s="103" t="s">
+      <c r="AS1" s="101"/>
+      <c r="AT1" s="101"/>
+      <c r="AU1" s="101"/>
+      <c r="AV1" s="101"/>
+      <c r="AW1" s="108" t="s">
         <v>15</v>
       </c>
-      <c r="AX1" s="103"/>
-      <c r="AY1" s="103"/>
-      <c r="AZ1" s="103"/>
-      <c r="BA1" s="103"/>
-      <c r="BB1" s="104" t="s">
+      <c r="AX1" s="108"/>
+      <c r="AY1" s="108"/>
+      <c r="AZ1" s="108"/>
+      <c r="BA1" s="108"/>
+      <c r="BB1" s="109" t="s">
         <v>16</v>
       </c>
-      <c r="BC1" s="104"/>
-      <c r="BD1" s="104"/>
-      <c r="BE1" s="104"/>
-      <c r="BF1" s="104"/>
+      <c r="BC1" s="109"/>
+      <c r="BD1" s="109"/>
+      <c r="BE1" s="109"/>
+      <c r="BF1" s="109"/>
       <c r="BG1" s="110" t="s">
         <v>17</v>
       </c>
@@ -1770,22 +1804,22 @@
       <c r="BI1" s="110"/>
       <c r="BJ1" s="110"/>
       <c r="BK1" s="110"/>
-      <c r="BL1" s="100" t="s">
+      <c r="BL1" s="106" t="s">
         <v>10</v>
       </c>
-      <c r="BM1" s="100" t="s">
+      <c r="BM1" s="106" t="s">
         <v>11</v>
       </c>
-      <c r="BN1" s="100" t="s">
+      <c r="BN1" s="106" t="s">
         <v>12</v>
       </c>
-      <c r="BO1" s="98" t="s">
+      <c r="BO1" s="100" t="s">
         <v>10</v>
       </c>
-      <c r="BP1" s="98" t="s">
+      <c r="BP1" s="100" t="s">
         <v>11</v>
       </c>
-      <c r="BQ1" s="98" t="s">
+      <c r="BQ1" s="100" t="s">
         <v>12</v>
       </c>
       <c r="BR1" s="2" t="s">
@@ -1794,28 +1828,28 @@
       <c r="BS1" s="2" t="s">
         <v>18</v>
       </c>
-      <c r="BT1" s="102" t="s">
+      <c r="BT1" s="101" t="s">
         <v>19</v>
       </c>
-      <c r="BU1" s="111" t="s">
+      <c r="BU1" s="99" t="s">
         <v>77</v>
       </c>
-      <c r="BV1" s="111" t="s">
+      <c r="BV1" s="99" t="s">
         <v>78</v>
       </c>
-      <c r="BW1" s="111" t="s">
+      <c r="BW1" s="99" t="s">
         <v>79</v>
       </c>
     </row>
-    <row r="2" spans="1:75" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A2" s="98"/>
-      <c r="B2" s="98"/>
-      <c r="C2" s="98"/>
-      <c r="D2" s="98"/>
-      <c r="E2" s="98"/>
-      <c r="F2" s="109"/>
-      <c r="G2" s="109"/>
-      <c r="H2" s="98"/>
+    <row r="2" spans="1:75" ht="15" x14ac:dyDescent="0.45">
+      <c r="A2" s="100"/>
+      <c r="B2" s="100"/>
+      <c r="C2" s="100"/>
+      <c r="D2" s="100"/>
+      <c r="E2" s="100"/>
+      <c r="F2" s="113"/>
+      <c r="G2" s="113"/>
+      <c r="H2" s="100"/>
       <c r="I2" s="7" t="s">
         <v>20</v>
       </c>
@@ -1981,24 +2015,24 @@
       <c r="BK2" s="5" t="s">
         <v>24</v>
       </c>
-      <c r="BL2" s="100"/>
-      <c r="BM2" s="100"/>
-      <c r="BN2" s="100"/>
-      <c r="BO2" s="98"/>
-      <c r="BP2" s="98"/>
-      <c r="BQ2" s="98"/>
+      <c r="BL2" s="106"/>
+      <c r="BM2" s="106"/>
+      <c r="BN2" s="106"/>
+      <c r="BO2" s="100"/>
+      <c r="BP2" s="100"/>
+      <c r="BQ2" s="100"/>
       <c r="BR2" s="2" t="s">
         <v>20</v>
       </c>
       <c r="BS2" s="2" t="s">
         <v>25</v>
       </c>
-      <c r="BT2" s="102"/>
-      <c r="BU2" s="111"/>
-      <c r="BV2" s="111"/>
-      <c r="BW2" s="111"/>
+      <c r="BT2" s="101"/>
+      <c r="BU2" s="99"/>
+      <c r="BV2" s="99"/>
+      <c r="BW2" s="99"/>
     </row>
-    <row r="3" spans="1:75" ht="30" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:75" ht="15" x14ac:dyDescent="0.45">
       <c r="A3" s="16">
         <v>1</v>
       </c>
@@ -2021,7 +2055,7 @@
         <v>112</v>
       </c>
       <c r="H3" s="16" t="s">
-        <v>195</v>
+        <v>193</v>
       </c>
       <c r="I3" s="17">
         <v>76</v>
@@ -2266,11 +2300,11 @@
         <f>IF(BT3&gt;=3.51,"Excellent",(IF(BT3&gt;=2.75,"Highly Satisfactory",(IF(BT3&gt;=2,"Satisfactory","FAILED")))))</f>
         <v>Highly Satisfactory</v>
       </c>
-      <c r="BW3" s="112" t="s">
-        <v>157</v>
+      <c r="BW3" s="97" t="s">
+        <v>156</v>
       </c>
     </row>
-    <row r="4" spans="1:75" ht="30" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:75" ht="15" x14ac:dyDescent="0.45">
       <c r="A4" s="16">
         <v>2</v>
       </c>
@@ -2293,7 +2327,7 @@
         <v>113</v>
       </c>
       <c r="H4" s="16" t="s">
-        <v>196</v>
+        <v>194</v>
       </c>
       <c r="I4" s="17">
         <v>76</v>
@@ -2539,10 +2573,10 @@
         <v>Highly Satisfactory</v>
       </c>
       <c r="BW4" s="95" t="s">
-        <v>158</v>
+        <v>157</v>
       </c>
     </row>
-    <row r="5" spans="1:75" ht="30" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:75" ht="15" x14ac:dyDescent="0.45">
       <c r="A5" s="16">
         <v>3</v>
       </c>
@@ -2565,7 +2599,7 @@
         <v>112</v>
       </c>
       <c r="H5" s="16" t="s">
-        <v>197</v>
+        <v>195</v>
       </c>
       <c r="I5" s="17">
         <v>77</v>
@@ -2812,7 +2846,7 @@
       </c>
       <c r="BW5" s="95"/>
     </row>
-    <row r="6" spans="1:75" ht="30" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:75" ht="15" x14ac:dyDescent="0.45">
       <c r="A6" s="16">
         <v>4</v>
       </c>
@@ -2835,7 +2869,7 @@
         <v>112</v>
       </c>
       <c r="H6" s="16" t="s">
-        <v>198</v>
+        <v>196</v>
       </c>
       <c r="I6" s="17">
         <v>76</v>
@@ -3080,11 +3114,11 @@
         <f t="shared" si="43"/>
         <v>Excellent</v>
       </c>
-      <c r="BW6" s="112" t="s">
-        <v>159</v>
+      <c r="BW6" s="97" t="s">
+        <v>158</v>
       </c>
     </row>
-    <row r="7" spans="1:75" ht="30" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:75" ht="15" x14ac:dyDescent="0.45">
       <c r="A7" s="16">
         <v>5</v>
       </c>
@@ -3107,7 +3141,7 @@
         <v>112</v>
       </c>
       <c r="H7" s="16" t="s">
-        <v>199</v>
+        <v>197</v>
       </c>
       <c r="I7" s="17">
         <v>77</v>
@@ -3353,10 +3387,10 @@
         <v>Excellent</v>
       </c>
       <c r="BW7" s="95" t="s">
-        <v>160</v>
+        <v>159</v>
       </c>
     </row>
-    <row r="8" spans="1:75" ht="30" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:75" ht="15" x14ac:dyDescent="0.45">
       <c r="A8" s="16">
         <v>6</v>
       </c>
@@ -3379,7 +3413,7 @@
         <v>113</v>
       </c>
       <c r="H8" s="16" t="s">
-        <v>200</v>
+        <v>198</v>
       </c>
       <c r="I8" s="17">
         <v>75</v>
@@ -3625,10 +3659,10 @@
         <v>Highly Satisfactory</v>
       </c>
       <c r="BW8" s="95" t="s">
-        <v>161</v>
+        <v>160</v>
       </c>
     </row>
-    <row r="9" spans="1:75" ht="30" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:75" ht="15" x14ac:dyDescent="0.45">
       <c r="A9" s="16">
         <v>7</v>
       </c>
@@ -3651,7 +3685,7 @@
         <v>113</v>
       </c>
       <c r="H9" s="16" t="s">
-        <v>201</v>
+        <v>199</v>
       </c>
       <c r="I9" s="17">
         <v>80</v>
@@ -3897,10 +3931,10 @@
         <v>Excellent</v>
       </c>
       <c r="BW9" s="95" t="s">
-        <v>162</v>
+        <v>161</v>
       </c>
     </row>
-    <row r="10" spans="1:75" ht="30" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:75" ht="15" x14ac:dyDescent="0.45">
       <c r="A10" s="16">
         <v>8</v>
       </c>
@@ -3923,7 +3957,7 @@
         <v>113</v>
       </c>
       <c r="H10" s="16" t="s">
-        <v>202</v>
+        <v>200</v>
       </c>
       <c r="I10" s="17">
         <v>75</v>
@@ -4169,10 +4203,10 @@
         <v>Highly Satisfactory</v>
       </c>
       <c r="BW10" s="95" t="s">
-        <v>240</v>
+        <v>238</v>
       </c>
     </row>
-    <row r="11" spans="1:75" ht="30" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:75" ht="15" x14ac:dyDescent="0.45">
       <c r="A11" s="16">
         <v>9</v>
       </c>
@@ -4195,7 +4229,7 @@
         <v>112</v>
       </c>
       <c r="H11" s="16" t="s">
-        <v>203</v>
+        <v>201</v>
       </c>
       <c r="I11" s="17">
         <v>75</v>
@@ -4441,10 +4475,10 @@
         <v>Highly Satisfactory</v>
       </c>
       <c r="BW11" s="95" t="s">
-        <v>163</v>
+        <v>162</v>
       </c>
     </row>
-    <row r="12" spans="1:75" ht="30" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:75" ht="15" x14ac:dyDescent="0.45">
       <c r="A12" s="16">
         <v>10</v>
       </c>
@@ -4467,7 +4501,7 @@
         <v>112</v>
       </c>
       <c r="H12" s="16" t="s">
-        <v>204</v>
+        <v>202</v>
       </c>
       <c r="I12" s="17">
         <v>76</v>
@@ -4713,10 +4747,10 @@
         <v>Highly Satisfactory</v>
       </c>
       <c r="BW12" s="95" t="s">
-        <v>164</v>
+        <v>163</v>
       </c>
     </row>
-    <row r="13" spans="1:75" ht="30" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:75" ht="15" x14ac:dyDescent="0.45">
       <c r="A13" s="16">
         <v>11</v>
       </c>
@@ -4739,7 +4773,7 @@
         <v>113</v>
       </c>
       <c r="H13" s="16" t="s">
-        <v>205</v>
+        <v>203</v>
       </c>
       <c r="I13" s="17">
         <v>75</v>
@@ -4985,10 +5019,10 @@
         <v>Highly Satisfactory</v>
       </c>
       <c r="BW13" s="95" t="s">
-        <v>165</v>
+        <v>164</v>
       </c>
     </row>
-    <row r="14" spans="1:75" ht="30" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:75" ht="15" x14ac:dyDescent="0.45">
       <c r="A14" s="16">
         <v>12</v>
       </c>
@@ -5011,7 +5045,7 @@
         <v>113</v>
       </c>
       <c r="H14" s="16" t="s">
-        <v>206</v>
+        <v>204</v>
       </c>
       <c r="I14" s="17">
         <v>74</v>
@@ -5257,10 +5291,10 @@
         <v>Highly Satisfactory</v>
       </c>
       <c r="BW14" s="95" t="s">
-        <v>166</v>
+        <v>165</v>
       </c>
     </row>
-    <row r="15" spans="1:75" ht="30" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:75" ht="15" x14ac:dyDescent="0.45">
       <c r="A15" s="16">
         <v>13</v>
       </c>
@@ -5283,7 +5317,7 @@
         <v>113</v>
       </c>
       <c r="H15" s="16" t="s">
-        <v>207</v>
+        <v>205</v>
       </c>
       <c r="I15" s="17">
         <v>78</v>
@@ -5529,10 +5563,10 @@
         <v>Excellent</v>
       </c>
       <c r="BW15" s="95" t="s">
-        <v>167</v>
+        <v>166</v>
       </c>
     </row>
-    <row r="16" spans="1:75" ht="30" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:75" ht="15" x14ac:dyDescent="0.45">
       <c r="A16" s="16">
         <v>14</v>
       </c>
@@ -5555,7 +5589,7 @@
         <v>112</v>
       </c>
       <c r="H16" s="16" t="s">
-        <v>208</v>
+        <v>206</v>
       </c>
       <c r="I16" s="17">
         <v>75</v>
@@ -5800,11 +5834,11 @@
         <f t="shared" si="43"/>
         <v>Highly Satisfactory</v>
       </c>
-      <c r="BW16" s="113" t="s">
-        <v>168</v>
+      <c r="BW16" s="98" t="s">
+        <v>167</v>
       </c>
     </row>
-    <row r="17" spans="1:75" ht="30" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:75" ht="15" x14ac:dyDescent="0.45">
       <c r="A17" s="16">
         <v>15</v>
       </c>
@@ -5827,7 +5861,7 @@
         <v>112</v>
       </c>
       <c r="H17" s="16" t="s">
-        <v>209</v>
+        <v>207</v>
       </c>
       <c r="I17" s="17">
         <v>76</v>
@@ -6073,10 +6107,10 @@
         <v>Highly Satisfactory</v>
       </c>
       <c r="BW17" s="95" t="s">
-        <v>169</v>
+        <v>168</v>
       </c>
     </row>
-    <row r="18" spans="1:75" ht="30" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:75" ht="15" x14ac:dyDescent="0.45">
       <c r="A18" s="16">
         <v>16</v>
       </c>
@@ -6099,7 +6133,7 @@
         <v>112</v>
       </c>
       <c r="H18" s="16" t="s">
-        <v>210</v>
+        <v>208</v>
       </c>
       <c r="I18" s="17">
         <v>74</v>
@@ -6345,14 +6379,14 @@
         <v>Highly Satisfactory</v>
       </c>
       <c r="BW18" s="95" t="s">
-        <v>170</v>
+        <v>169</v>
       </c>
     </row>
-    <row r="19" spans="1:75" ht="30" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:75" ht="15" x14ac:dyDescent="0.45">
       <c r="A19" s="16">
         <v>17</v>
       </c>
-      <c r="B19" s="96" t="s">
+      <c r="B19" s="114" t="s">
         <v>43</v>
       </c>
       <c r="C19" s="16">
@@ -6371,7 +6405,7 @@
         <v>113</v>
       </c>
       <c r="H19" s="16" t="s">
-        <v>211</v>
+        <v>209</v>
       </c>
       <c r="I19" s="17">
         <v>80</v>
@@ -6616,9 +6650,11 @@
         <f t="shared" si="43"/>
         <v>Highly Satisfactory</v>
       </c>
-      <c r="BW19" s="95"/>
+      <c r="BW19" s="95" t="s">
+        <v>243</v>
+      </c>
     </row>
-    <row r="20" spans="1:75" ht="30" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:75" ht="15" x14ac:dyDescent="0.45">
       <c r="A20" s="16">
         <v>18</v>
       </c>
@@ -6641,7 +6677,7 @@
         <v>112</v>
       </c>
       <c r="H20" s="16" t="s">
-        <v>212</v>
+        <v>210</v>
       </c>
       <c r="I20" s="17">
         <v>76</v>
@@ -6887,10 +6923,10 @@
         <v>Highly Satisfactory</v>
       </c>
       <c r="BW20" s="95" t="s">
-        <v>171</v>
+        <v>170</v>
       </c>
     </row>
-    <row r="21" spans="1:75" ht="30" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:75" ht="15" x14ac:dyDescent="0.45">
       <c r="A21" s="16">
         <v>19</v>
       </c>
@@ -6913,7 +6949,7 @@
         <v>113</v>
       </c>
       <c r="H21" s="16" t="s">
-        <v>213</v>
+        <v>211</v>
       </c>
       <c r="I21" s="17">
         <v>74</v>
@@ -7158,11 +7194,11 @@
         <f t="shared" si="43"/>
         <v>Highly Satisfactory</v>
       </c>
-      <c r="BW21" s="113" t="s">
-        <v>172</v>
+      <c r="BW21" s="98" t="s">
+        <v>171</v>
       </c>
     </row>
-    <row r="22" spans="1:75" ht="21.95" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:75" ht="21.95" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A22" s="16">
         <v>34</v>
       </c>
@@ -7185,7 +7221,7 @@
         <v>112</v>
       </c>
       <c r="H22" s="16" t="s">
-        <v>214</v>
+        <v>212</v>
       </c>
       <c r="I22" s="17">
         <v>80</v>
@@ -7431,10 +7467,10 @@
         <v>Excellent</v>
       </c>
       <c r="BW22" s="95" t="s">
-        <v>173</v>
+        <v>172</v>
       </c>
     </row>
-    <row r="23" spans="1:75" ht="30" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:75" ht="15" x14ac:dyDescent="0.45">
       <c r="A23" s="16">
         <v>20</v>
       </c>
@@ -7457,7 +7493,7 @@
         <v>112</v>
       </c>
       <c r="H23" s="16" t="s">
-        <v>215</v>
+        <v>213</v>
       </c>
       <c r="I23" s="17">
         <v>74</v>
@@ -7703,10 +7739,10 @@
         <v>Highly Satisfactory</v>
       </c>
       <c r="BW23" s="95" t="s">
-        <v>174</v>
+        <v>173</v>
       </c>
     </row>
-    <row r="24" spans="1:75" ht="30" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:75" ht="15" x14ac:dyDescent="0.45">
       <c r="A24" s="16">
         <v>21</v>
       </c>
@@ -7729,7 +7765,7 @@
         <v>113</v>
       </c>
       <c r="H24" s="16" t="s">
-        <v>216</v>
+        <v>214</v>
       </c>
       <c r="I24" s="17">
         <v>74</v>
@@ -7975,10 +8011,10 @@
         <v>Highly Satisfactory</v>
       </c>
       <c r="BW24" s="95" t="s">
-        <v>175</v>
+        <v>174</v>
       </c>
     </row>
-    <row r="25" spans="1:75" ht="30" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:75" ht="15" x14ac:dyDescent="0.45">
       <c r="A25" s="16">
         <v>22</v>
       </c>
@@ -8001,7 +8037,7 @@
         <v>113</v>
       </c>
       <c r="H25" s="16" t="s">
-        <v>217</v>
+        <v>215</v>
       </c>
       <c r="I25" s="17">
         <v>78</v>
@@ -8247,10 +8283,10 @@
         <v>Excellent</v>
       </c>
       <c r="BW25" s="95" t="s">
-        <v>176</v>
+        <v>175</v>
       </c>
     </row>
-    <row r="26" spans="1:75" ht="30" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:75" ht="15" x14ac:dyDescent="0.45">
       <c r="A26" s="16">
         <v>23</v>
       </c>
@@ -8273,7 +8309,7 @@
         <v>113</v>
       </c>
       <c r="H26" s="16" t="s">
-        <v>218</v>
+        <v>216</v>
       </c>
       <c r="I26" s="17">
         <v>75</v>
@@ -8519,10 +8555,10 @@
         <v>Highly Satisfactory</v>
       </c>
       <c r="BW26" s="95" t="s">
-        <v>177</v>
+        <v>176</v>
       </c>
     </row>
-    <row r="27" spans="1:75" ht="30" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:75" ht="15" x14ac:dyDescent="0.45">
       <c r="A27" s="16">
         <v>24</v>
       </c>
@@ -8545,7 +8581,7 @@
         <v>112</v>
       </c>
       <c r="H27" s="16" t="s">
-        <v>219</v>
+        <v>217</v>
       </c>
       <c r="I27" s="17">
         <v>76</v>
@@ -8791,10 +8827,10 @@
         <v>Excellent</v>
       </c>
       <c r="BW27" s="95" t="s">
-        <v>178</v>
+        <v>177</v>
       </c>
     </row>
-    <row r="28" spans="1:75" ht="30" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:75" ht="15" x14ac:dyDescent="0.45">
       <c r="A28" s="16">
         <v>25</v>
       </c>
@@ -8817,7 +8853,7 @@
         <v>113</v>
       </c>
       <c r="H28" s="16" t="s">
-        <v>220</v>
+        <v>218</v>
       </c>
       <c r="I28" s="17">
         <v>74</v>
@@ -9063,10 +9099,10 @@
         <v>Highly Satisfactory</v>
       </c>
       <c r="BW28" s="95" t="s">
-        <v>179</v>
+        <v>178</v>
       </c>
     </row>
-    <row r="29" spans="1:75" ht="30" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:75" ht="15" x14ac:dyDescent="0.45">
       <c r="A29" s="16">
         <v>26</v>
       </c>
@@ -9083,13 +9119,13 @@
         <v>147</v>
       </c>
       <c r="F29" s="75" t="s">
-        <v>148</v>
+        <v>240</v>
       </c>
       <c r="G29" s="75" t="s">
         <v>112</v>
       </c>
       <c r="H29" s="16" t="s">
-        <v>221</v>
+        <v>219</v>
       </c>
       <c r="I29" s="17">
         <v>78</v>
@@ -9335,10 +9371,10 @@
         <v>Excellent</v>
       </c>
       <c r="BW29" s="95" t="s">
-        <v>180</v>
+        <v>179</v>
       </c>
     </row>
-    <row r="30" spans="1:75" ht="30" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:75" ht="15" x14ac:dyDescent="0.45">
       <c r="A30" s="16">
         <v>27</v>
       </c>
@@ -9361,7 +9397,7 @@
         <v>113</v>
       </c>
       <c r="H30" s="16" t="s">
-        <v>222</v>
+        <v>220</v>
       </c>
       <c r="I30" s="17">
         <v>74</v>
@@ -9608,7 +9644,7 @@
       </c>
       <c r="BW30" s="95"/>
     </row>
-    <row r="31" spans="1:75" ht="30" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:75" ht="15" x14ac:dyDescent="0.45">
       <c r="A31" s="16">
         <v>28</v>
       </c>
@@ -9631,7 +9667,7 @@
         <v>113</v>
       </c>
       <c r="H31" s="16" t="s">
-        <v>223</v>
+        <v>221</v>
       </c>
       <c r="I31" s="17">
         <v>78</v>
@@ -9877,10 +9913,10 @@
         <v>Highly Satisfactory</v>
       </c>
       <c r="BW31" s="95" t="s">
-        <v>181</v>
+        <v>180</v>
       </c>
     </row>
-    <row r="32" spans="1:75" ht="30" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:75" ht="15" x14ac:dyDescent="0.45">
       <c r="A32" s="16">
         <v>29</v>
       </c>
@@ -9897,13 +9933,13 @@
         <v>118</v>
       </c>
       <c r="F32" s="75" t="s">
-        <v>149</v>
+        <v>148</v>
       </c>
       <c r="G32" s="75" t="s">
         <v>112</v>
       </c>
       <c r="H32" s="16" t="s">
-        <v>224</v>
+        <v>222</v>
       </c>
       <c r="I32" s="17">
         <v>74</v>
@@ -10150,7 +10186,7 @@
       </c>
       <c r="BW32" s="95"/>
     </row>
-    <row r="33" spans="1:75" ht="30" x14ac:dyDescent="0.25">
+    <row r="33" spans="1:75" ht="15" x14ac:dyDescent="0.45">
       <c r="A33" s="16">
         <v>30</v>
       </c>
@@ -10164,16 +10200,16 @@
         <v>26</v>
       </c>
       <c r="E33" s="16" t="s">
+        <v>149</v>
+      </c>
+      <c r="F33" s="75" t="s">
         <v>150</v>
-      </c>
-      <c r="F33" s="75" t="s">
-        <v>151</v>
       </c>
       <c r="G33" s="75" t="s">
         <v>112</v>
       </c>
       <c r="H33" s="16" t="s">
-        <v>225</v>
+        <v>223</v>
       </c>
       <c r="I33" s="17">
         <v>80</v>
@@ -10419,10 +10455,10 @@
         <v>Excellent</v>
       </c>
       <c r="BW33" s="95" t="s">
-        <v>182</v>
+        <v>181</v>
       </c>
     </row>
-    <row r="34" spans="1:75" ht="30" x14ac:dyDescent="0.25">
+    <row r="34" spans="1:75" ht="15" x14ac:dyDescent="0.45">
       <c r="A34" s="16">
         <v>31</v>
       </c>
@@ -10436,16 +10472,16 @@
         <v>26</v>
       </c>
       <c r="E34" s="16" t="s">
+        <v>151</v>
+      </c>
+      <c r="F34" s="75" t="s">
         <v>152</v>
-      </c>
-      <c r="F34" s="75" t="s">
-        <v>153</v>
       </c>
       <c r="G34" s="75" t="s">
         <v>113</v>
       </c>
       <c r="H34" s="16" t="s">
-        <v>226</v>
+        <v>224</v>
       </c>
       <c r="I34" s="17">
         <v>75</v>
@@ -10691,10 +10727,10 @@
         <v>Highly Satisfactory</v>
       </c>
       <c r="BW34" s="95" t="s">
-        <v>183</v>
+        <v>182</v>
       </c>
     </row>
-    <row r="35" spans="1:75" ht="30" x14ac:dyDescent="0.25">
+    <row r="35" spans="1:75" ht="15" x14ac:dyDescent="0.45">
       <c r="A35" s="16">
         <v>32</v>
       </c>
@@ -10717,7 +10753,7 @@
         <v>112</v>
       </c>
       <c r="H35" s="16" t="s">
-        <v>227</v>
+        <v>225</v>
       </c>
       <c r="I35" s="17">
         <v>79</v>
@@ -10962,11 +10998,11 @@
         <f t="shared" si="43"/>
         <v>Excellent</v>
       </c>
-      <c r="BW35" s="113" t="s">
-        <v>184</v>
+      <c r="BW35" s="98" t="s">
+        <v>183</v>
       </c>
     </row>
-    <row r="36" spans="1:75" ht="30" x14ac:dyDescent="0.25">
+    <row r="36" spans="1:75" ht="15" x14ac:dyDescent="0.45">
       <c r="A36" s="16">
         <v>33</v>
       </c>
@@ -10989,7 +11025,7 @@
         <v>112</v>
       </c>
       <c r="H36" s="16" t="s">
-        <v>228</v>
+        <v>226</v>
       </c>
       <c r="I36" s="17">
         <v>76</v>
@@ -11235,10 +11271,10 @@
         <v>Excellent</v>
       </c>
       <c r="BW36" s="95" t="s">
-        <v>185</v>
+        <v>241</v>
       </c>
     </row>
-    <row r="37" spans="1:75" ht="30" x14ac:dyDescent="0.25">
+    <row r="37" spans="1:75" ht="15" x14ac:dyDescent="0.45">
       <c r="A37" s="16">
         <v>34</v>
       </c>
@@ -11261,7 +11297,7 @@
         <v>112</v>
       </c>
       <c r="H37" s="16" t="s">
-        <v>229</v>
+        <v>227</v>
       </c>
       <c r="I37" s="17">
         <v>80</v>
@@ -11506,11 +11542,11 @@
         <f t="shared" si="43"/>
         <v>Excellent</v>
       </c>
-      <c r="BW37" s="113" t="s">
-        <v>186</v>
+      <c r="BW37" s="98" t="s">
+        <v>184</v>
       </c>
     </row>
-    <row r="38" spans="1:75" ht="30" x14ac:dyDescent="0.25">
+    <row r="38" spans="1:75" ht="15" x14ac:dyDescent="0.45">
       <c r="A38" s="16">
         <v>35</v>
       </c>
@@ -11533,7 +11569,7 @@
         <v>112</v>
       </c>
       <c r="H38" s="16" t="s">
-        <v>230</v>
+        <v>228</v>
       </c>
       <c r="I38" s="17">
         <v>80</v>
@@ -11779,10 +11815,10 @@
         <v>Excellent</v>
       </c>
       <c r="BW38" s="95" t="s">
-        <v>187</v>
+        <v>185</v>
       </c>
     </row>
-    <row r="39" spans="1:75" ht="30" x14ac:dyDescent="0.25">
+    <row r="39" spans="1:75" ht="15" x14ac:dyDescent="0.45">
       <c r="A39" s="16">
         <v>36</v>
       </c>
@@ -11796,16 +11832,16 @@
         <v>26</v>
       </c>
       <c r="E39" s="16" t="s">
+        <v>153</v>
+      </c>
+      <c r="F39" s="75" t="s">
         <v>154</v>
-      </c>
-      <c r="F39" s="75" t="s">
-        <v>155</v>
       </c>
       <c r="G39" s="75" t="s">
         <v>112</v>
       </c>
       <c r="H39" s="16" t="s">
-        <v>231</v>
+        <v>229</v>
       </c>
       <c r="I39" s="17">
         <v>80</v>
@@ -12051,10 +12087,10 @@
         <v>Highly Satisfactory</v>
       </c>
       <c r="BW39" s="95" t="s">
-        <v>188</v>
+        <v>186</v>
       </c>
     </row>
-    <row r="40" spans="1:75" ht="30" x14ac:dyDescent="0.25">
+    <row r="40" spans="1:75" ht="15" x14ac:dyDescent="0.45">
       <c r="A40" s="16">
         <v>37</v>
       </c>
@@ -12077,7 +12113,7 @@
         <v>113</v>
       </c>
       <c r="H40" s="16" t="s">
-        <v>232</v>
+        <v>230</v>
       </c>
       <c r="I40" s="63">
         <v>75</v>
@@ -12325,7 +12361,7 @@
         <v>242</v>
       </c>
     </row>
-    <row r="41" spans="1:75" ht="30" x14ac:dyDescent="0.25">
+    <row r="41" spans="1:75" ht="15" x14ac:dyDescent="0.45">
       <c r="A41" s="16">
         <v>38</v>
       </c>
@@ -12342,13 +12378,13 @@
         <v>96</v>
       </c>
       <c r="F41" s="75" t="s">
-        <v>156</v>
+        <v>155</v>
       </c>
       <c r="G41" s="75" t="s">
         <v>112</v>
       </c>
       <c r="H41" s="16" t="s">
-        <v>233</v>
+        <v>231</v>
       </c>
       <c r="I41" s="17">
         <v>80</v>
@@ -12594,10 +12630,10 @@
         <v>Excellent</v>
       </c>
       <c r="BW41" s="95" t="s">
-        <v>189</v>
+        <v>187</v>
       </c>
     </row>
-    <row r="42" spans="1:75" ht="30" x14ac:dyDescent="0.25">
+    <row r="42" spans="1:75" ht="15" x14ac:dyDescent="0.45">
       <c r="A42" s="16">
         <v>39</v>
       </c>
@@ -12620,7 +12656,7 @@
         <v>112</v>
       </c>
       <c r="H42" s="16" t="s">
-        <v>234</v>
+        <v>232</v>
       </c>
       <c r="I42" s="17">
         <v>80</v>
@@ -12866,10 +12902,10 @@
         <v>Excellent</v>
       </c>
       <c r="BW42" s="95" t="s">
-        <v>190</v>
+        <v>188</v>
       </c>
     </row>
-    <row r="43" spans="1:75" ht="30" x14ac:dyDescent="0.25">
+    <row r="43" spans="1:75" ht="15" x14ac:dyDescent="0.45">
       <c r="A43" s="16">
         <v>40</v>
       </c>
@@ -12892,7 +12928,7 @@
         <v>112</v>
       </c>
       <c r="H43" s="16" t="s">
-        <v>235</v>
+        <v>233</v>
       </c>
       <c r="I43" s="17">
         <v>80</v>
@@ -13138,14 +13174,14 @@
         <v>Excellent</v>
       </c>
       <c r="BW43" s="95" t="s">
-        <v>191</v>
+        <v>189</v>
       </c>
     </row>
-    <row r="44" spans="1:75" ht="30" x14ac:dyDescent="0.25">
+    <row r="44" spans="1:75" ht="15" x14ac:dyDescent="0.45">
       <c r="A44" s="16">
         <v>41</v>
       </c>
-      <c r="B44" s="96" t="s">
+      <c r="B44" s="114" t="s">
         <v>69</v>
       </c>
       <c r="C44" s="16">
@@ -13164,7 +13200,7 @@
         <v>112</v>
       </c>
       <c r="H44" s="16" t="s">
-        <v>236</v>
+        <v>234</v>
       </c>
       <c r="I44" s="17">
         <v>74</v>
@@ -13410,10 +13446,10 @@
         <v>Highly Satisfactory</v>
       </c>
       <c r="BW44" s="95" t="s">
-        <v>241</v>
+        <v>239</v>
       </c>
     </row>
-    <row r="45" spans="1:75" ht="30" x14ac:dyDescent="0.25">
+    <row r="45" spans="1:75" ht="15" x14ac:dyDescent="0.45">
       <c r="A45" s="16">
         <v>42</v>
       </c>
@@ -13436,7 +13472,7 @@
         <v>112</v>
       </c>
       <c r="H45" s="16" t="s">
-        <v>237</v>
+        <v>235</v>
       </c>
       <c r="I45" s="17">
         <v>75</v>
@@ -13682,10 +13718,10 @@
         <v>Excellent</v>
       </c>
       <c r="BW45" s="95" t="s">
-        <v>192</v>
+        <v>190</v>
       </c>
     </row>
-    <row r="46" spans="1:75" ht="30" x14ac:dyDescent="0.25">
+    <row r="46" spans="1:75" ht="15" x14ac:dyDescent="0.45">
       <c r="A46" s="16">
         <v>43</v>
       </c>
@@ -13708,7 +13744,7 @@
         <v>112</v>
       </c>
       <c r="H46" s="16" t="s">
-        <v>238</v>
+        <v>236</v>
       </c>
       <c r="I46" s="17">
         <v>80</v>
@@ -13954,10 +13990,10 @@
         <v>Excellent</v>
       </c>
       <c r="BW46" s="95" t="s">
-        <v>193</v>
+        <v>191</v>
       </c>
     </row>
-    <row r="47" spans="1:75" ht="30" x14ac:dyDescent="0.25">
+    <row r="47" spans="1:75" ht="15" x14ac:dyDescent="0.45">
       <c r="A47" s="16">
         <v>44</v>
       </c>
@@ -13980,7 +14016,7 @@
         <v>112</v>
       </c>
       <c r="H47" s="16" t="s">
-        <v>239</v>
+        <v>237</v>
       </c>
       <c r="I47" s="17">
         <v>80</v>
@@ -14225,31 +14261,12 @@
         <f t="shared" si="43"/>
         <v>Highly Satisfactory</v>
       </c>
-      <c r="BW47" s="113" t="s">
-        <v>194</v>
+      <c r="BW47" s="98" t="s">
+        <v>192</v>
       </c>
     </row>
   </sheetData>
   <mergeCells count="29">
-    <mergeCell ref="BU1:BU2"/>
-    <mergeCell ref="BV1:BV2"/>
-    <mergeCell ref="BW1:BW2"/>
-    <mergeCell ref="BO1:BO2"/>
-    <mergeCell ref="BP1:BP2"/>
-    <mergeCell ref="BQ1:BQ2"/>
-    <mergeCell ref="BT1:BT2"/>
-    <mergeCell ref="S1:W1"/>
-    <mergeCell ref="X1:AB1"/>
-    <mergeCell ref="AC1:AG1"/>
-    <mergeCell ref="AH1:AL1"/>
-    <mergeCell ref="BL1:BL2"/>
-    <mergeCell ref="BN1:BN2"/>
-    <mergeCell ref="AM1:AQ1"/>
-    <mergeCell ref="AR1:AV1"/>
-    <mergeCell ref="AW1:BA1"/>
-    <mergeCell ref="BB1:BF1"/>
-    <mergeCell ref="BG1:BK1"/>
-    <mergeCell ref="BM1:BM2"/>
     <mergeCell ref="N1:R1"/>
     <mergeCell ref="A1:A2"/>
     <mergeCell ref="B1:B2"/>
@@ -14260,8 +14277,28 @@
     <mergeCell ref="F1:F2"/>
     <mergeCell ref="G1:G2"/>
     <mergeCell ref="H1:H2"/>
+    <mergeCell ref="BN1:BN2"/>
+    <mergeCell ref="AM1:AQ1"/>
+    <mergeCell ref="AR1:AV1"/>
+    <mergeCell ref="AW1:BA1"/>
+    <mergeCell ref="BB1:BF1"/>
+    <mergeCell ref="BG1:BK1"/>
+    <mergeCell ref="BM1:BM2"/>
+    <mergeCell ref="S1:W1"/>
+    <mergeCell ref="X1:AB1"/>
+    <mergeCell ref="AC1:AG1"/>
+    <mergeCell ref="AH1:AL1"/>
+    <mergeCell ref="BL1:BL2"/>
+    <mergeCell ref="BU1:BU2"/>
+    <mergeCell ref="BV1:BV2"/>
+    <mergeCell ref="BW1:BW2"/>
+    <mergeCell ref="BO1:BO2"/>
+    <mergeCell ref="BP1:BP2"/>
+    <mergeCell ref="BQ1:BQ2"/>
+    <mergeCell ref="BT1:BT2"/>
   </mergeCells>
   <phoneticPr fontId="13" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
perbaiki Data TTL & No Transkip Ners
</commit_message>
<xml_diff>
--- a/Ners/2023-2024/Transkip Nilai Ners 2023-2024.xlsx
+++ b/Ners/2023-2024/Transkip Nilai Ners 2023-2024.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Nando\Documents\Stikes\Transkip Nilai 2025\Ners\2023-2024\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1EEBA472-A362-4A85-A11C-A08D86520544}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9C9D296C-6E19-4F14-88EE-A08796E3D764}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-98" yWindow="-98" windowWidth="21795" windowHeight="12975" xr2:uid="{435B60B8-694F-4DDA-ADD2-15262503367A}"/>
   </bookViews>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="401" uniqueCount="244">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="403" uniqueCount="247">
   <si>
     <t>NO</t>
   </si>
@@ -300,9 +300,6 @@
     <t>20 Maret 1991</t>
   </si>
   <si>
-    <t>Kp. Juhar</t>
-  </si>
-  <si>
     <t>01 Agustus 1986</t>
   </si>
   <si>
@@ -613,141 +610,6 @@
   </si>
   <si>
     <t>Penerapan Prinsip Hand Hygiene Di Ruangan Bedah Rumah Sakit Umum Daerah Dabo Tahun 2024</t>
-  </si>
-  <si>
-    <t>641 / 14 / XII / 2025</t>
-  </si>
-  <si>
-    <t>642 / 14 / XII / 2025</t>
-  </si>
-  <si>
-    <t>643 / 14 / XII / 2025</t>
-  </si>
-  <si>
-    <t>644 / 14 / XII / 2025</t>
-  </si>
-  <si>
-    <t>645 / 14 / XII / 2025</t>
-  </si>
-  <si>
-    <t>646 / 14 / XII / 2025</t>
-  </si>
-  <si>
-    <t>647 / 14 / XII / 2025</t>
-  </si>
-  <si>
-    <t>648 / 14 / XII / 2025</t>
-  </si>
-  <si>
-    <t>649 / 14 / XII / 2025</t>
-  </si>
-  <si>
-    <t>650 / 14 / XII / 2025</t>
-  </si>
-  <si>
-    <t>651 / 14 / XII / 2025</t>
-  </si>
-  <si>
-    <t>652 / 14 / XII / 2025</t>
-  </si>
-  <si>
-    <t>653 / 14 / XII / 2025</t>
-  </si>
-  <si>
-    <t>654 / 14 / XII / 2025</t>
-  </si>
-  <si>
-    <t>655 / 14 / XII / 2025</t>
-  </si>
-  <si>
-    <t>656 / 14 / XII / 2025</t>
-  </si>
-  <si>
-    <t>657 / 14 / XII / 2025</t>
-  </si>
-  <si>
-    <t>658 / 14 / XII / 2025</t>
-  </si>
-  <si>
-    <t>659 / 14 / XII / 2025</t>
-  </si>
-  <si>
-    <t>660 / 14 / XII / 2025</t>
-  </si>
-  <si>
-    <t>661 / 14 / XII / 2025</t>
-  </si>
-  <si>
-    <t>662 / 14 / XII / 2025</t>
-  </si>
-  <si>
-    <t>663 / 14 / XII / 2025</t>
-  </si>
-  <si>
-    <t>664 / 14 / XII / 2025</t>
-  </si>
-  <si>
-    <t>665 / 14 / XII / 2025</t>
-  </si>
-  <si>
-    <t>666 / 14 / XII / 2025</t>
-  </si>
-  <si>
-    <t>667 / 14 / XII / 2025</t>
-  </si>
-  <si>
-    <t>668 / 14 / XII / 2025</t>
-  </si>
-  <si>
-    <t>669 / 14 / XII / 2025</t>
-  </si>
-  <si>
-    <t>670 / 14 / XII / 2025</t>
-  </si>
-  <si>
-    <t>671 / 14 / XII / 2025</t>
-  </si>
-  <si>
-    <t>672 / 14 / XII / 2025</t>
-  </si>
-  <si>
-    <t>673 / 14 / XII / 2025</t>
-  </si>
-  <si>
-    <t>674 / 14 / XII / 2025</t>
-  </si>
-  <si>
-    <t>675 / 14 / XII / 2025</t>
-  </si>
-  <si>
-    <t>676 / 14 / XII / 2025</t>
-  </si>
-  <si>
-    <t>677 / 14 / XII / 2025</t>
-  </si>
-  <si>
-    <t>678 / 14 / XII / 2025</t>
-  </si>
-  <si>
-    <t>679 / 14 / XII / 2025</t>
-  </si>
-  <si>
-    <t>680 / 14 / XII / 2025</t>
-  </si>
-  <si>
-    <t>681 / 14 / XII / 2025</t>
-  </si>
-  <si>
-    <t>682 / 14 / XII / 2025</t>
-  </si>
-  <si>
-    <t>683 / 14 / XII / 2025</t>
-  </si>
-  <si>
-    <t>684 / 14 / XII / 2025</t>
-  </si>
-  <si>
-    <t>685 / 14 / XII / 2025</t>
   </si>
   <si>
     <t>Penerapan Pre dan Post Conference Keperawatan untuk Meningkatkan Mutu Asuhan Keperawatan di Ruang Rawat Inap RSUD Tarempa.</t>
@@ -787,6 +649,153 @@
       </rPr>
       <t xml:space="preserve"> di Ruang Rawat Inap RSUD Palmatak</t>
     </r>
+  </si>
+  <si>
+    <t>Asuhan Keperawatan Hipertermia Pada An. A Dengan Kejang Demam Dan Penerapan Kompres Bawang Merah Di Ruang Rawat Inap Anak RSUD Tarempa</t>
+  </si>
+  <si>
+    <t>Kampung Juhar</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Terempa </t>
+  </si>
+  <si>
+    <t>Asuhan Keperawatan Nyeri Akut Pada Ny S Dengan Hipertensi Dan Penerapan Rendaman Kurma Di Desa Tarempa Timur Kecamatan Siantan</t>
+  </si>
+  <si>
+    <t>642 / 14 / XI / 2025</t>
+  </si>
+  <si>
+    <t>641 / 14 / V / 2025</t>
+  </si>
+  <si>
+    <t>643 / 14 / V / 2025</t>
+  </si>
+  <si>
+    <t>644 / 14 / V / 2025</t>
+  </si>
+  <si>
+    <t>645 / 14 / V / 2025</t>
+  </si>
+  <si>
+    <t>646 / 14 / XI / 2025</t>
+  </si>
+  <si>
+    <t>647 / 14 / XI / 2025</t>
+  </si>
+  <si>
+    <t>648 / 14 / XI / 2025</t>
+  </si>
+  <si>
+    <t>649 / 14 / V / 2025</t>
+  </si>
+  <si>
+    <t>650 / 14 / V / 2025</t>
+  </si>
+  <si>
+    <t>651 / 14 / XI / 2025</t>
+  </si>
+  <si>
+    <t>652 / 14 / XI / 2025</t>
+  </si>
+  <si>
+    <t>653 / 14 / XI / 2025</t>
+  </si>
+  <si>
+    <t>657 / 14 / XI / 2025</t>
+  </si>
+  <si>
+    <t>659 / 14 / XI / 2025</t>
+  </si>
+  <si>
+    <t>662 / 14 / XI / 2025</t>
+  </si>
+  <si>
+    <t>663 / 14 / XI / 2025</t>
+  </si>
+  <si>
+    <t>664 / 14 / XI / 2025</t>
+  </si>
+  <si>
+    <t>666 / 14 / XI / 2025</t>
+  </si>
+  <si>
+    <t>668 / 14 / XI / 2025</t>
+  </si>
+  <si>
+    <t>669 / 14 / XI / 2025</t>
+  </si>
+  <si>
+    <t>672 / 14 / XI / 2025</t>
+  </si>
+  <si>
+    <t>678 / 14 / XI / 2025</t>
+  </si>
+  <si>
+    <t>654 / 14 / V/ 2025</t>
+  </si>
+  <si>
+    <t>655 / 14 / V / 2025</t>
+  </si>
+  <si>
+    <t>656 / 14 / V / 2025</t>
+  </si>
+  <si>
+    <t>658 / 14 / V / 2025</t>
+  </si>
+  <si>
+    <t>660 / 14 / V / 2025</t>
+  </si>
+  <si>
+    <t>661 / 14 / V / 2025</t>
+  </si>
+  <si>
+    <t>665 / 14 / V / 2025</t>
+  </si>
+  <si>
+    <t>667 / 14 / V / 2025</t>
+  </si>
+  <si>
+    <t>670 / 14 / V / 2025</t>
+  </si>
+  <si>
+    <t>671 / 14 / V / 2025</t>
+  </si>
+  <si>
+    <t>673 / 14 / V / 2025</t>
+  </si>
+  <si>
+    <t>674 / 14 / V / 2025</t>
+  </si>
+  <si>
+    <t>675 / 14 / V / 2025</t>
+  </si>
+  <si>
+    <t>676 / 14 / V / 2025</t>
+  </si>
+  <si>
+    <t>677 / 14 / V / 2025</t>
+  </si>
+  <si>
+    <t>679 / 14 / V / 2025</t>
+  </si>
+  <si>
+    <t>680 / 14 / V / 2025</t>
+  </si>
+  <si>
+    <t>681 / 14 / V / 2025</t>
+  </si>
+  <si>
+    <t>682 / 14 / V / 2025</t>
+  </si>
+  <si>
+    <t>683 / 14 / V / 2025</t>
+  </si>
+  <si>
+    <t>684 / 14 / V / 2025</t>
+  </si>
+  <si>
+    <t>685 / 14 / V / 2025</t>
   </si>
 </sst>
 </file>
@@ -1299,13 +1308,34 @@
     <xf numFmtId="0" fontId="12" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="1" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="1" fillId="2" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="9" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="10" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="1" fillId="11" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="12" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="13" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="14" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="5" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -1320,28 +1350,7 @@
     <xf numFmtId="0" fontId="1" fillId="8" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="9" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="10" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="12" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="13" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="14" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="49" fontId="1" fillId="2" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="7" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -1666,10 +1675,10 @@
   <dimension ref="A1:BW47"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <pane xSplit="2" ySplit="2" topLeftCell="AN13" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="2" ySplit="2" topLeftCell="C23" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="C1" sqref="C1"/>
       <selection pane="bottomLeft" activeCell="A3" sqref="A3"/>
-      <selection pane="bottomRight" activeCell="BW20" sqref="BW20"/>
+      <selection pane="bottomRight" activeCell="H47" sqref="H47"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
@@ -1718,99 +1727,99 @@
       <c r="E1" s="100" t="s">
         <v>73</v>
       </c>
-      <c r="F1" s="113" t="s">
+      <c r="F1" s="102" t="s">
         <v>74</v>
       </c>
-      <c r="G1" s="113" t="s">
+      <c r="G1" s="102" t="s">
         <v>75</v>
       </c>
       <c r="H1" s="100" t="s">
         <v>76</v>
       </c>
-      <c r="I1" s="112" t="s">
-        <v>4</v>
-      </c>
-      <c r="J1" s="112"/>
-      <c r="K1" s="112"/>
-      <c r="L1" s="112"/>
-      <c r="M1" s="112"/>
-      <c r="N1" s="111" t="s">
+      <c r="I1" s="101" t="s">
+        <v>4</v>
+      </c>
+      <c r="J1" s="101"/>
+      <c r="K1" s="101"/>
+      <c r="L1" s="101"/>
+      <c r="M1" s="101"/>
+      <c r="N1" s="99" t="s">
         <v>5</v>
       </c>
-      <c r="O1" s="111"/>
-      <c r="P1" s="111"/>
-      <c r="Q1" s="111"/>
-      <c r="R1" s="111"/>
-      <c r="S1" s="102" t="s">
+      <c r="O1" s="99"/>
+      <c r="P1" s="99"/>
+      <c r="Q1" s="99"/>
+      <c r="R1" s="99"/>
+      <c r="S1" s="109" t="s">
         <v>6</v>
       </c>
-      <c r="T1" s="102"/>
-      <c r="U1" s="102"/>
-      <c r="V1" s="102"/>
-      <c r="W1" s="102"/>
-      <c r="X1" s="103" t="s">
+      <c r="T1" s="109"/>
+      <c r="U1" s="109"/>
+      <c r="V1" s="109"/>
+      <c r="W1" s="109"/>
+      <c r="X1" s="110" t="s">
         <v>7</v>
       </c>
-      <c r="Y1" s="103"/>
-      <c r="Z1" s="103"/>
-      <c r="AA1" s="103"/>
-      <c r="AB1" s="103"/>
-      <c r="AC1" s="104" t="s">
+      <c r="Y1" s="110"/>
+      <c r="Z1" s="110"/>
+      <c r="AA1" s="110"/>
+      <c r="AB1" s="110"/>
+      <c r="AC1" s="111" t="s">
         <v>8</v>
       </c>
-      <c r="AD1" s="104"/>
-      <c r="AE1" s="104"/>
-      <c r="AF1" s="104"/>
-      <c r="AG1" s="104"/>
-      <c r="AH1" s="105" t="s">
+      <c r="AD1" s="111"/>
+      <c r="AE1" s="111"/>
+      <c r="AF1" s="111"/>
+      <c r="AG1" s="111"/>
+      <c r="AH1" s="112" t="s">
         <v>9</v>
       </c>
-      <c r="AI1" s="105"/>
-      <c r="AJ1" s="105"/>
-      <c r="AK1" s="105"/>
-      <c r="AL1" s="105"/>
-      <c r="AM1" s="107" t="s">
+      <c r="AI1" s="112"/>
+      <c r="AJ1" s="112"/>
+      <c r="AK1" s="112"/>
+      <c r="AL1" s="112"/>
+      <c r="AM1" s="104" t="s">
         <v>13</v>
       </c>
-      <c r="AN1" s="107"/>
-      <c r="AO1" s="107"/>
-      <c r="AP1" s="107"/>
-      <c r="AQ1" s="107"/>
-      <c r="AR1" s="101" t="s">
+      <c r="AN1" s="104"/>
+      <c r="AO1" s="104"/>
+      <c r="AP1" s="104"/>
+      <c r="AQ1" s="104"/>
+      <c r="AR1" s="105" t="s">
         <v>14</v>
       </c>
-      <c r="AS1" s="101"/>
-      <c r="AT1" s="101"/>
-      <c r="AU1" s="101"/>
-      <c r="AV1" s="101"/>
-      <c r="AW1" s="108" t="s">
+      <c r="AS1" s="105"/>
+      <c r="AT1" s="105"/>
+      <c r="AU1" s="105"/>
+      <c r="AV1" s="105"/>
+      <c r="AW1" s="106" t="s">
         <v>15</v>
       </c>
-      <c r="AX1" s="108"/>
-      <c r="AY1" s="108"/>
-      <c r="AZ1" s="108"/>
-      <c r="BA1" s="108"/>
-      <c r="BB1" s="109" t="s">
+      <c r="AX1" s="106"/>
+      <c r="AY1" s="106"/>
+      <c r="AZ1" s="106"/>
+      <c r="BA1" s="106"/>
+      <c r="BB1" s="107" t="s">
         <v>16</v>
       </c>
-      <c r="BC1" s="109"/>
-      <c r="BD1" s="109"/>
-      <c r="BE1" s="109"/>
-      <c r="BF1" s="109"/>
-      <c r="BG1" s="110" t="s">
+      <c r="BC1" s="107"/>
+      <c r="BD1" s="107"/>
+      <c r="BE1" s="107"/>
+      <c r="BF1" s="107"/>
+      <c r="BG1" s="108" t="s">
         <v>17</v>
       </c>
-      <c r="BH1" s="110"/>
-      <c r="BI1" s="110"/>
-      <c r="BJ1" s="110"/>
-      <c r="BK1" s="110"/>
-      <c r="BL1" s="106" t="s">
+      <c r="BH1" s="108"/>
+      <c r="BI1" s="108"/>
+      <c r="BJ1" s="108"/>
+      <c r="BK1" s="108"/>
+      <c r="BL1" s="103" t="s">
         <v>10</v>
       </c>
-      <c r="BM1" s="106" t="s">
+      <c r="BM1" s="103" t="s">
         <v>11</v>
       </c>
-      <c r="BN1" s="106" t="s">
+      <c r="BN1" s="103" t="s">
         <v>12</v>
       </c>
       <c r="BO1" s="100" t="s">
@@ -1828,16 +1837,16 @@
       <c r="BS1" s="2" t="s">
         <v>18</v>
       </c>
-      <c r="BT1" s="101" t="s">
+      <c r="BT1" s="105" t="s">
         <v>19</v>
       </c>
-      <c r="BU1" s="99" t="s">
+      <c r="BU1" s="113" t="s">
         <v>77</v>
       </c>
-      <c r="BV1" s="99" t="s">
+      <c r="BV1" s="113" t="s">
         <v>78</v>
       </c>
-      <c r="BW1" s="99" t="s">
+      <c r="BW1" s="113" t="s">
         <v>79</v>
       </c>
     </row>
@@ -1847,8 +1856,8 @@
       <c r="C2" s="100"/>
       <c r="D2" s="100"/>
       <c r="E2" s="100"/>
-      <c r="F2" s="113"/>
-      <c r="G2" s="113"/>
+      <c r="F2" s="102"/>
+      <c r="G2" s="102"/>
       <c r="H2" s="100"/>
       <c r="I2" s="7" t="s">
         <v>20</v>
@@ -2015,9 +2024,9 @@
       <c r="BK2" s="5" t="s">
         <v>24</v>
       </c>
-      <c r="BL2" s="106"/>
-      <c r="BM2" s="106"/>
-      <c r="BN2" s="106"/>
+      <c r="BL2" s="103"/>
+      <c r="BM2" s="103"/>
+      <c r="BN2" s="103"/>
       <c r="BO2" s="100"/>
       <c r="BP2" s="100"/>
       <c r="BQ2" s="100"/>
@@ -2027,10 +2036,10 @@
       <c r="BS2" s="2" t="s">
         <v>25</v>
       </c>
-      <c r="BT2" s="101"/>
-      <c r="BU2" s="99"/>
-      <c r="BV2" s="99"/>
-      <c r="BW2" s="99"/>
+      <c r="BT2" s="105"/>
+      <c r="BU2" s="113"/>
+      <c r="BV2" s="113"/>
+      <c r="BW2" s="113"/>
     </row>
     <row r="3" spans="1:75" ht="15" x14ac:dyDescent="0.45">
       <c r="A3" s="16">
@@ -2052,10 +2061,10 @@
         <v>81</v>
       </c>
       <c r="G3" s="75" t="s">
-        <v>112</v>
+        <v>111</v>
       </c>
       <c r="H3" s="16" t="s">
-        <v>193</v>
+        <v>203</v>
       </c>
       <c r="I3" s="17">
         <v>76</v>
@@ -2301,7 +2310,7 @@
         <v>Highly Satisfactory</v>
       </c>
       <c r="BW3" s="97" t="s">
-        <v>156</v>
+        <v>155</v>
       </c>
     </row>
     <row r="4" spans="1:75" ht="15" x14ac:dyDescent="0.45">
@@ -2318,16 +2327,16 @@
         <v>26</v>
       </c>
       <c r="E4" s="16" t="s">
+        <v>113</v>
+      </c>
+      <c r="F4" s="75" t="s">
         <v>114</v>
       </c>
-      <c r="F4" s="75" t="s">
-        <v>115</v>
-      </c>
       <c r="G4" s="75" t="s">
-        <v>113</v>
+        <v>112</v>
       </c>
       <c r="H4" s="16" t="s">
-        <v>194</v>
+        <v>202</v>
       </c>
       <c r="I4" s="17">
         <v>76</v>
@@ -2573,14 +2582,14 @@
         <v>Highly Satisfactory</v>
       </c>
       <c r="BW4" s="95" t="s">
-        <v>157</v>
+        <v>156</v>
       </c>
     </row>
     <row r="5" spans="1:75" ht="15" x14ac:dyDescent="0.45">
       <c r="A5" s="16">
         <v>3</v>
       </c>
-      <c r="B5" s="96" t="s">
+      <c r="B5" s="114" t="s">
         <v>29</v>
       </c>
       <c r="C5" s="16">
@@ -2590,16 +2599,16 @@
         <v>26</v>
       </c>
       <c r="E5" s="16" t="s">
-        <v>118</v>
+        <v>200</v>
       </c>
       <c r="F5" s="75" t="s">
-        <v>137</v>
+        <v>136</v>
       </c>
       <c r="G5" s="75" t="s">
-        <v>112</v>
+        <v>111</v>
       </c>
       <c r="H5" s="16" t="s">
-        <v>195</v>
+        <v>204</v>
       </c>
       <c r="I5" s="17">
         <v>77</v>
@@ -2844,7 +2853,9 @@
         <f t="shared" si="43"/>
         <v>Excellent</v>
       </c>
-      <c r="BW5" s="95"/>
+      <c r="BW5" s="95" t="s">
+        <v>201</v>
+      </c>
     </row>
     <row r="6" spans="1:75" ht="15" x14ac:dyDescent="0.45">
       <c r="A6" s="16">
@@ -2866,10 +2877,10 @@
         <v>83</v>
       </c>
       <c r="G6" s="75" t="s">
-        <v>112</v>
+        <v>111</v>
       </c>
       <c r="H6" s="16" t="s">
-        <v>196</v>
+        <v>205</v>
       </c>
       <c r="I6" s="17">
         <v>76</v>
@@ -3115,7 +3126,7 @@
         <v>Excellent</v>
       </c>
       <c r="BW6" s="97" t="s">
-        <v>158</v>
+        <v>157</v>
       </c>
     </row>
     <row r="7" spans="1:75" ht="15" x14ac:dyDescent="0.45">
@@ -3132,16 +3143,16 @@
         <v>26</v>
       </c>
       <c r="E7" s="16" t="s">
-        <v>131</v>
+        <v>130</v>
       </c>
       <c r="F7" s="75" t="s">
-        <v>138</v>
+        <v>137</v>
       </c>
       <c r="G7" s="75" t="s">
-        <v>112</v>
+        <v>111</v>
       </c>
       <c r="H7" s="16" t="s">
-        <v>197</v>
+        <v>206</v>
       </c>
       <c r="I7" s="17">
         <v>77</v>
@@ -3387,7 +3398,7 @@
         <v>Excellent</v>
       </c>
       <c r="BW7" s="95" t="s">
-        <v>159</v>
+        <v>158</v>
       </c>
     </row>
     <row r="8" spans="1:75" ht="15" x14ac:dyDescent="0.45">
@@ -3404,16 +3415,16 @@
         <v>26</v>
       </c>
       <c r="E8" s="16" t="s">
+        <v>138</v>
+      </c>
+      <c r="F8" s="75" t="s">
         <v>139</v>
       </c>
-      <c r="F8" s="75" t="s">
-        <v>140</v>
-      </c>
       <c r="G8" s="75" t="s">
-        <v>113</v>
+        <v>112</v>
       </c>
       <c r="H8" s="16" t="s">
-        <v>198</v>
+        <v>207</v>
       </c>
       <c r="I8" s="17">
         <v>75</v>
@@ -3659,7 +3670,7 @@
         <v>Highly Satisfactory</v>
       </c>
       <c r="BW8" s="95" t="s">
-        <v>160</v>
+        <v>159</v>
       </c>
     </row>
     <row r="9" spans="1:75" ht="15" x14ac:dyDescent="0.45">
@@ -3676,16 +3687,16 @@
         <v>26</v>
       </c>
       <c r="E9" s="94" t="s">
+        <v>115</v>
+      </c>
+      <c r="F9" s="75" t="s">
         <v>116</v>
       </c>
-      <c r="F9" s="75" t="s">
-        <v>117</v>
-      </c>
       <c r="G9" s="75" t="s">
-        <v>113</v>
+        <v>112</v>
       </c>
       <c r="H9" s="16" t="s">
-        <v>199</v>
+        <v>208</v>
       </c>
       <c r="I9" s="17">
         <v>80</v>
@@ -3931,7 +3942,7 @@
         <v>Excellent</v>
       </c>
       <c r="BW9" s="95" t="s">
-        <v>161</v>
+        <v>160</v>
       </c>
     </row>
     <row r="10" spans="1:75" ht="15" x14ac:dyDescent="0.45">
@@ -3948,16 +3959,16 @@
         <v>26</v>
       </c>
       <c r="E10" s="94" t="s">
+        <v>117</v>
+      </c>
+      <c r="F10" s="75" t="s">
         <v>118</v>
       </c>
-      <c r="F10" s="75" t="s">
-        <v>119</v>
-      </c>
       <c r="G10" s="75" t="s">
-        <v>113</v>
+        <v>112</v>
       </c>
       <c r="H10" s="16" t="s">
-        <v>200</v>
+        <v>209</v>
       </c>
       <c r="I10" s="17">
         <v>75</v>
@@ -4203,7 +4214,7 @@
         <v>Highly Satisfactory</v>
       </c>
       <c r="BW10" s="95" t="s">
-        <v>238</v>
+        <v>192</v>
       </c>
     </row>
     <row r="11" spans="1:75" ht="15" x14ac:dyDescent="0.45">
@@ -4226,10 +4237,10 @@
         <v>85</v>
       </c>
       <c r="G11" s="75" t="s">
-        <v>112</v>
+        <v>111</v>
       </c>
       <c r="H11" s="16" t="s">
-        <v>201</v>
+        <v>210</v>
       </c>
       <c r="I11" s="17">
         <v>75</v>
@@ -4475,7 +4486,7 @@
         <v>Highly Satisfactory</v>
       </c>
       <c r="BW11" s="95" t="s">
-        <v>162</v>
+        <v>161</v>
       </c>
     </row>
     <row r="12" spans="1:75" ht="15" x14ac:dyDescent="0.45">
@@ -4498,10 +4509,10 @@
         <v>87</v>
       </c>
       <c r="G12" s="75" t="s">
-        <v>112</v>
+        <v>111</v>
       </c>
       <c r="H12" s="16" t="s">
-        <v>202</v>
+        <v>211</v>
       </c>
       <c r="I12" s="17">
         <v>76</v>
@@ -4747,7 +4758,7 @@
         <v>Highly Satisfactory</v>
       </c>
       <c r="BW12" s="95" t="s">
-        <v>163</v>
+        <v>162</v>
       </c>
     </row>
     <row r="13" spans="1:75" ht="15" x14ac:dyDescent="0.45">
@@ -4764,16 +4775,16 @@
         <v>26</v>
       </c>
       <c r="E13" s="94" t="s">
-        <v>114</v>
+        <v>113</v>
       </c>
       <c r="F13" s="75" t="s">
-        <v>120</v>
+        <v>119</v>
       </c>
       <c r="G13" s="75" t="s">
-        <v>113</v>
+        <v>112</v>
       </c>
       <c r="H13" s="16" t="s">
-        <v>203</v>
+        <v>212</v>
       </c>
       <c r="I13" s="17">
         <v>75</v>
@@ -5019,7 +5030,7 @@
         <v>Highly Satisfactory</v>
       </c>
       <c r="BW13" s="95" t="s">
-        <v>164</v>
+        <v>163</v>
       </c>
     </row>
     <row r="14" spans="1:75" ht="15" x14ac:dyDescent="0.45">
@@ -5036,16 +5047,16 @@
         <v>26</v>
       </c>
       <c r="E14" s="94" t="s">
+        <v>120</v>
+      </c>
+      <c r="F14" s="75" t="s">
         <v>121</v>
       </c>
-      <c r="F14" s="75" t="s">
-        <v>122</v>
-      </c>
       <c r="G14" s="75" t="s">
-        <v>113</v>
+        <v>112</v>
       </c>
       <c r="H14" s="16" t="s">
-        <v>204</v>
+        <v>213</v>
       </c>
       <c r="I14" s="17">
         <v>74</v>
@@ -5291,7 +5302,7 @@
         <v>Highly Satisfactory</v>
       </c>
       <c r="BW14" s="95" t="s">
-        <v>165</v>
+        <v>164</v>
       </c>
     </row>
     <row r="15" spans="1:75" ht="15" x14ac:dyDescent="0.45">
@@ -5308,16 +5319,16 @@
         <v>26</v>
       </c>
       <c r="E15" s="94" t="s">
+        <v>122</v>
+      </c>
+      <c r="F15" s="75" t="s">
         <v>123</v>
       </c>
-      <c r="F15" s="75" t="s">
-        <v>124</v>
-      </c>
       <c r="G15" s="75" t="s">
-        <v>113</v>
+        <v>112</v>
       </c>
       <c r="H15" s="16" t="s">
-        <v>205</v>
+        <v>214</v>
       </c>
       <c r="I15" s="17">
         <v>78</v>
@@ -5563,7 +5574,7 @@
         <v>Excellent</v>
       </c>
       <c r="BW15" s="95" t="s">
-        <v>166</v>
+        <v>165</v>
       </c>
     </row>
     <row r="16" spans="1:75" ht="15" x14ac:dyDescent="0.45">
@@ -5580,16 +5591,16 @@
         <v>26</v>
       </c>
       <c r="E16" s="16" t="s">
-        <v>118</v>
+        <v>117</v>
       </c>
       <c r="F16" s="75" t="s">
-        <v>125</v>
+        <v>124</v>
       </c>
       <c r="G16" s="75" t="s">
-        <v>112</v>
+        <v>111</v>
       </c>
       <c r="H16" s="16" t="s">
-        <v>206</v>
+        <v>225</v>
       </c>
       <c r="I16" s="17">
         <v>75</v>
@@ -5835,7 +5846,7 @@
         <v>Highly Satisfactory</v>
       </c>
       <c r="BW16" s="98" t="s">
-        <v>167</v>
+        <v>166</v>
       </c>
     </row>
     <row r="17" spans="1:75" ht="15" x14ac:dyDescent="0.45">
@@ -5852,16 +5863,16 @@
         <v>26</v>
       </c>
       <c r="E17" s="16" t="s">
+        <v>199</v>
+      </c>
+      <c r="F17" s="75" t="s">
         <v>88</v>
       </c>
-      <c r="F17" s="75" t="s">
-        <v>89</v>
-      </c>
       <c r="G17" s="75" t="s">
-        <v>112</v>
+        <v>111</v>
       </c>
       <c r="H17" s="16" t="s">
-        <v>207</v>
+        <v>226</v>
       </c>
       <c r="I17" s="17">
         <v>76</v>
@@ -6107,7 +6118,7 @@
         <v>Highly Satisfactory</v>
       </c>
       <c r="BW17" s="95" t="s">
-        <v>168</v>
+        <v>167</v>
       </c>
     </row>
     <row r="18" spans="1:75" ht="15" x14ac:dyDescent="0.45">
@@ -6124,16 +6135,16 @@
         <v>26</v>
       </c>
       <c r="E18" s="16" t="s">
-        <v>92</v>
+        <v>91</v>
       </c>
       <c r="F18" s="75" t="s">
-        <v>141</v>
+        <v>140</v>
       </c>
       <c r="G18" s="75" t="s">
-        <v>112</v>
+        <v>111</v>
       </c>
       <c r="H18" s="16" t="s">
-        <v>208</v>
+        <v>227</v>
       </c>
       <c r="I18" s="17">
         <v>74</v>
@@ -6379,14 +6390,14 @@
         <v>Highly Satisfactory</v>
       </c>
       <c r="BW18" s="95" t="s">
-        <v>169</v>
+        <v>168</v>
       </c>
     </row>
     <row r="19" spans="1:75" ht="15" x14ac:dyDescent="0.45">
       <c r="A19" s="16">
         <v>17</v>
       </c>
-      <c r="B19" s="114" t="s">
+      <c r="B19" s="16" t="s">
         <v>43</v>
       </c>
       <c r="C19" s="16">
@@ -6396,16 +6407,16 @@
         <v>26</v>
       </c>
       <c r="E19" s="16" t="s">
+        <v>141</v>
+      </c>
+      <c r="F19" s="75" t="s">
         <v>142</v>
       </c>
-      <c r="F19" s="75" t="s">
-        <v>143</v>
-      </c>
       <c r="G19" s="75" t="s">
-        <v>113</v>
+        <v>112</v>
       </c>
       <c r="H19" s="16" t="s">
-        <v>209</v>
+        <v>215</v>
       </c>
       <c r="I19" s="17">
         <v>80</v>
@@ -6651,7 +6662,7 @@
         <v>Highly Satisfactory</v>
       </c>
       <c r="BW19" s="95" t="s">
-        <v>243</v>
+        <v>197</v>
       </c>
     </row>
     <row r="20" spans="1:75" ht="15" x14ac:dyDescent="0.45">
@@ -6668,16 +6679,16 @@
         <v>26</v>
       </c>
       <c r="E20" s="95" t="s">
+        <v>89</v>
+      </c>
+      <c r="F20" s="75" t="s">
         <v>90</v>
       </c>
-      <c r="F20" s="75" t="s">
-        <v>91</v>
-      </c>
       <c r="G20" s="75" t="s">
-        <v>112</v>
+        <v>111</v>
       </c>
       <c r="H20" s="16" t="s">
-        <v>210</v>
+        <v>228</v>
       </c>
       <c r="I20" s="17">
         <v>76</v>
@@ -6923,7 +6934,7 @@
         <v>Highly Satisfactory</v>
       </c>
       <c r="BW20" s="95" t="s">
-        <v>170</v>
+        <v>169</v>
       </c>
     </row>
     <row r="21" spans="1:75" ht="15" x14ac:dyDescent="0.45">
@@ -6940,16 +6951,16 @@
         <v>26</v>
       </c>
       <c r="E21" s="94" t="s">
-        <v>118</v>
+        <v>117</v>
       </c>
       <c r="F21" s="75" t="s">
-        <v>125</v>
+        <v>124</v>
       </c>
       <c r="G21" s="75" t="s">
-        <v>113</v>
+        <v>112</v>
       </c>
       <c r="H21" s="16" t="s">
-        <v>211</v>
+        <v>216</v>
       </c>
       <c r="I21" s="17">
         <v>74</v>
@@ -7195,7 +7206,7 @@
         <v>Highly Satisfactory</v>
       </c>
       <c r="BW21" s="98" t="s">
-        <v>171</v>
+        <v>170</v>
       </c>
     </row>
     <row r="22" spans="1:75" ht="21.95" customHeight="1" x14ac:dyDescent="0.45">
@@ -7212,16 +7223,16 @@
         <v>26</v>
       </c>
       <c r="E22" s="16" t="s">
+        <v>143</v>
+      </c>
+      <c r="F22" s="75" t="s">
         <v>144</v>
       </c>
-      <c r="F22" s="75" t="s">
-        <v>145</v>
-      </c>
       <c r="G22" s="75" t="s">
-        <v>112</v>
+        <v>111</v>
       </c>
       <c r="H22" s="16" t="s">
-        <v>212</v>
+        <v>229</v>
       </c>
       <c r="I22" s="17">
         <v>80</v>
@@ -7467,7 +7478,7 @@
         <v>Excellent</v>
       </c>
       <c r="BW22" s="95" t="s">
-        <v>172</v>
+        <v>171</v>
       </c>
     </row>
     <row r="23" spans="1:75" ht="15" x14ac:dyDescent="0.45">
@@ -7484,16 +7495,16 @@
         <v>26</v>
       </c>
       <c r="E23" s="95" t="s">
+        <v>91</v>
+      </c>
+      <c r="F23" s="75" t="s">
         <v>92</v>
       </c>
-      <c r="F23" s="75" t="s">
-        <v>93</v>
-      </c>
       <c r="G23" s="75" t="s">
-        <v>112</v>
+        <v>111</v>
       </c>
       <c r="H23" s="16" t="s">
-        <v>213</v>
+        <v>230</v>
       </c>
       <c r="I23" s="17">
         <v>74</v>
@@ -7739,7 +7750,7 @@
         <v>Highly Satisfactory</v>
       </c>
       <c r="BW23" s="95" t="s">
-        <v>173</v>
+        <v>172</v>
       </c>
     </row>
     <row r="24" spans="1:75" ht="15" x14ac:dyDescent="0.45">
@@ -7756,16 +7767,16 @@
         <v>26</v>
       </c>
       <c r="E24" s="94" t="s">
-        <v>114</v>
+        <v>113</v>
       </c>
       <c r="F24" s="75" t="s">
-        <v>126</v>
+        <v>125</v>
       </c>
       <c r="G24" s="75" t="s">
-        <v>113</v>
+        <v>112</v>
       </c>
       <c r="H24" s="16" t="s">
-        <v>214</v>
+        <v>217</v>
       </c>
       <c r="I24" s="17">
         <v>74</v>
@@ -8011,7 +8022,7 @@
         <v>Highly Satisfactory</v>
       </c>
       <c r="BW24" s="95" t="s">
-        <v>174</v>
+        <v>173</v>
       </c>
     </row>
     <row r="25" spans="1:75" ht="15" x14ac:dyDescent="0.45">
@@ -8028,16 +8039,16 @@
         <v>26</v>
       </c>
       <c r="E25" s="94" t="s">
+        <v>126</v>
+      </c>
+      <c r="F25" s="75" t="s">
         <v>127</v>
       </c>
-      <c r="F25" s="75" t="s">
-        <v>128</v>
-      </c>
       <c r="G25" s="75" t="s">
-        <v>113</v>
+        <v>112</v>
       </c>
       <c r="H25" s="16" t="s">
-        <v>215</v>
+        <v>218</v>
       </c>
       <c r="I25" s="17">
         <v>78</v>
@@ -8283,7 +8294,7 @@
         <v>Excellent</v>
       </c>
       <c r="BW25" s="95" t="s">
-        <v>175</v>
+        <v>174</v>
       </c>
     </row>
     <row r="26" spans="1:75" ht="15" x14ac:dyDescent="0.45">
@@ -8300,16 +8311,16 @@
         <v>26</v>
       </c>
       <c r="E26" s="94" t="s">
+        <v>128</v>
+      </c>
+      <c r="F26" s="75" t="s">
         <v>129</v>
       </c>
-      <c r="F26" s="75" t="s">
-        <v>130</v>
-      </c>
       <c r="G26" s="75" t="s">
-        <v>113</v>
+        <v>112</v>
       </c>
       <c r="H26" s="16" t="s">
-        <v>216</v>
+        <v>219</v>
       </c>
       <c r="I26" s="17">
         <v>75</v>
@@ -8555,7 +8566,7 @@
         <v>Highly Satisfactory</v>
       </c>
       <c r="BW26" s="95" t="s">
-        <v>176</v>
+        <v>175</v>
       </c>
     </row>
     <row r="27" spans="1:75" ht="15" x14ac:dyDescent="0.45">
@@ -8572,16 +8583,16 @@
         <v>26</v>
       </c>
       <c r="E27" s="16" t="s">
+        <v>93</v>
+      </c>
+      <c r="F27" s="75" t="s">
         <v>94</v>
       </c>
-      <c r="F27" s="75" t="s">
-        <v>95</v>
-      </c>
       <c r="G27" s="75" t="s">
-        <v>112</v>
+        <v>111</v>
       </c>
       <c r="H27" s="16" t="s">
-        <v>217</v>
+        <v>231</v>
       </c>
       <c r="I27" s="17">
         <v>76</v>
@@ -8827,7 +8838,7 @@
         <v>Excellent</v>
       </c>
       <c r="BW27" s="95" t="s">
-        <v>177</v>
+        <v>176</v>
       </c>
     </row>
     <row r="28" spans="1:75" ht="15" x14ac:dyDescent="0.45">
@@ -8844,16 +8855,16 @@
         <v>26</v>
       </c>
       <c r="E28" s="16" t="s">
-        <v>118</v>
+        <v>117</v>
       </c>
       <c r="F28" s="75" t="s">
-        <v>146</v>
+        <v>145</v>
       </c>
       <c r="G28" s="75" t="s">
-        <v>113</v>
+        <v>112</v>
       </c>
       <c r="H28" s="16" t="s">
-        <v>218</v>
+        <v>220</v>
       </c>
       <c r="I28" s="17">
         <v>74</v>
@@ -9099,7 +9110,7 @@
         <v>Highly Satisfactory</v>
       </c>
       <c r="BW28" s="95" t="s">
-        <v>178</v>
+        <v>177</v>
       </c>
     </row>
     <row r="29" spans="1:75" ht="15" x14ac:dyDescent="0.45">
@@ -9116,16 +9127,16 @@
         <v>26</v>
       </c>
       <c r="E29" s="16" t="s">
-        <v>147</v>
+        <v>146</v>
       </c>
       <c r="F29" s="75" t="s">
-        <v>240</v>
+        <v>194</v>
       </c>
       <c r="G29" s="75" t="s">
-        <v>112</v>
+        <v>111</v>
       </c>
       <c r="H29" s="16" t="s">
-        <v>219</v>
+        <v>232</v>
       </c>
       <c r="I29" s="17">
         <v>78</v>
@@ -9371,7 +9382,7 @@
         <v>Excellent</v>
       </c>
       <c r="BW29" s="95" t="s">
-        <v>179</v>
+        <v>178</v>
       </c>
     </row>
     <row r="30" spans="1:75" ht="15" x14ac:dyDescent="0.45">
@@ -9388,16 +9399,16 @@
         <v>26</v>
       </c>
       <c r="E30" s="94" t="s">
+        <v>130</v>
+      </c>
+      <c r="F30" s="75" t="s">
         <v>131</v>
       </c>
-      <c r="F30" s="75" t="s">
-        <v>132</v>
-      </c>
       <c r="G30" s="75" t="s">
-        <v>113</v>
+        <v>112</v>
       </c>
       <c r="H30" s="16" t="s">
-        <v>220</v>
+        <v>221</v>
       </c>
       <c r="I30" s="17">
         <v>74</v>
@@ -9642,7 +9653,9 @@
         <f t="shared" si="43"/>
         <v>Highly Satisfactory</v>
       </c>
-      <c r="BW30" s="95"/>
+      <c r="BW30" s="95" t="s">
+        <v>198</v>
+      </c>
     </row>
     <row r="31" spans="1:75" ht="15" x14ac:dyDescent="0.45">
       <c r="A31" s="16">
@@ -9658,16 +9671,16 @@
         <v>26</v>
       </c>
       <c r="E31" s="94" t="s">
+        <v>132</v>
+      </c>
+      <c r="F31" s="75" t="s">
         <v>133</v>
       </c>
-      <c r="F31" s="75" t="s">
-        <v>134</v>
-      </c>
       <c r="G31" s="75" t="s">
-        <v>113</v>
+        <v>112</v>
       </c>
       <c r="H31" s="16" t="s">
-        <v>221</v>
+        <v>222</v>
       </c>
       <c r="I31" s="17">
         <v>78</v>
@@ -9913,7 +9926,7 @@
         <v>Highly Satisfactory</v>
       </c>
       <c r="BW31" s="95" t="s">
-        <v>180</v>
+        <v>179</v>
       </c>
     </row>
     <row r="32" spans="1:75" ht="15" x14ac:dyDescent="0.45">
@@ -9930,16 +9943,16 @@
         <v>26</v>
       </c>
       <c r="E32" s="16" t="s">
-        <v>118</v>
+        <v>117</v>
       </c>
       <c r="F32" s="75" t="s">
-        <v>148</v>
+        <v>147</v>
       </c>
       <c r="G32" s="75" t="s">
-        <v>112</v>
+        <v>111</v>
       </c>
       <c r="H32" s="16" t="s">
-        <v>222</v>
+        <v>233</v>
       </c>
       <c r="I32" s="17">
         <v>74</v>
@@ -10200,16 +10213,16 @@
         <v>26</v>
       </c>
       <c r="E33" s="16" t="s">
+        <v>148</v>
+      </c>
+      <c r="F33" s="75" t="s">
         <v>149</v>
       </c>
-      <c r="F33" s="75" t="s">
-        <v>150</v>
-      </c>
       <c r="G33" s="75" t="s">
-        <v>112</v>
+        <v>111</v>
       </c>
       <c r="H33" s="16" t="s">
-        <v>223</v>
+        <v>234</v>
       </c>
       <c r="I33" s="17">
         <v>80</v>
@@ -10455,7 +10468,7 @@
         <v>Excellent</v>
       </c>
       <c r="BW33" s="95" t="s">
-        <v>181</v>
+        <v>180</v>
       </c>
     </row>
     <row r="34" spans="1:75" ht="15" x14ac:dyDescent="0.45">
@@ -10472,16 +10485,16 @@
         <v>26</v>
       </c>
       <c r="E34" s="16" t="s">
+        <v>150</v>
+      </c>
+      <c r="F34" s="75" t="s">
         <v>151</v>
       </c>
-      <c r="F34" s="75" t="s">
-        <v>152</v>
-      </c>
       <c r="G34" s="75" t="s">
-        <v>113</v>
+        <v>112</v>
       </c>
       <c r="H34" s="16" t="s">
-        <v>224</v>
+        <v>223</v>
       </c>
       <c r="I34" s="17">
         <v>75</v>
@@ -10727,7 +10740,7 @@
         <v>Highly Satisfactory</v>
       </c>
       <c r="BW34" s="95" t="s">
-        <v>182</v>
+        <v>181</v>
       </c>
     </row>
     <row r="35" spans="1:75" ht="15" x14ac:dyDescent="0.45">
@@ -10744,16 +10757,16 @@
         <v>26</v>
       </c>
       <c r="E35" s="95" t="s">
+        <v>95</v>
+      </c>
+      <c r="F35" s="75" t="s">
         <v>96</v>
       </c>
-      <c r="F35" s="75" t="s">
-        <v>97</v>
-      </c>
       <c r="G35" s="75" t="s">
-        <v>112</v>
+        <v>111</v>
       </c>
       <c r="H35" s="16" t="s">
-        <v>225</v>
+        <v>235</v>
       </c>
       <c r="I35" s="17">
         <v>79</v>
@@ -10999,7 +11012,7 @@
         <v>Excellent</v>
       </c>
       <c r="BW35" s="98" t="s">
-        <v>183</v>
+        <v>182</v>
       </c>
     </row>
     <row r="36" spans="1:75" ht="15" x14ac:dyDescent="0.45">
@@ -11016,16 +11029,16 @@
         <v>26</v>
       </c>
       <c r="E36" s="95" t="s">
+        <v>97</v>
+      </c>
+      <c r="F36" s="75" t="s">
         <v>98</v>
       </c>
-      <c r="F36" s="75" t="s">
-        <v>99</v>
-      </c>
       <c r="G36" s="75" t="s">
-        <v>112</v>
+        <v>111</v>
       </c>
       <c r="H36" s="16" t="s">
-        <v>226</v>
+        <v>236</v>
       </c>
       <c r="I36" s="17">
         <v>76</v>
@@ -11271,7 +11284,7 @@
         <v>Excellent</v>
       </c>
       <c r="BW36" s="95" t="s">
-        <v>241</v>
+        <v>195</v>
       </c>
     </row>
     <row r="37" spans="1:75" ht="15" x14ac:dyDescent="0.45">
@@ -11288,16 +11301,16 @@
         <v>26</v>
       </c>
       <c r="E37" s="95" t="s">
+        <v>99</v>
+      </c>
+      <c r="F37" s="75" t="s">
         <v>100</v>
       </c>
-      <c r="F37" s="75" t="s">
-        <v>101</v>
-      </c>
       <c r="G37" s="75" t="s">
-        <v>112</v>
+        <v>111</v>
       </c>
       <c r="H37" s="16" t="s">
-        <v>227</v>
+        <v>237</v>
       </c>
       <c r="I37" s="17">
         <v>80</v>
@@ -11543,7 +11556,7 @@
         <v>Excellent</v>
       </c>
       <c r="BW37" s="98" t="s">
-        <v>184</v>
+        <v>183</v>
       </c>
     </row>
     <row r="38" spans="1:75" ht="15" x14ac:dyDescent="0.45">
@@ -11560,16 +11573,16 @@
         <v>26</v>
       </c>
       <c r="E38" s="95" t="s">
+        <v>101</v>
+      </c>
+      <c r="F38" s="75" t="s">
         <v>102</v>
       </c>
-      <c r="F38" s="75" t="s">
-        <v>103</v>
-      </c>
       <c r="G38" s="75" t="s">
-        <v>112</v>
+        <v>111</v>
       </c>
       <c r="H38" s="16" t="s">
-        <v>228</v>
+        <v>238</v>
       </c>
       <c r="I38" s="17">
         <v>80</v>
@@ -11815,7 +11828,7 @@
         <v>Excellent</v>
       </c>
       <c r="BW38" s="95" t="s">
-        <v>185</v>
+        <v>184</v>
       </c>
     </row>
     <row r="39" spans="1:75" ht="15" x14ac:dyDescent="0.45">
@@ -11832,16 +11845,16 @@
         <v>26</v>
       </c>
       <c r="E39" s="16" t="s">
+        <v>152</v>
+      </c>
+      <c r="F39" s="75" t="s">
         <v>153</v>
       </c>
-      <c r="F39" s="75" t="s">
-        <v>154</v>
-      </c>
       <c r="G39" s="75" t="s">
-        <v>112</v>
+        <v>111</v>
       </c>
       <c r="H39" s="16" t="s">
-        <v>229</v>
+        <v>239</v>
       </c>
       <c r="I39" s="17">
         <v>80</v>
@@ -12087,7 +12100,7 @@
         <v>Highly Satisfactory</v>
       </c>
       <c r="BW39" s="95" t="s">
-        <v>186</v>
+        <v>185</v>
       </c>
     </row>
     <row r="40" spans="1:75" ht="15" x14ac:dyDescent="0.45">
@@ -12104,16 +12117,16 @@
         <v>26</v>
       </c>
       <c r="E40" s="94" t="s">
+        <v>134</v>
+      </c>
+      <c r="F40" s="75" t="s">
         <v>135</v>
       </c>
-      <c r="F40" s="75" t="s">
-        <v>136</v>
-      </c>
       <c r="G40" s="75" t="s">
-        <v>113</v>
+        <v>112</v>
       </c>
       <c r="H40" s="16" t="s">
-        <v>230</v>
+        <v>224</v>
       </c>
       <c r="I40" s="63">
         <v>75</v>
@@ -12358,7 +12371,7 @@
         <v>Highly Satisfactory</v>
       </c>
       <c r="BW40" s="95" t="s">
-        <v>242</v>
+        <v>196</v>
       </c>
     </row>
     <row r="41" spans="1:75" ht="15" x14ac:dyDescent="0.45">
@@ -12375,16 +12388,16 @@
         <v>26</v>
       </c>
       <c r="E41" s="16" t="s">
-        <v>96</v>
+        <v>95</v>
       </c>
       <c r="F41" s="75" t="s">
-        <v>155</v>
+        <v>154</v>
       </c>
       <c r="G41" s="75" t="s">
-        <v>112</v>
+        <v>111</v>
       </c>
       <c r="H41" s="16" t="s">
-        <v>231</v>
+        <v>240</v>
       </c>
       <c r="I41" s="17">
         <v>80</v>
@@ -12630,7 +12643,7 @@
         <v>Excellent</v>
       </c>
       <c r="BW41" s="95" t="s">
-        <v>187</v>
+        <v>186</v>
       </c>
     </row>
     <row r="42" spans="1:75" ht="15" x14ac:dyDescent="0.45">
@@ -12647,16 +12660,16 @@
         <v>26</v>
       </c>
       <c r="E42" s="95" t="s">
-        <v>96</v>
+        <v>95</v>
       </c>
       <c r="F42" s="75" t="s">
-        <v>104</v>
+        <v>103</v>
       </c>
       <c r="G42" s="75" t="s">
-        <v>112</v>
+        <v>111</v>
       </c>
       <c r="H42" s="16" t="s">
-        <v>232</v>
+        <v>241</v>
       </c>
       <c r="I42" s="17">
         <v>80</v>
@@ -12902,7 +12915,7 @@
         <v>Excellent</v>
       </c>
       <c r="BW42" s="95" t="s">
-        <v>188</v>
+        <v>187</v>
       </c>
     </row>
     <row r="43" spans="1:75" ht="15" x14ac:dyDescent="0.45">
@@ -12919,16 +12932,16 @@
         <v>26</v>
       </c>
       <c r="E43" s="95" t="s">
-        <v>96</v>
+        <v>95</v>
       </c>
       <c r="F43" s="75" t="s">
-        <v>105</v>
+        <v>104</v>
       </c>
       <c r="G43" s="75" t="s">
-        <v>112</v>
+        <v>111</v>
       </c>
       <c r="H43" s="16" t="s">
-        <v>233</v>
+        <v>242</v>
       </c>
       <c r="I43" s="17">
         <v>80</v>
@@ -13174,14 +13187,14 @@
         <v>Excellent</v>
       </c>
       <c r="BW43" s="95" t="s">
-        <v>189</v>
+        <v>188</v>
       </c>
     </row>
     <row r="44" spans="1:75" ht="15" x14ac:dyDescent="0.45">
       <c r="A44" s="16">
         <v>41</v>
       </c>
-      <c r="B44" s="114" t="s">
+      <c r="B44" s="16" t="s">
         <v>69</v>
       </c>
       <c r="C44" s="16">
@@ -13191,16 +13204,16 @@
         <v>26</v>
       </c>
       <c r="E44" s="95" t="s">
+        <v>105</v>
+      </c>
+      <c r="F44" s="75" t="s">
         <v>106</v>
       </c>
-      <c r="F44" s="75" t="s">
-        <v>107</v>
-      </c>
       <c r="G44" s="75" t="s">
-        <v>112</v>
+        <v>111</v>
       </c>
       <c r="H44" s="16" t="s">
-        <v>234</v>
+        <v>243</v>
       </c>
       <c r="I44" s="17">
         <v>74</v>
@@ -13446,7 +13459,7 @@
         <v>Highly Satisfactory</v>
       </c>
       <c r="BW44" s="95" t="s">
-        <v>239</v>
+        <v>193</v>
       </c>
     </row>
     <row r="45" spans="1:75" ht="15" x14ac:dyDescent="0.45">
@@ -13463,16 +13476,16 @@
         <v>26</v>
       </c>
       <c r="E45" s="95" t="s">
+        <v>107</v>
+      </c>
+      <c r="F45" s="75" t="s">
         <v>108</v>
       </c>
-      <c r="F45" s="75" t="s">
-        <v>109</v>
-      </c>
       <c r="G45" s="75" t="s">
-        <v>112</v>
+        <v>111</v>
       </c>
       <c r="H45" s="16" t="s">
-        <v>235</v>
+        <v>244</v>
       </c>
       <c r="I45" s="17">
         <v>75</v>
@@ -13718,7 +13731,7 @@
         <v>Excellent</v>
       </c>
       <c r="BW45" s="95" t="s">
-        <v>190</v>
+        <v>189</v>
       </c>
     </row>
     <row r="46" spans="1:75" ht="15" x14ac:dyDescent="0.45">
@@ -13735,16 +13748,16 @@
         <v>26</v>
       </c>
       <c r="E46" s="95" t="s">
-        <v>96</v>
+        <v>95</v>
       </c>
       <c r="F46" s="75" t="s">
-        <v>110</v>
+        <v>109</v>
       </c>
       <c r="G46" s="75" t="s">
-        <v>112</v>
+        <v>111</v>
       </c>
       <c r="H46" s="16" t="s">
-        <v>236</v>
+        <v>245</v>
       </c>
       <c r="I46" s="17">
         <v>80</v>
@@ -13990,7 +14003,7 @@
         <v>Excellent</v>
       </c>
       <c r="BW46" s="95" t="s">
-        <v>191</v>
+        <v>190</v>
       </c>
     </row>
     <row r="47" spans="1:75" ht="15" x14ac:dyDescent="0.45">
@@ -14007,16 +14020,16 @@
         <v>26</v>
       </c>
       <c r="E47" s="95" t="s">
-        <v>96</v>
+        <v>95</v>
       </c>
       <c r="F47" s="75" t="s">
+        <v>110</v>
+      </c>
+      <c r="G47" s="75" t="s">
         <v>111</v>
       </c>
-      <c r="G47" s="75" t="s">
-        <v>112</v>
-      </c>
       <c r="H47" s="16" t="s">
-        <v>237</v>
+        <v>246</v>
       </c>
       <c r="I47" s="17">
         <v>80</v>
@@ -14262,11 +14275,30 @@
         <v>Highly Satisfactory</v>
       </c>
       <c r="BW47" s="98" t="s">
-        <v>192</v>
+        <v>191</v>
       </c>
     </row>
   </sheetData>
   <mergeCells count="29">
+    <mergeCell ref="BU1:BU2"/>
+    <mergeCell ref="BV1:BV2"/>
+    <mergeCell ref="BW1:BW2"/>
+    <mergeCell ref="BO1:BO2"/>
+    <mergeCell ref="BP1:BP2"/>
+    <mergeCell ref="BQ1:BQ2"/>
+    <mergeCell ref="BT1:BT2"/>
+    <mergeCell ref="S1:W1"/>
+    <mergeCell ref="X1:AB1"/>
+    <mergeCell ref="AC1:AG1"/>
+    <mergeCell ref="AH1:AL1"/>
+    <mergeCell ref="BL1:BL2"/>
+    <mergeCell ref="BN1:BN2"/>
+    <mergeCell ref="AM1:AQ1"/>
+    <mergeCell ref="AR1:AV1"/>
+    <mergeCell ref="AW1:BA1"/>
+    <mergeCell ref="BB1:BF1"/>
+    <mergeCell ref="BG1:BK1"/>
+    <mergeCell ref="BM1:BM2"/>
     <mergeCell ref="N1:R1"/>
     <mergeCell ref="A1:A2"/>
     <mergeCell ref="B1:B2"/>
@@ -14277,25 +14309,6 @@
     <mergeCell ref="F1:F2"/>
     <mergeCell ref="G1:G2"/>
     <mergeCell ref="H1:H2"/>
-    <mergeCell ref="BN1:BN2"/>
-    <mergeCell ref="AM1:AQ1"/>
-    <mergeCell ref="AR1:AV1"/>
-    <mergeCell ref="AW1:BA1"/>
-    <mergeCell ref="BB1:BF1"/>
-    <mergeCell ref="BG1:BK1"/>
-    <mergeCell ref="BM1:BM2"/>
-    <mergeCell ref="S1:W1"/>
-    <mergeCell ref="X1:AB1"/>
-    <mergeCell ref="AC1:AG1"/>
-    <mergeCell ref="AH1:AL1"/>
-    <mergeCell ref="BL1:BL2"/>
-    <mergeCell ref="BU1:BU2"/>
-    <mergeCell ref="BV1:BV2"/>
-    <mergeCell ref="BW1:BW2"/>
-    <mergeCell ref="BO1:BO2"/>
-    <mergeCell ref="BP1:BP2"/>
-    <mergeCell ref="BQ1:BQ2"/>
-    <mergeCell ref="BT1:BT2"/>
   </mergeCells>
   <phoneticPr fontId="13" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
penambahan judul bu yeni ekasari Ners 2023
</commit_message>
<xml_diff>
--- a/Ners/2023-2024/Transkip Nilai Ners 2023-2024.xlsx
+++ b/Ners/2023-2024/Transkip Nilai Ners 2023-2024.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Nando\Documents\Stikes\Transkip Nilai 2025\Ners\2023-2024\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9C9D296C-6E19-4F14-88EE-A08796E3D764}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4FFB8D91-3D7C-4A14-A9E9-B7AC2C838359}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-98" yWindow="-98" windowWidth="21795" windowHeight="12975" xr2:uid="{435B60B8-694F-4DDA-ADD2-15262503367A}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{435B60B8-694F-4DDA-ADD2-15262503367A}"/>
   </bookViews>
   <sheets>
     <sheet name="Transkip" sheetId="1" r:id="rId1"/>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="403" uniqueCount="247">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="404" uniqueCount="248">
   <si>
     <t>NO</t>
   </si>
@@ -615,13 +615,7 @@
     <t>Penerapan Pre dan Post Conference Keperawatan untuk Meningkatkan Mutu Asuhan Keperawatan di Ruang Rawat Inap RSUD Tarempa.</t>
   </si>
   <si>
-    <t>ASUHAN KEPERAWATAN HALUSINASI PADA NN.L DENGAN SKIZOFRENIA PARANOID DAN PENERAPAN STRATEGI PELAKSANAAN HALUSINASI DI WILAYAH DAIK LINGGA TAHUN 2024</t>
-  </si>
-  <si>
     <t>22 Februari 1985</t>
-  </si>
-  <si>
-    <t>ASUHAN KEPERAWATAN GANGGUAN TUMBUH KEMBANG AN.ER DENGAN STUNTING PADA KELUARGA TN.C DAN PENERAPAN PIJAT TUI NA DI RT 01 RW 02 KELURAHAN RAYA KECAMATAN SINGKEP BARAT TAHUN 2024</t>
   </si>
   <si>
     <t>Asuhan Keperawatan Gangguan Integeritas Kulit Pada An.A Dengan Luka Bakar Dan Penerapan Aloevera Di Paviliun Cindai Rsud Encik Maryam Kabupaten Lingga</t>
@@ -796,6 +790,15 @@
   </si>
   <si>
     <t>685 / 14 / V / 2025</t>
+  </si>
+  <si>
+    <t>Asuhan Keperawatan Nyeri Akut Pada  Tn. M Dengan Gout Arthritis Dan Penerapan Kompres Hangat Jahe Merah Di Desa Tarempa Timur</t>
+  </si>
+  <si>
+    <t>Asuhan Keperawatan Gangguan Tumbuh Kembang An.Er Dengan Stunting Pada Keluarga Tn.C Dan Penerapan Pijat Tui Na Di RT 01 RW 02 Kelurahan Raya Kecamatan Singkep Barat Tahun 2024</t>
+  </si>
+  <si>
+    <t>Asuhan Keperawatan Halusinasi Pada Nn.L Dengan Skizofrenia Paranoid Dan Penerapan Strategi Pelaksanaan Halusinasi Di Wilayah Daik Lingga Tahun 2024</t>
   </si>
 </sst>
 </file>
@@ -1014,7 +1017,7 @@
       <alignment vertical="center"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="115">
+  <cellXfs count="114">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="10" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -1299,43 +1302,19 @@
     <xf numFmtId="0" fontId="11" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="7" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="11" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="12" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="49" fontId="1" fillId="2" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="9" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="10" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="1" fillId="11" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="12" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="13" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="14" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="5" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -1350,7 +1329,28 @@
     <xf numFmtId="0" fontId="1" fillId="8" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="1" fillId="9" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="10" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="12" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="13" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="14" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="1" fillId="2" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="7" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -1675,160 +1675,160 @@
   <dimension ref="A1:BW47"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <pane xSplit="2" ySplit="2" topLeftCell="C23" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="2" ySplit="2" topLeftCell="BJ21" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="C1" sqref="C1"/>
       <selection pane="bottomLeft" activeCell="A3" sqref="A3"/>
-      <selection pane="bottomRight" activeCell="H47" sqref="H47"/>
+      <selection pane="bottomRight" activeCell="B32" sqref="B32"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="8" customWidth="1"/>
-    <col min="2" max="2" width="30.1328125" customWidth="1"/>
+    <col min="2" max="2" width="30.140625" customWidth="1"/>
     <col min="3" max="3" width="18" customWidth="1"/>
-    <col min="4" max="4" width="20.265625" customWidth="1"/>
-    <col min="5" max="5" width="20.265625" style="74" customWidth="1"/>
-    <col min="6" max="6" width="24.3984375" style="77" customWidth="1"/>
-    <col min="7" max="7" width="20.265625" style="76" customWidth="1"/>
-    <col min="8" max="8" width="20.265625" customWidth="1"/>
-    <col min="9" max="46" width="6.73046875" customWidth="1"/>
+    <col min="4" max="4" width="20.28515625" customWidth="1"/>
+    <col min="5" max="5" width="20.28515625" style="74" customWidth="1"/>
+    <col min="6" max="6" width="24.42578125" style="77" customWidth="1"/>
+    <col min="7" max="7" width="20.28515625" style="76" customWidth="1"/>
+    <col min="8" max="8" width="20.28515625" customWidth="1"/>
+    <col min="9" max="46" width="6.7109375" customWidth="1"/>
     <col min="47" max="47" width="8" customWidth="1"/>
-    <col min="48" max="48" width="6.73046875" customWidth="1"/>
-    <col min="49" max="49" width="8.1328125" customWidth="1"/>
-    <col min="50" max="53" width="6.73046875" customWidth="1"/>
-    <col min="54" max="54" width="8.265625" customWidth="1"/>
-    <col min="55" max="63" width="6.73046875" customWidth="1"/>
-    <col min="64" max="64" width="8.1328125" customWidth="1"/>
-    <col min="65" max="65" width="6.73046875" customWidth="1"/>
-    <col min="66" max="66" width="8.265625" customWidth="1"/>
-    <col min="68" max="68" width="6.73046875" customWidth="1"/>
-    <col min="69" max="69" width="8.86328125" customWidth="1"/>
-    <col min="70" max="70" width="11.1328125" customWidth="1"/>
+    <col min="48" max="48" width="6.7109375" customWidth="1"/>
+    <col min="49" max="49" width="8.140625" customWidth="1"/>
+    <col min="50" max="53" width="6.7109375" customWidth="1"/>
+    <col min="54" max="54" width="8.28515625" customWidth="1"/>
+    <col min="55" max="63" width="6.7109375" customWidth="1"/>
+    <col min="64" max="64" width="8.140625" customWidth="1"/>
+    <col min="65" max="65" width="6.7109375" customWidth="1"/>
+    <col min="66" max="66" width="8.28515625" customWidth="1"/>
+    <col min="68" max="68" width="6.7109375" customWidth="1"/>
+    <col min="69" max="69" width="8.85546875" customWidth="1"/>
+    <col min="70" max="70" width="11.140625" customWidth="1"/>
     <col min="71" max="71" width="10" customWidth="1"/>
-    <col min="72" max="72" width="13.3984375" customWidth="1"/>
-    <col min="73" max="73" width="18.1328125" customWidth="1"/>
-    <col min="74" max="74" width="17.86328125" customWidth="1"/>
-    <col min="75" max="75" width="27.265625" customWidth="1"/>
+    <col min="72" max="72" width="13.42578125" customWidth="1"/>
+    <col min="73" max="73" width="18.140625" customWidth="1"/>
+    <col min="74" max="74" width="17.85546875" customWidth="1"/>
+    <col min="75" max="75" width="27.28515625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:75" ht="15" x14ac:dyDescent="0.45">
-      <c r="A1" s="100" t="s">
+    <row r="1" spans="1:75" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A1" s="99" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="100" t="s">
+      <c r="B1" s="99" t="s">
         <v>1</v>
       </c>
-      <c r="C1" s="100" t="s">
+      <c r="C1" s="99" t="s">
         <v>2</v>
       </c>
-      <c r="D1" s="100" t="s">
-        <v>3</v>
-      </c>
-      <c r="E1" s="100" t="s">
+      <c r="D1" s="99" t="s">
+        <v>3</v>
+      </c>
+      <c r="E1" s="99" t="s">
         <v>73</v>
       </c>
-      <c r="F1" s="102" t="s">
+      <c r="F1" s="112" t="s">
         <v>74</v>
       </c>
-      <c r="G1" s="102" t="s">
+      <c r="G1" s="112" t="s">
         <v>75</v>
       </c>
-      <c r="H1" s="100" t="s">
+      <c r="H1" s="99" t="s">
         <v>76</v>
       </c>
-      <c r="I1" s="101" t="s">
-        <v>4</v>
-      </c>
-      <c r="J1" s="101"/>
-      <c r="K1" s="101"/>
-      <c r="L1" s="101"/>
-      <c r="M1" s="101"/>
-      <c r="N1" s="99" t="s">
+      <c r="I1" s="111" t="s">
+        <v>4</v>
+      </c>
+      <c r="J1" s="111"/>
+      <c r="K1" s="111"/>
+      <c r="L1" s="111"/>
+      <c r="M1" s="111"/>
+      <c r="N1" s="110" t="s">
         <v>5</v>
       </c>
-      <c r="O1" s="99"/>
-      <c r="P1" s="99"/>
-      <c r="Q1" s="99"/>
-      <c r="R1" s="99"/>
-      <c r="S1" s="109" t="s">
+      <c r="O1" s="110"/>
+      <c r="P1" s="110"/>
+      <c r="Q1" s="110"/>
+      <c r="R1" s="110"/>
+      <c r="S1" s="101" t="s">
         <v>6</v>
       </c>
-      <c r="T1" s="109"/>
-      <c r="U1" s="109"/>
-      <c r="V1" s="109"/>
-      <c r="W1" s="109"/>
-      <c r="X1" s="110" t="s">
+      <c r="T1" s="101"/>
+      <c r="U1" s="101"/>
+      <c r="V1" s="101"/>
+      <c r="W1" s="101"/>
+      <c r="X1" s="102" t="s">
         <v>7</v>
       </c>
-      <c r="Y1" s="110"/>
-      <c r="Z1" s="110"/>
-      <c r="AA1" s="110"/>
-      <c r="AB1" s="110"/>
-      <c r="AC1" s="111" t="s">
+      <c r="Y1" s="102"/>
+      <c r="Z1" s="102"/>
+      <c r="AA1" s="102"/>
+      <c r="AB1" s="102"/>
+      <c r="AC1" s="103" t="s">
         <v>8</v>
       </c>
-      <c r="AD1" s="111"/>
-      <c r="AE1" s="111"/>
-      <c r="AF1" s="111"/>
-      <c r="AG1" s="111"/>
-      <c r="AH1" s="112" t="s">
+      <c r="AD1" s="103"/>
+      <c r="AE1" s="103"/>
+      <c r="AF1" s="103"/>
+      <c r="AG1" s="103"/>
+      <c r="AH1" s="104" t="s">
         <v>9</v>
       </c>
-      <c r="AI1" s="112"/>
-      <c r="AJ1" s="112"/>
-      <c r="AK1" s="112"/>
-      <c r="AL1" s="112"/>
-      <c r="AM1" s="104" t="s">
+      <c r="AI1" s="104"/>
+      <c r="AJ1" s="104"/>
+      <c r="AK1" s="104"/>
+      <c r="AL1" s="104"/>
+      <c r="AM1" s="106" t="s">
         <v>13</v>
       </c>
-      <c r="AN1" s="104"/>
-      <c r="AO1" s="104"/>
-      <c r="AP1" s="104"/>
-      <c r="AQ1" s="104"/>
-      <c r="AR1" s="105" t="s">
+      <c r="AN1" s="106"/>
+      <c r="AO1" s="106"/>
+      <c r="AP1" s="106"/>
+      <c r="AQ1" s="106"/>
+      <c r="AR1" s="100" t="s">
         <v>14</v>
       </c>
-      <c r="AS1" s="105"/>
-      <c r="AT1" s="105"/>
-      <c r="AU1" s="105"/>
-      <c r="AV1" s="105"/>
-      <c r="AW1" s="106" t="s">
+      <c r="AS1" s="100"/>
+      <c r="AT1" s="100"/>
+      <c r="AU1" s="100"/>
+      <c r="AV1" s="100"/>
+      <c r="AW1" s="107" t="s">
         <v>15</v>
       </c>
-      <c r="AX1" s="106"/>
-      <c r="AY1" s="106"/>
-      <c r="AZ1" s="106"/>
-      <c r="BA1" s="106"/>
-      <c r="BB1" s="107" t="s">
+      <c r="AX1" s="107"/>
+      <c r="AY1" s="107"/>
+      <c r="AZ1" s="107"/>
+      <c r="BA1" s="107"/>
+      <c r="BB1" s="108" t="s">
         <v>16</v>
       </c>
-      <c r="BC1" s="107"/>
-      <c r="BD1" s="107"/>
-      <c r="BE1" s="107"/>
-      <c r="BF1" s="107"/>
-      <c r="BG1" s="108" t="s">
+      <c r="BC1" s="108"/>
+      <c r="BD1" s="108"/>
+      <c r="BE1" s="108"/>
+      <c r="BF1" s="108"/>
+      <c r="BG1" s="109" t="s">
         <v>17</v>
       </c>
-      <c r="BH1" s="108"/>
-      <c r="BI1" s="108"/>
-      <c r="BJ1" s="108"/>
-      <c r="BK1" s="108"/>
-      <c r="BL1" s="103" t="s">
+      <c r="BH1" s="109"/>
+      <c r="BI1" s="109"/>
+      <c r="BJ1" s="109"/>
+      <c r="BK1" s="109"/>
+      <c r="BL1" s="105" t="s">
         <v>10</v>
       </c>
-      <c r="BM1" s="103" t="s">
+      <c r="BM1" s="105" t="s">
         <v>11</v>
       </c>
-      <c r="BN1" s="103" t="s">
+      <c r="BN1" s="105" t="s">
         <v>12</v>
       </c>
-      <c r="BO1" s="100" t="s">
+      <c r="BO1" s="99" t="s">
         <v>10</v>
       </c>
-      <c r="BP1" s="100" t="s">
+      <c r="BP1" s="99" t="s">
         <v>11</v>
       </c>
-      <c r="BQ1" s="100" t="s">
+      <c r="BQ1" s="99" t="s">
         <v>12</v>
       </c>
       <c r="BR1" s="2" t="s">
@@ -1837,28 +1837,28 @@
       <c r="BS1" s="2" t="s">
         <v>18</v>
       </c>
-      <c r="BT1" s="105" t="s">
+      <c r="BT1" s="100" t="s">
         <v>19</v>
       </c>
-      <c r="BU1" s="113" t="s">
+      <c r="BU1" s="98" t="s">
         <v>77</v>
       </c>
-      <c r="BV1" s="113" t="s">
+      <c r="BV1" s="98" t="s">
         <v>78</v>
       </c>
-      <c r="BW1" s="113" t="s">
+      <c r="BW1" s="98" t="s">
         <v>79</v>
       </c>
     </row>
-    <row r="2" spans="1:75" ht="15" x14ac:dyDescent="0.45">
-      <c r="A2" s="100"/>
-      <c r="B2" s="100"/>
-      <c r="C2" s="100"/>
-      <c r="D2" s="100"/>
-      <c r="E2" s="100"/>
-      <c r="F2" s="102"/>
-      <c r="G2" s="102"/>
-      <c r="H2" s="100"/>
+    <row r="2" spans="1:75" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A2" s="99"/>
+      <c r="B2" s="99"/>
+      <c r="C2" s="99"/>
+      <c r="D2" s="99"/>
+      <c r="E2" s="99"/>
+      <c r="F2" s="112"/>
+      <c r="G2" s="112"/>
+      <c r="H2" s="99"/>
       <c r="I2" s="7" t="s">
         <v>20</v>
       </c>
@@ -2024,24 +2024,24 @@
       <c r="BK2" s="5" t="s">
         <v>24</v>
       </c>
-      <c r="BL2" s="103"/>
-      <c r="BM2" s="103"/>
-      <c r="BN2" s="103"/>
-      <c r="BO2" s="100"/>
-      <c r="BP2" s="100"/>
-      <c r="BQ2" s="100"/>
+      <c r="BL2" s="105"/>
+      <c r="BM2" s="105"/>
+      <c r="BN2" s="105"/>
+      <c r="BO2" s="99"/>
+      <c r="BP2" s="99"/>
+      <c r="BQ2" s="99"/>
       <c r="BR2" s="2" t="s">
         <v>20</v>
       </c>
       <c r="BS2" s="2" t="s">
         <v>25</v>
       </c>
-      <c r="BT2" s="105"/>
-      <c r="BU2" s="113"/>
-      <c r="BV2" s="113"/>
-      <c r="BW2" s="113"/>
+      <c r="BT2" s="100"/>
+      <c r="BU2" s="98"/>
+      <c r="BV2" s="98"/>
+      <c r="BW2" s="98"/>
     </row>
-    <row r="3" spans="1:75" ht="15" x14ac:dyDescent="0.45">
+    <row r="3" spans="1:75" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A3" s="16">
         <v>1</v>
       </c>
@@ -2064,7 +2064,7 @@
         <v>111</v>
       </c>
       <c r="H3" s="16" t="s">
-        <v>203</v>
+        <v>201</v>
       </c>
       <c r="I3" s="17">
         <v>76</v>
@@ -2309,11 +2309,11 @@
         <f>IF(BT3&gt;=3.51,"Excellent",(IF(BT3&gt;=2.75,"Highly Satisfactory",(IF(BT3&gt;=2,"Satisfactory","FAILED")))))</f>
         <v>Highly Satisfactory</v>
       </c>
-      <c r="BW3" s="97" t="s">
+      <c r="BW3" s="96" t="s">
         <v>155</v>
       </c>
     </row>
-    <row r="4" spans="1:75" ht="15" x14ac:dyDescent="0.45">
+    <row r="4" spans="1:75" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A4" s="16">
         <v>2</v>
       </c>
@@ -2336,7 +2336,7 @@
         <v>112</v>
       </c>
       <c r="H4" s="16" t="s">
-        <v>202</v>
+        <v>200</v>
       </c>
       <c r="I4" s="17">
         <v>76</v>
@@ -2585,11 +2585,11 @@
         <v>156</v>
       </c>
     </row>
-    <row r="5" spans="1:75" ht="15" x14ac:dyDescent="0.45">
+    <row r="5" spans="1:75" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A5" s="16">
         <v>3</v>
       </c>
-      <c r="B5" s="114" t="s">
+      <c r="B5" s="16" t="s">
         <v>29</v>
       </c>
       <c r="C5" s="16">
@@ -2599,7 +2599,7 @@
         <v>26</v>
       </c>
       <c r="E5" s="16" t="s">
-        <v>200</v>
+        <v>198</v>
       </c>
       <c r="F5" s="75" t="s">
         <v>136</v>
@@ -2608,7 +2608,7 @@
         <v>111</v>
       </c>
       <c r="H5" s="16" t="s">
-        <v>204</v>
+        <v>202</v>
       </c>
       <c r="I5" s="17">
         <v>77</v>
@@ -2854,10 +2854,10 @@
         <v>Excellent</v>
       </c>
       <c r="BW5" s="95" t="s">
-        <v>201</v>
+        <v>199</v>
       </c>
     </row>
-    <row r="6" spans="1:75" ht="15" x14ac:dyDescent="0.45">
+    <row r="6" spans="1:75" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A6" s="16">
         <v>4</v>
       </c>
@@ -2880,7 +2880,7 @@
         <v>111</v>
       </c>
       <c r="H6" s="16" t="s">
-        <v>205</v>
+        <v>203</v>
       </c>
       <c r="I6" s="17">
         <v>76</v>
@@ -3125,11 +3125,11 @@
         <f t="shared" si="43"/>
         <v>Excellent</v>
       </c>
-      <c r="BW6" s="97" t="s">
+      <c r="BW6" s="96" t="s">
         <v>157</v>
       </c>
     </row>
-    <row r="7" spans="1:75" ht="15" x14ac:dyDescent="0.45">
+    <row r="7" spans="1:75" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A7" s="16">
         <v>5</v>
       </c>
@@ -3152,7 +3152,7 @@
         <v>111</v>
       </c>
       <c r="H7" s="16" t="s">
-        <v>206</v>
+        <v>204</v>
       </c>
       <c r="I7" s="17">
         <v>77</v>
@@ -3401,7 +3401,7 @@
         <v>158</v>
       </c>
     </row>
-    <row r="8" spans="1:75" ht="15" x14ac:dyDescent="0.45">
+    <row r="8" spans="1:75" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A8" s="16">
         <v>6</v>
       </c>
@@ -3424,7 +3424,7 @@
         <v>112</v>
       </c>
       <c r="H8" s="16" t="s">
-        <v>207</v>
+        <v>205</v>
       </c>
       <c r="I8" s="17">
         <v>75</v>
@@ -3673,7 +3673,7 @@
         <v>159</v>
       </c>
     </row>
-    <row r="9" spans="1:75" ht="15" x14ac:dyDescent="0.45">
+    <row r="9" spans="1:75" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A9" s="16">
         <v>7</v>
       </c>
@@ -3696,7 +3696,7 @@
         <v>112</v>
       </c>
       <c r="H9" s="16" t="s">
-        <v>208</v>
+        <v>206</v>
       </c>
       <c r="I9" s="17">
         <v>80</v>
@@ -3945,7 +3945,7 @@
         <v>160</v>
       </c>
     </row>
-    <row r="10" spans="1:75" ht="15" x14ac:dyDescent="0.45">
+    <row r="10" spans="1:75" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A10" s="16">
         <v>8</v>
       </c>
@@ -3968,7 +3968,7 @@
         <v>112</v>
       </c>
       <c r="H10" s="16" t="s">
-        <v>209</v>
+        <v>207</v>
       </c>
       <c r="I10" s="17">
         <v>75</v>
@@ -4217,7 +4217,7 @@
         <v>192</v>
       </c>
     </row>
-    <row r="11" spans="1:75" ht="15" x14ac:dyDescent="0.45">
+    <row r="11" spans="1:75" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A11" s="16">
         <v>9</v>
       </c>
@@ -4240,7 +4240,7 @@
         <v>111</v>
       </c>
       <c r="H11" s="16" t="s">
-        <v>210</v>
+        <v>208</v>
       </c>
       <c r="I11" s="17">
         <v>75</v>
@@ -4489,7 +4489,7 @@
         <v>161</v>
       </c>
     </row>
-    <row r="12" spans="1:75" ht="15" x14ac:dyDescent="0.45">
+    <row r="12" spans="1:75" x14ac:dyDescent="0.25">
       <c r="A12" s="16">
         <v>10</v>
       </c>
@@ -4512,7 +4512,7 @@
         <v>111</v>
       </c>
       <c r="H12" s="16" t="s">
-        <v>211</v>
+        <v>209</v>
       </c>
       <c r="I12" s="17">
         <v>76</v>
@@ -4761,7 +4761,7 @@
         <v>162</v>
       </c>
     </row>
-    <row r="13" spans="1:75" ht="15" x14ac:dyDescent="0.45">
+    <row r="13" spans="1:75" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A13" s="16">
         <v>11</v>
       </c>
@@ -4784,7 +4784,7 @@
         <v>112</v>
       </c>
       <c r="H13" s="16" t="s">
-        <v>212</v>
+        <v>210</v>
       </c>
       <c r="I13" s="17">
         <v>75</v>
@@ -5033,7 +5033,7 @@
         <v>163</v>
       </c>
     </row>
-    <row r="14" spans="1:75" ht="15" x14ac:dyDescent="0.45">
+    <row r="14" spans="1:75" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A14" s="16">
         <v>12</v>
       </c>
@@ -5056,7 +5056,7 @@
         <v>112</v>
       </c>
       <c r="H14" s="16" t="s">
-        <v>213</v>
+        <v>211</v>
       </c>
       <c r="I14" s="17">
         <v>74</v>
@@ -5305,7 +5305,7 @@
         <v>164</v>
       </c>
     </row>
-    <row r="15" spans="1:75" ht="15" x14ac:dyDescent="0.45">
+    <row r="15" spans="1:75" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A15" s="16">
         <v>13</v>
       </c>
@@ -5328,7 +5328,7 @@
         <v>112</v>
       </c>
       <c r="H15" s="16" t="s">
-        <v>214</v>
+        <v>212</v>
       </c>
       <c r="I15" s="17">
         <v>78</v>
@@ -5577,7 +5577,7 @@
         <v>165</v>
       </c>
     </row>
-    <row r="16" spans="1:75" ht="15" x14ac:dyDescent="0.45">
+    <row r="16" spans="1:75" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A16" s="16">
         <v>14</v>
       </c>
@@ -5600,7 +5600,7 @@
         <v>111</v>
       </c>
       <c r="H16" s="16" t="s">
-        <v>225</v>
+        <v>223</v>
       </c>
       <c r="I16" s="17">
         <v>75</v>
@@ -5845,11 +5845,11 @@
         <f t="shared" si="43"/>
         <v>Highly Satisfactory</v>
       </c>
-      <c r="BW16" s="98" t="s">
+      <c r="BW16" s="97" t="s">
         <v>166</v>
       </c>
     </row>
-    <row r="17" spans="1:75" ht="15" x14ac:dyDescent="0.45">
+    <row r="17" spans="1:75" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A17" s="16">
         <v>15</v>
       </c>
@@ -5863,7 +5863,7 @@
         <v>26</v>
       </c>
       <c r="E17" s="16" t="s">
-        <v>199</v>
+        <v>197</v>
       </c>
       <c r="F17" s="75" t="s">
         <v>88</v>
@@ -5872,7 +5872,7 @@
         <v>111</v>
       </c>
       <c r="H17" s="16" t="s">
-        <v>226</v>
+        <v>224</v>
       </c>
       <c r="I17" s="17">
         <v>76</v>
@@ -6121,7 +6121,7 @@
         <v>167</v>
       </c>
     </row>
-    <row r="18" spans="1:75" ht="15" x14ac:dyDescent="0.45">
+    <row r="18" spans="1:75" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A18" s="16">
         <v>16</v>
       </c>
@@ -6144,7 +6144,7 @@
         <v>111</v>
       </c>
       <c r="H18" s="16" t="s">
-        <v>227</v>
+        <v>225</v>
       </c>
       <c r="I18" s="17">
         <v>74</v>
@@ -6393,7 +6393,7 @@
         <v>168</v>
       </c>
     </row>
-    <row r="19" spans="1:75" ht="15" x14ac:dyDescent="0.45">
+    <row r="19" spans="1:75" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A19" s="16">
         <v>17</v>
       </c>
@@ -6416,7 +6416,7 @@
         <v>112</v>
       </c>
       <c r="H19" s="16" t="s">
-        <v>215</v>
+        <v>213</v>
       </c>
       <c r="I19" s="17">
         <v>80</v>
@@ -6662,10 +6662,10 @@
         <v>Highly Satisfactory</v>
       </c>
       <c r="BW19" s="95" t="s">
-        <v>197</v>
+        <v>195</v>
       </c>
     </row>
-    <row r="20" spans="1:75" ht="15" x14ac:dyDescent="0.45">
+    <row r="20" spans="1:75" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A20" s="16">
         <v>18</v>
       </c>
@@ -6688,7 +6688,7 @@
         <v>111</v>
       </c>
       <c r="H20" s="16" t="s">
-        <v>228</v>
+        <v>226</v>
       </c>
       <c r="I20" s="17">
         <v>76</v>
@@ -6937,7 +6937,7 @@
         <v>169</v>
       </c>
     </row>
-    <row r="21" spans="1:75" ht="15" x14ac:dyDescent="0.45">
+    <row r="21" spans="1:75" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A21" s="16">
         <v>19</v>
       </c>
@@ -6960,7 +6960,7 @@
         <v>112</v>
       </c>
       <c r="H21" s="16" t="s">
-        <v>216</v>
+        <v>214</v>
       </c>
       <c r="I21" s="17">
         <v>74</v>
@@ -7205,11 +7205,11 @@
         <f t="shared" si="43"/>
         <v>Highly Satisfactory</v>
       </c>
-      <c r="BW21" s="98" t="s">
+      <c r="BW21" s="97" t="s">
         <v>170</v>
       </c>
     </row>
-    <row r="22" spans="1:75" ht="21.95" customHeight="1" x14ac:dyDescent="0.45">
+    <row r="22" spans="1:75" ht="21.95" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A22" s="16">
         <v>34</v>
       </c>
@@ -7232,7 +7232,7 @@
         <v>111</v>
       </c>
       <c r="H22" s="16" t="s">
-        <v>229</v>
+        <v>227</v>
       </c>
       <c r="I22" s="17">
         <v>80</v>
@@ -7481,7 +7481,7 @@
         <v>171</v>
       </c>
     </row>
-    <row r="23" spans="1:75" ht="15" x14ac:dyDescent="0.45">
+    <row r="23" spans="1:75" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A23" s="16">
         <v>20</v>
       </c>
@@ -7504,7 +7504,7 @@
         <v>111</v>
       </c>
       <c r="H23" s="16" t="s">
-        <v>230</v>
+        <v>228</v>
       </c>
       <c r="I23" s="17">
         <v>74</v>
@@ -7753,7 +7753,7 @@
         <v>172</v>
       </c>
     </row>
-    <row r="24" spans="1:75" ht="15" x14ac:dyDescent="0.45">
+    <row r="24" spans="1:75" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A24" s="16">
         <v>21</v>
       </c>
@@ -7776,7 +7776,7 @@
         <v>112</v>
       </c>
       <c r="H24" s="16" t="s">
-        <v>217</v>
+        <v>215</v>
       </c>
       <c r="I24" s="17">
         <v>74</v>
@@ -8025,7 +8025,7 @@
         <v>173</v>
       </c>
     </row>
-    <row r="25" spans="1:75" ht="15" x14ac:dyDescent="0.45">
+    <row r="25" spans="1:75" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A25" s="16">
         <v>22</v>
       </c>
@@ -8048,7 +8048,7 @@
         <v>112</v>
       </c>
       <c r="H25" s="16" t="s">
-        <v>218</v>
+        <v>216</v>
       </c>
       <c r="I25" s="17">
         <v>78</v>
@@ -8297,7 +8297,7 @@
         <v>174</v>
       </c>
     </row>
-    <row r="26" spans="1:75" ht="15" x14ac:dyDescent="0.45">
+    <row r="26" spans="1:75" x14ac:dyDescent="0.25">
       <c r="A26" s="16">
         <v>23</v>
       </c>
@@ -8320,7 +8320,7 @@
         <v>112</v>
       </c>
       <c r="H26" s="16" t="s">
-        <v>219</v>
+        <v>217</v>
       </c>
       <c r="I26" s="17">
         <v>75</v>
@@ -8569,7 +8569,7 @@
         <v>175</v>
       </c>
     </row>
-    <row r="27" spans="1:75" ht="15" x14ac:dyDescent="0.45">
+    <row r="27" spans="1:75" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A27" s="16">
         <v>24</v>
       </c>
@@ -8592,7 +8592,7 @@
         <v>111</v>
       </c>
       <c r="H27" s="16" t="s">
-        <v>231</v>
+        <v>229</v>
       </c>
       <c r="I27" s="17">
         <v>76</v>
@@ -8841,7 +8841,7 @@
         <v>176</v>
       </c>
     </row>
-    <row r="28" spans="1:75" ht="15" x14ac:dyDescent="0.45">
+    <row r="28" spans="1:75" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A28" s="16">
         <v>25</v>
       </c>
@@ -8864,7 +8864,7 @@
         <v>112</v>
       </c>
       <c r="H28" s="16" t="s">
-        <v>220</v>
+        <v>218</v>
       </c>
       <c r="I28" s="17">
         <v>74</v>
@@ -9113,7 +9113,7 @@
         <v>177</v>
       </c>
     </row>
-    <row r="29" spans="1:75" ht="15" x14ac:dyDescent="0.45">
+    <row r="29" spans="1:75" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A29" s="16">
         <v>26</v>
       </c>
@@ -9130,13 +9130,13 @@
         <v>146</v>
       </c>
       <c r="F29" s="75" t="s">
-        <v>194</v>
+        <v>193</v>
       </c>
       <c r="G29" s="75" t="s">
         <v>111</v>
       </c>
       <c r="H29" s="16" t="s">
-        <v>232</v>
+        <v>230</v>
       </c>
       <c r="I29" s="17">
         <v>78</v>
@@ -9385,11 +9385,11 @@
         <v>178</v>
       </c>
     </row>
-    <row r="30" spans="1:75" ht="15" x14ac:dyDescent="0.45">
+    <row r="30" spans="1:75" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A30" s="16">
         <v>27</v>
       </c>
-      <c r="B30" s="96" t="s">
+      <c r="B30" s="113" t="s">
         <v>54</v>
       </c>
       <c r="C30" s="16">
@@ -9408,7 +9408,7 @@
         <v>112</v>
       </c>
       <c r="H30" s="16" t="s">
-        <v>221</v>
+        <v>219</v>
       </c>
       <c r="I30" s="17">
         <v>74</v>
@@ -9654,10 +9654,10 @@
         <v>Highly Satisfactory</v>
       </c>
       <c r="BW30" s="95" t="s">
-        <v>198</v>
+        <v>196</v>
       </c>
     </row>
-    <row r="31" spans="1:75" ht="15" x14ac:dyDescent="0.45">
+    <row r="31" spans="1:75" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A31" s="16">
         <v>28</v>
       </c>
@@ -9680,7 +9680,7 @@
         <v>112</v>
       </c>
       <c r="H31" s="16" t="s">
-        <v>222</v>
+        <v>220</v>
       </c>
       <c r="I31" s="17">
         <v>78</v>
@@ -9929,11 +9929,11 @@
         <v>179</v>
       </c>
     </row>
-    <row r="32" spans="1:75" ht="15" x14ac:dyDescent="0.45">
+    <row r="32" spans="1:75" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A32" s="16">
         <v>29</v>
       </c>
-      <c r="B32" s="96" t="s">
+      <c r="B32" s="113" t="s">
         <v>56</v>
       </c>
       <c r="C32" s="16">
@@ -9952,7 +9952,7 @@
         <v>111</v>
       </c>
       <c r="H32" s="16" t="s">
-        <v>233</v>
+        <v>231</v>
       </c>
       <c r="I32" s="17">
         <v>74</v>
@@ -10197,9 +10197,11 @@
         <f t="shared" si="43"/>
         <v>Highly Satisfactory</v>
       </c>
-      <c r="BW32" s="95"/>
+      <c r="BW32" s="95" t="s">
+        <v>245</v>
+      </c>
     </row>
-    <row r="33" spans="1:75" ht="15" x14ac:dyDescent="0.45">
+    <row r="33" spans="1:75" x14ac:dyDescent="0.25">
       <c r="A33" s="16">
         <v>30</v>
       </c>
@@ -10222,7 +10224,7 @@
         <v>111</v>
       </c>
       <c r="H33" s="16" t="s">
-        <v>234</v>
+        <v>232</v>
       </c>
       <c r="I33" s="17">
         <v>80</v>
@@ -10471,7 +10473,7 @@
         <v>180</v>
       </c>
     </row>
-    <row r="34" spans="1:75" ht="15" x14ac:dyDescent="0.45">
+    <row r="34" spans="1:75" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A34" s="16">
         <v>31</v>
       </c>
@@ -10494,7 +10496,7 @@
         <v>112</v>
       </c>
       <c r="H34" s="16" t="s">
-        <v>223</v>
+        <v>221</v>
       </c>
       <c r="I34" s="17">
         <v>75</v>
@@ -10743,7 +10745,7 @@
         <v>181</v>
       </c>
     </row>
-    <row r="35" spans="1:75" ht="15" x14ac:dyDescent="0.45">
+    <row r="35" spans="1:75" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A35" s="16">
         <v>32</v>
       </c>
@@ -10766,7 +10768,7 @@
         <v>111</v>
       </c>
       <c r="H35" s="16" t="s">
-        <v>235</v>
+        <v>233</v>
       </c>
       <c r="I35" s="17">
         <v>79</v>
@@ -11011,11 +11013,11 @@
         <f t="shared" si="43"/>
         <v>Excellent</v>
       </c>
-      <c r="BW35" s="98" t="s">
+      <c r="BW35" s="97" t="s">
         <v>182</v>
       </c>
     </row>
-    <row r="36" spans="1:75" ht="15" x14ac:dyDescent="0.45">
+    <row r="36" spans="1:75" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A36" s="16">
         <v>33</v>
       </c>
@@ -11038,7 +11040,7 @@
         <v>111</v>
       </c>
       <c r="H36" s="16" t="s">
-        <v>236</v>
+        <v>234</v>
       </c>
       <c r="I36" s="17">
         <v>76</v>
@@ -11284,10 +11286,10 @@
         <v>Excellent</v>
       </c>
       <c r="BW36" s="95" t="s">
-        <v>195</v>
+        <v>246</v>
       </c>
     </row>
-    <row r="37" spans="1:75" ht="15" x14ac:dyDescent="0.45">
+    <row r="37" spans="1:75" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A37" s="16">
         <v>34</v>
       </c>
@@ -11310,7 +11312,7 @@
         <v>111</v>
       </c>
       <c r="H37" s="16" t="s">
-        <v>237</v>
+        <v>235</v>
       </c>
       <c r="I37" s="17">
         <v>80</v>
@@ -11555,11 +11557,11 @@
         <f t="shared" si="43"/>
         <v>Excellent</v>
       </c>
-      <c r="BW37" s="98" t="s">
+      <c r="BW37" s="97" t="s">
         <v>183</v>
       </c>
     </row>
-    <row r="38" spans="1:75" ht="15" x14ac:dyDescent="0.45">
+    <row r="38" spans="1:75" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A38" s="16">
         <v>35</v>
       </c>
@@ -11582,7 +11584,7 @@
         <v>111</v>
       </c>
       <c r="H38" s="16" t="s">
-        <v>238</v>
+        <v>236</v>
       </c>
       <c r="I38" s="17">
         <v>80</v>
@@ -11831,7 +11833,7 @@
         <v>184</v>
       </c>
     </row>
-    <row r="39" spans="1:75" ht="15" x14ac:dyDescent="0.45">
+    <row r="39" spans="1:75" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A39" s="16">
         <v>36</v>
       </c>
@@ -11854,7 +11856,7 @@
         <v>111</v>
       </c>
       <c r="H39" s="16" t="s">
-        <v>239</v>
+        <v>237</v>
       </c>
       <c r="I39" s="17">
         <v>80</v>
@@ -12103,7 +12105,7 @@
         <v>185</v>
       </c>
     </row>
-    <row r="40" spans="1:75" ht="15" x14ac:dyDescent="0.45">
+    <row r="40" spans="1:75" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A40" s="16">
         <v>37</v>
       </c>
@@ -12126,7 +12128,7 @@
         <v>112</v>
       </c>
       <c r="H40" s="16" t="s">
-        <v>224</v>
+        <v>222</v>
       </c>
       <c r="I40" s="63">
         <v>75</v>
@@ -12371,10 +12373,10 @@
         <v>Highly Satisfactory</v>
       </c>
       <c r="BW40" s="95" t="s">
-        <v>196</v>
+        <v>194</v>
       </c>
     </row>
-    <row r="41" spans="1:75" ht="15" x14ac:dyDescent="0.45">
+    <row r="41" spans="1:75" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A41" s="16">
         <v>38</v>
       </c>
@@ -12397,7 +12399,7 @@
         <v>111</v>
       </c>
       <c r="H41" s="16" t="s">
-        <v>240</v>
+        <v>238</v>
       </c>
       <c r="I41" s="17">
         <v>80</v>
@@ -12646,7 +12648,7 @@
         <v>186</v>
       </c>
     </row>
-    <row r="42" spans="1:75" ht="15" x14ac:dyDescent="0.45">
+    <row r="42" spans="1:75" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A42" s="16">
         <v>39</v>
       </c>
@@ -12669,7 +12671,7 @@
         <v>111</v>
       </c>
       <c r="H42" s="16" t="s">
-        <v>241</v>
+        <v>239</v>
       </c>
       <c r="I42" s="17">
         <v>80</v>
@@ -12918,7 +12920,7 @@
         <v>187</v>
       </c>
     </row>
-    <row r="43" spans="1:75" ht="15" x14ac:dyDescent="0.45">
+    <row r="43" spans="1:75" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A43" s="16">
         <v>40</v>
       </c>
@@ -12941,7 +12943,7 @@
         <v>111</v>
       </c>
       <c r="H43" s="16" t="s">
-        <v>242</v>
+        <v>240</v>
       </c>
       <c r="I43" s="17">
         <v>80</v>
@@ -13190,7 +13192,7 @@
         <v>188</v>
       </c>
     </row>
-    <row r="44" spans="1:75" ht="15" x14ac:dyDescent="0.45">
+    <row r="44" spans="1:75" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A44" s="16">
         <v>41</v>
       </c>
@@ -13213,7 +13215,7 @@
         <v>111</v>
       </c>
       <c r="H44" s="16" t="s">
-        <v>243</v>
+        <v>241</v>
       </c>
       <c r="I44" s="17">
         <v>74</v>
@@ -13459,10 +13461,10 @@
         <v>Highly Satisfactory</v>
       </c>
       <c r="BW44" s="95" t="s">
-        <v>193</v>
+        <v>247</v>
       </c>
     </row>
-    <row r="45" spans="1:75" ht="15" x14ac:dyDescent="0.45">
+    <row r="45" spans="1:75" x14ac:dyDescent="0.25">
       <c r="A45" s="16">
         <v>42</v>
       </c>
@@ -13485,7 +13487,7 @@
         <v>111</v>
       </c>
       <c r="H45" s="16" t="s">
-        <v>244</v>
+        <v>242</v>
       </c>
       <c r="I45" s="17">
         <v>75</v>
@@ -13734,7 +13736,7 @@
         <v>189</v>
       </c>
     </row>
-    <row r="46" spans="1:75" ht="15" x14ac:dyDescent="0.45">
+    <row r="46" spans="1:75" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A46" s="16">
         <v>43</v>
       </c>
@@ -13757,7 +13759,7 @@
         <v>111</v>
       </c>
       <c r="H46" s="16" t="s">
-        <v>245</v>
+        <v>243</v>
       </c>
       <c r="I46" s="17">
         <v>80</v>
@@ -14006,7 +14008,7 @@
         <v>190</v>
       </c>
     </row>
-    <row r="47" spans="1:75" ht="15" x14ac:dyDescent="0.45">
+    <row r="47" spans="1:75" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A47" s="16">
         <v>44</v>
       </c>
@@ -14029,7 +14031,7 @@
         <v>111</v>
       </c>
       <c r="H47" s="16" t="s">
-        <v>246</v>
+        <v>244</v>
       </c>
       <c r="I47" s="17">
         <v>80</v>
@@ -14274,31 +14276,12 @@
         <f t="shared" si="43"/>
         <v>Highly Satisfactory</v>
       </c>
-      <c r="BW47" s="98" t="s">
+      <c r="BW47" s="97" t="s">
         <v>191</v>
       </c>
     </row>
   </sheetData>
   <mergeCells count="29">
-    <mergeCell ref="BU1:BU2"/>
-    <mergeCell ref="BV1:BV2"/>
-    <mergeCell ref="BW1:BW2"/>
-    <mergeCell ref="BO1:BO2"/>
-    <mergeCell ref="BP1:BP2"/>
-    <mergeCell ref="BQ1:BQ2"/>
-    <mergeCell ref="BT1:BT2"/>
-    <mergeCell ref="S1:W1"/>
-    <mergeCell ref="X1:AB1"/>
-    <mergeCell ref="AC1:AG1"/>
-    <mergeCell ref="AH1:AL1"/>
-    <mergeCell ref="BL1:BL2"/>
-    <mergeCell ref="BN1:BN2"/>
-    <mergeCell ref="AM1:AQ1"/>
-    <mergeCell ref="AR1:AV1"/>
-    <mergeCell ref="AW1:BA1"/>
-    <mergeCell ref="BB1:BF1"/>
-    <mergeCell ref="BG1:BK1"/>
-    <mergeCell ref="BM1:BM2"/>
     <mergeCell ref="N1:R1"/>
     <mergeCell ref="A1:A2"/>
     <mergeCell ref="B1:B2"/>
@@ -14309,6 +14292,25 @@
     <mergeCell ref="F1:F2"/>
     <mergeCell ref="G1:G2"/>
     <mergeCell ref="H1:H2"/>
+    <mergeCell ref="BN1:BN2"/>
+    <mergeCell ref="AM1:AQ1"/>
+    <mergeCell ref="AR1:AV1"/>
+    <mergeCell ref="AW1:BA1"/>
+    <mergeCell ref="BB1:BF1"/>
+    <mergeCell ref="BG1:BK1"/>
+    <mergeCell ref="BM1:BM2"/>
+    <mergeCell ref="S1:W1"/>
+    <mergeCell ref="X1:AB1"/>
+    <mergeCell ref="AC1:AG1"/>
+    <mergeCell ref="AH1:AL1"/>
+    <mergeCell ref="BL1:BL2"/>
+    <mergeCell ref="BU1:BU2"/>
+    <mergeCell ref="BV1:BV2"/>
+    <mergeCell ref="BW1:BW2"/>
+    <mergeCell ref="BO1:BO2"/>
+    <mergeCell ref="BP1:BP2"/>
+    <mergeCell ref="BQ1:BQ2"/>
+    <mergeCell ref="BT1:BT2"/>
   </mergeCells>
   <phoneticPr fontId="13" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
menambahkan judul bahasa inggris di excel ners dan rpl
</commit_message>
<xml_diff>
--- a/Ners/2023-2024/Transkip Nilai Ners 2023-2024.xlsx
+++ b/Ners/2023-2024/Transkip Nilai Ners 2023-2024.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Nando\Documents\Stikes\Transkip Nilai 2025\Ners\2023-2024\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4FFB8D91-3D7C-4A14-A9E9-B7AC2C838359}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A03190A8-A1A0-4713-B0CB-85BB637E0513}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{435B60B8-694F-4DDA-ADD2-15262503367A}"/>
   </bookViews>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="404" uniqueCount="248">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="450" uniqueCount="294">
   <si>
     <t>NO</t>
   </si>
@@ -800,12 +800,150 @@
   <si>
     <t>Asuhan Keperawatan Halusinasi Pada Nn.L Dengan Skizofrenia Paranoid Dan Penerapan Strategi Pelaksanaan Halusinasi Di Wilayah Daik Lingga Tahun 2024</t>
   </si>
+  <si>
+    <t>JUDUL INGGRIS</t>
+  </si>
+  <si>
+    <t>Chronic Pain Nursing Care in Mr. Y with Cholelithiasis and Application of Guided Imagery at Palmatak Regional General Hospital, Anambas Islands, 2023</t>
+  </si>
+  <si>
+    <t>Acute Pain Nursing Care in Mr. S with Hypertension and Application of Warm Compress on Five Fingers in the Siantan Public Health Center Working Area, 2024</t>
+  </si>
+  <si>
+    <t>Chronic Pain Nursing Care in Mr. A with Hypertension and Application of Warm Water Foot Soak in Ladam Village, Palmatak District, 2024</t>
+  </si>
+  <si>
+    <t>Hypokalemia Nursing Care in Mr./Ms. D with Gastroenteritis and Application of Honey and Oral Rehydration Solution Administration in the Pediatric Ward of Tarempa Regional General Hospital</t>
+  </si>
+  <si>
+    <t>Nursing Care for Mr. A's Family for Mrs. P with Hypertension with the Administration of Boiled Moringa Leaf Therapy in Bukit Village, East Jemaja District, 2024</t>
+  </si>
+  <si>
+    <t>Nursing Care for Ineffective Cerebral Tissue Perfusion Risk in Mr. A with Mild Head Injury and Application of Slow Deep Breathing Therapy in the Emergency Room of Tarempa Regional General Hospital, 2024</t>
+  </si>
+  <si>
+    <t>Nursing Care for Impaired Physical Mobility in Mr. D with Non-Hemorrhagic Stroke and Application of Passive Range of Motion Therapy in the Inpatient Ward of Tarempa Regional General Hospital, 2023</t>
+  </si>
+  <si>
+    <t>Application of Pre and Post Nursing Conference to Improve the Quality of Nursing Care in the Inpatient Ward of Tarempa Regional General Hospital</t>
+  </si>
+  <si>
+    <t>Nursing Care for Unstable Blood Glucose Levels in Mrs. L with Diabetes Mellitus and Application of Foot Exercises at Palmatak Public Health Center, 2024</t>
+  </si>
+  <si>
+    <t>Acute Pain Nursing Care in Mrs. E with Hypertension and Application of Warm Water Foot Soak in Ladam Village, Palmatak District, 2024</t>
+  </si>
+  <si>
+    <t>Nursing Care for Ineffective Peripheral Perfusion in Mrs. H with Hypertension and Application of Warm Water Foot Soak Therapy in Tebang Village, Palmatak District, 2024</t>
+  </si>
+  <si>
+    <t>Nursing Care for Ineffective Airway Clearance in Mr./Ms. F with Bronchopneumonia and Application of Postural Drainage, Clapping, and Effective Cough in the Pediatric Ward of Tarempa Regional General Hospital, 2024</t>
+  </si>
+  <si>
+    <t>Acute Pain Nursing Care in Mr. A with Low Back Pain and Application of Benson Relaxation Therapy in the Male Inpatient Ward of Tarempa Regional General Hospital</t>
+  </si>
+  <si>
+    <t>Hypovolemia Nursing Care in Mr./Ms. F with Dengue Hemorrhagic Fever (DHF) and Application of Fluid Administration Education at Tarempa Regional General Hospital</t>
+  </si>
+  <si>
+    <t>Nursing Care for Ineffective Breathing Pattern in Mrs. S with Asthmatic Status and Application of Buteyko Installation in the Emergency Room of Palmatak Regional General Hospital, 2024</t>
+  </si>
+  <si>
+    <t>Nursing Care for Ineffective Cerebral Perfusion Risk in Mrs. Y with Hypertension and Application of Boiled Betel Leaf in East Tarempa Village, Tarempa Public Health Center Working Area, 2024</t>
+  </si>
+  <si>
+    <t>Nursing Care for Ineffective Airway Clearance in Mr. D with Effective Cough &amp; Pursed Lips Breathing Technique in the Inpatient Ward of Palmatak Regional General Hospital</t>
+  </si>
+  <si>
+    <t>Acute Pain Nursing Care in Mrs. R with Hypertension and Application of Watermelon Juice in East Tarempa Village</t>
+  </si>
+  <si>
+    <t>Acute Pain Nursing Care in Mrs. N with Post-Appendectomy Operation and Application of Benson Relaxation Technique in the Female Inpatient Ward of Palmatak Regional General Hospital</t>
+  </si>
+  <si>
+    <t>Nursing Care for Decreased Cardiac Output in Mrs. S with Medical Diagnosis of Hypertension and Application of Cucumber Juice Administration in the East Jemaja Public Health Center Working Area</t>
+  </si>
+  <si>
+    <t>Chronic Pain Nursing Care in Mr. M with Osteoarthritis and Application of Range of Motion (ROM) Exercise in Ladam Village, Palmatak District, 2024</t>
+  </si>
+  <si>
+    <t>Application of Handover Using SBAR Communication Technique on Patient Safety in the Palmatak Inpatient Ward, 2024</t>
+  </si>
+  <si>
+    <t>Hyperthermia Nursing Care in Mrs. K with Hypertension and Application of Acupressure Therapy in Ladam Village, Palmatak District, 2024</t>
+  </si>
+  <si>
+    <t>Hyperthermia Nursing Care in Mr./Ms. M with Hyperpyrexia and Application of Warm Water Compress in the Pediatric Ward of Tarempa Regional General Hospital</t>
+  </si>
+  <si>
+    <t>Nursing Care for Impaired Skin Integrity in Mr. A with Diabetes Mellitus and Application of Metronidazole Compress at Tarempa Regional General Hospital</t>
+  </si>
+  <si>
+    <t>Acute Pain Nursing Care in Mrs. A with Post-Caesarean Section and Application of Effleurage Massage Relaxation Technique at Palmatak Regional General Hospital, 2023</t>
+  </si>
+  <si>
+    <t>Application of Lemon Oil Aromatherapy in Mrs. R with Hyperemesis Gravidarum (Heg) in the Midwifery Ward of East Jemaja Public Health Center, 2023</t>
+  </si>
+  <si>
+    <t>Hyperthermia Nursing Care in Mr./Ms. A with Febrile Seizures and Application of Onion Compress in the Pediatric Inpatient Ward of Tarempa Regional General Hospital</t>
+  </si>
+  <si>
+    <t>Hyperthermia Nursing Care in Mrs. A with Osteoarthritis and Application of Active Range of Motion (ROM) Exercise in East Tarempa Village, Tarempa Public Health Center Working Area, 2024</t>
+  </si>
+  <si>
+    <t>Acute Pain Nursing Care in Mr. M with Gout Arthritis and Application of Warm Jeram Compress in the Pediatric Ward of Tarempa</t>
+  </si>
+  <si>
+    <t>Chronic Pain Nursing Care in Mr. S with Ca. Buik (Abdominal Cancer) and Application of Guided Relaxation Technique in the Male Inpatient Ward of Tarempa Regional General Hospital, 2023</t>
+  </si>
+  <si>
+    <t>Acute Pain Nursing Care in Mrs. B with Post-Caesarean Section and Application of Benson Relaxation Therapy in the Maternity Inpatient Ward of Palmatak Regional General Hospital</t>
+  </si>
+  <si>
+    <t>Nursing Care for Unstable Blood Glucose Levels in Mrs. J with Diabetes Mellitus and Application of Dhikr Therapy in the Female Ward of Dabo Regional General Hospital, 2023</t>
+  </si>
+  <si>
+    <t>Nursing Care for Impaired Growth and Development in Mr./Ms. Er with Stunting in Mr. I's Family and Application of Tu Na Massage in RT 01 RW 02 Raya Village, West Singkep District, 2023</t>
+  </si>
+  <si>
+    <t>Acute Pain Nursing Care in Infant I with Post-Appendectomy and Application of Benson Relaxation at Dabo Regional General Hospital, 2023</t>
+  </si>
+  <si>
+    <t>Chronic Pain Nursing Care in Mrs. A with Ca. Mamae (Breast Cancer) and Application of Benson Relaxation Technique in the Female Ward of Dabo Regional General Hospital, 2023</t>
+  </si>
+  <si>
+    <t>Nursing Care for Ineffective Airway Clearance in Mr. Y with COPD and Application of Pursed Lip Breathing in the Male Ward of Dabo Regional General Hospital, 2023</t>
+  </si>
+  <si>
+    <t>Nursing Care for Impaired Skin Integrity in Mr./Ms. A with Burn Wound and Application of Aloe Vera in Cinda Pavilion, Encik Mariyam Regional General Hospital, Lingga Regency</t>
+  </si>
+  <si>
+    <t>Acute Pain Nursing Care in Mr. A with Hemorrhoidality and Application of Finger Clenching Relaxation Technique at Dabo Regional General Hospital, 2023</t>
+  </si>
+  <si>
+    <t>Acute Pain Nursing Care in Mrs. H with Post-Hemorrhoidectomy Operation and Application of Cold Compress in the Female Ward of Dabo Regional General Hospital, 2023</t>
+  </si>
+  <si>
+    <t>Nursing Care for Ineffective Airway Clearance in Mr./Ms. A and Implementation of Hot Water Vapor Therapy and Eucalyptus Oil in the Pediatric Ward of Dabo Regional General Hospital</t>
+  </si>
+  <si>
+    <t>Nursing Care for Hallucinations in Ms. L with Paranoid Schizophrenia and Application of Hallucination Implementation Strategy in the Dabo, Lingga Region, 2024</t>
+  </si>
+  <si>
+    <t>Acute Pain Nursing Care in Mrs. M with Post-Caesarean Section Operation and Application of Early Mobilization in the Songket Inpatient Ward, Encik Mariyam Regional General Hospital, 2024</t>
+  </si>
+  <si>
+    <t>Acute Pain Nursing Care in Mrs. M with Post-Caesarean Section Operation and Application of Lavender Aromatherapy at Dabo Regional General Hospital, 2023</t>
+  </si>
+  <si>
+    <t>Application of Hand Hygiene Principle in the Surgical Ward of Dabo Regional General Hospital, 2024</t>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="15" x14ac:knownFonts="1">
+  <fonts count="16" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -894,6 +1032,13 @@
     </font>
     <font>
       <i/>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Arial"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <b/>
       <sz val="11"/>
       <color theme="1"/>
       <name val="Arial"/>
@@ -1017,7 +1162,7 @@
       <alignment vertical="center"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="114">
+  <cellXfs count="115">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="10" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -1302,19 +1447,34 @@
     <xf numFmtId="0" fontId="11" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="11" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="1" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="1" fillId="2" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="9" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="10" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="1" fillId="11" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="12" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="13" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="14" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="5" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -1329,33 +1489,19 @@
     <xf numFmtId="0" fontId="1" fillId="8" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="9" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="10" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="12" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="13" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="14" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="49" fontId="1" fillId="2" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="3">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -1672,13 +1818,13 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{FE191EAF-C86A-4A83-8BAB-B026E2D7004C}">
-  <dimension ref="A1:BW47"/>
+  <dimension ref="A1:BX47"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <pane xSplit="2" ySplit="2" topLeftCell="BJ21" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="2" ySplit="2" topLeftCell="C24" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="C1" sqref="C1"/>
       <selection pane="bottomLeft" activeCell="A3" sqref="A3"/>
-      <selection pane="bottomRight" activeCell="B32" sqref="B32"/>
+      <selection pane="bottomRight" activeCell="I46" sqref="I46"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1708,127 +1854,128 @@
     <col min="72" max="72" width="13.42578125" customWidth="1"/>
     <col min="73" max="73" width="18.140625" customWidth="1"/>
     <col min="74" max="74" width="17.85546875" customWidth="1"/>
-    <col min="75" max="75" width="27.28515625" customWidth="1"/>
+    <col min="75" max="75" width="201.5703125" bestFit="1" customWidth="1"/>
+    <col min="76" max="76" width="194" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:75" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A1" s="99" t="s">
+    <row r="1" spans="1:76" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A1" s="97" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="99" t="s">
+      <c r="B1" s="97" t="s">
         <v>1</v>
       </c>
-      <c r="C1" s="99" t="s">
+      <c r="C1" s="97" t="s">
         <v>2</v>
       </c>
-      <c r="D1" s="99" t="s">
-        <v>3</v>
-      </c>
-      <c r="E1" s="99" t="s">
+      <c r="D1" s="97" t="s">
+        <v>3</v>
+      </c>
+      <c r="E1" s="97" t="s">
         <v>73</v>
       </c>
-      <c r="F1" s="112" t="s">
+      <c r="F1" s="99" t="s">
         <v>74</v>
       </c>
-      <c r="G1" s="112" t="s">
+      <c r="G1" s="99" t="s">
         <v>75</v>
       </c>
-      <c r="H1" s="99" t="s">
+      <c r="H1" s="97" t="s">
         <v>76</v>
       </c>
-      <c r="I1" s="111" t="s">
-        <v>4</v>
-      </c>
-      <c r="J1" s="111"/>
-      <c r="K1" s="111"/>
-      <c r="L1" s="111"/>
-      <c r="M1" s="111"/>
-      <c r="N1" s="110" t="s">
+      <c r="I1" s="98" t="s">
+        <v>4</v>
+      </c>
+      <c r="J1" s="98"/>
+      <c r="K1" s="98"/>
+      <c r="L1" s="98"/>
+      <c r="M1" s="98"/>
+      <c r="N1" s="96" t="s">
         <v>5</v>
       </c>
-      <c r="O1" s="110"/>
-      <c r="P1" s="110"/>
-      <c r="Q1" s="110"/>
-      <c r="R1" s="110"/>
-      <c r="S1" s="101" t="s">
+      <c r="O1" s="96"/>
+      <c r="P1" s="96"/>
+      <c r="Q1" s="96"/>
+      <c r="R1" s="96"/>
+      <c r="S1" s="106" t="s">
         <v>6</v>
       </c>
-      <c r="T1" s="101"/>
-      <c r="U1" s="101"/>
-      <c r="V1" s="101"/>
-      <c r="W1" s="101"/>
-      <c r="X1" s="102" t="s">
+      <c r="T1" s="106"/>
+      <c r="U1" s="106"/>
+      <c r="V1" s="106"/>
+      <c r="W1" s="106"/>
+      <c r="X1" s="107" t="s">
         <v>7</v>
       </c>
-      <c r="Y1" s="102"/>
-      <c r="Z1" s="102"/>
-      <c r="AA1" s="102"/>
-      <c r="AB1" s="102"/>
-      <c r="AC1" s="103" t="s">
+      <c r="Y1" s="107"/>
+      <c r="Z1" s="107"/>
+      <c r="AA1" s="107"/>
+      <c r="AB1" s="107"/>
+      <c r="AC1" s="108" t="s">
         <v>8</v>
       </c>
-      <c r="AD1" s="103"/>
-      <c r="AE1" s="103"/>
-      <c r="AF1" s="103"/>
-      <c r="AG1" s="103"/>
-      <c r="AH1" s="104" t="s">
+      <c r="AD1" s="108"/>
+      <c r="AE1" s="108"/>
+      <c r="AF1" s="108"/>
+      <c r="AG1" s="108"/>
+      <c r="AH1" s="109" t="s">
         <v>9</v>
       </c>
-      <c r="AI1" s="104"/>
-      <c r="AJ1" s="104"/>
-      <c r="AK1" s="104"/>
-      <c r="AL1" s="104"/>
-      <c r="AM1" s="106" t="s">
+      <c r="AI1" s="109"/>
+      <c r="AJ1" s="109"/>
+      <c r="AK1" s="109"/>
+      <c r="AL1" s="109"/>
+      <c r="AM1" s="101" t="s">
         <v>13</v>
       </c>
-      <c r="AN1" s="106"/>
-      <c r="AO1" s="106"/>
-      <c r="AP1" s="106"/>
-      <c r="AQ1" s="106"/>
-      <c r="AR1" s="100" t="s">
+      <c r="AN1" s="101"/>
+      <c r="AO1" s="101"/>
+      <c r="AP1" s="101"/>
+      <c r="AQ1" s="101"/>
+      <c r="AR1" s="102" t="s">
         <v>14</v>
       </c>
-      <c r="AS1" s="100"/>
-      <c r="AT1" s="100"/>
-      <c r="AU1" s="100"/>
-      <c r="AV1" s="100"/>
-      <c r="AW1" s="107" t="s">
+      <c r="AS1" s="102"/>
+      <c r="AT1" s="102"/>
+      <c r="AU1" s="102"/>
+      <c r="AV1" s="102"/>
+      <c r="AW1" s="103" t="s">
         <v>15</v>
       </c>
-      <c r="AX1" s="107"/>
-      <c r="AY1" s="107"/>
-      <c r="AZ1" s="107"/>
-      <c r="BA1" s="107"/>
-      <c r="BB1" s="108" t="s">
+      <c r="AX1" s="103"/>
+      <c r="AY1" s="103"/>
+      <c r="AZ1" s="103"/>
+      <c r="BA1" s="103"/>
+      <c r="BB1" s="104" t="s">
         <v>16</v>
       </c>
-      <c r="BC1" s="108"/>
-      <c r="BD1" s="108"/>
-      <c r="BE1" s="108"/>
-      <c r="BF1" s="108"/>
-      <c r="BG1" s="109" t="s">
+      <c r="BC1" s="104"/>
+      <c r="BD1" s="104"/>
+      <c r="BE1" s="104"/>
+      <c r="BF1" s="104"/>
+      <c r="BG1" s="105" t="s">
         <v>17</v>
       </c>
-      <c r="BH1" s="109"/>
-      <c r="BI1" s="109"/>
-      <c r="BJ1" s="109"/>
-      <c r="BK1" s="109"/>
-      <c r="BL1" s="105" t="s">
+      <c r="BH1" s="105"/>
+      <c r="BI1" s="105"/>
+      <c r="BJ1" s="105"/>
+      <c r="BK1" s="105"/>
+      <c r="BL1" s="100" t="s">
         <v>10</v>
       </c>
-      <c r="BM1" s="105" t="s">
+      <c r="BM1" s="100" t="s">
         <v>11</v>
       </c>
-      <c r="BN1" s="105" t="s">
+      <c r="BN1" s="100" t="s">
         <v>12</v>
       </c>
-      <c r="BO1" s="99" t="s">
+      <c r="BO1" s="97" t="s">
         <v>10</v>
       </c>
-      <c r="BP1" s="99" t="s">
+      <c r="BP1" s="97" t="s">
         <v>11</v>
       </c>
-      <c r="BQ1" s="99" t="s">
+      <c r="BQ1" s="97" t="s">
         <v>12</v>
       </c>
       <c r="BR1" s="2" t="s">
@@ -1837,28 +1984,31 @@
       <c r="BS1" s="2" t="s">
         <v>18</v>
       </c>
-      <c r="BT1" s="100" t="s">
+      <c r="BT1" s="102" t="s">
         <v>19</v>
       </c>
-      <c r="BU1" s="98" t="s">
+      <c r="BU1" s="110" t="s">
         <v>77</v>
       </c>
-      <c r="BV1" s="98" t="s">
+      <c r="BV1" s="110" t="s">
         <v>78</v>
       </c>
-      <c r="BW1" s="98" t="s">
+      <c r="BW1" s="110" t="s">
         <v>79</v>
       </c>
+      <c r="BX1" s="113" t="s">
+        <v>248</v>
+      </c>
     </row>
-    <row r="2" spans="1:75" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A2" s="99"/>
-      <c r="B2" s="99"/>
-      <c r="C2" s="99"/>
-      <c r="D2" s="99"/>
-      <c r="E2" s="99"/>
-      <c r="F2" s="112"/>
-      <c r="G2" s="112"/>
-      <c r="H2" s="99"/>
+    <row r="2" spans="1:76" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A2" s="97"/>
+      <c r="B2" s="97"/>
+      <c r="C2" s="97"/>
+      <c r="D2" s="97"/>
+      <c r="E2" s="97"/>
+      <c r="F2" s="99"/>
+      <c r="G2" s="99"/>
+      <c r="H2" s="97"/>
       <c r="I2" s="7" t="s">
         <v>20</v>
       </c>
@@ -2024,24 +2174,25 @@
       <c r="BK2" s="5" t="s">
         <v>24</v>
       </c>
-      <c r="BL2" s="105"/>
-      <c r="BM2" s="105"/>
-      <c r="BN2" s="105"/>
-      <c r="BO2" s="99"/>
-      <c r="BP2" s="99"/>
-      <c r="BQ2" s="99"/>
+      <c r="BL2" s="100"/>
+      <c r="BM2" s="100"/>
+      <c r="BN2" s="100"/>
+      <c r="BO2" s="97"/>
+      <c r="BP2" s="97"/>
+      <c r="BQ2" s="97"/>
       <c r="BR2" s="2" t="s">
         <v>20</v>
       </c>
       <c r="BS2" s="2" t="s">
         <v>25</v>
       </c>
-      <c r="BT2" s="100"/>
-      <c r="BU2" s="98"/>
-      <c r="BV2" s="98"/>
-      <c r="BW2" s="98"/>
+      <c r="BT2" s="102"/>
+      <c r="BU2" s="110"/>
+      <c r="BV2" s="110"/>
+      <c r="BW2" s="110"/>
+      <c r="BX2" s="113"/>
     </row>
-    <row r="3" spans="1:75" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:76" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A3" s="16">
         <v>1</v>
       </c>
@@ -2309,11 +2460,14 @@
         <f>IF(BT3&gt;=3.51,"Excellent",(IF(BT3&gt;=2.75,"Highly Satisfactory",(IF(BT3&gt;=2,"Satisfactory","FAILED")))))</f>
         <v>Highly Satisfactory</v>
       </c>
-      <c r="BW3" s="96" t="s">
+      <c r="BW3" s="111" t="s">
         <v>155</v>
       </c>
+      <c r="BX3" s="114" t="s">
+        <v>249</v>
+      </c>
     </row>
-    <row r="4" spans="1:75" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:76" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A4" s="16">
         <v>2</v>
       </c>
@@ -2581,11 +2735,14 @@
         <f t="shared" ref="BV4:BV47" si="43">IF(BT4&gt;=3.51,"Excellent",(IF(BT4&gt;=2.75,"Highly Satisfactory",(IF(BT4&gt;=2,"Satisfactory","FAILED")))))</f>
         <v>Highly Satisfactory</v>
       </c>
-      <c r="BW4" s="95" t="s">
+      <c r="BW4" s="111" t="s">
         <v>156</v>
       </c>
+      <c r="BX4" s="114" t="s">
+        <v>250</v>
+      </c>
     </row>
-    <row r="5" spans="1:75" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:76" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A5" s="16">
         <v>3</v>
       </c>
@@ -2853,11 +3010,14 @@
         <f t="shared" si="43"/>
         <v>Excellent</v>
       </c>
-      <c r="BW5" s="95" t="s">
+      <c r="BW5" s="111" t="s">
         <v>199</v>
       </c>
+      <c r="BX5" s="114" t="s">
+        <v>251</v>
+      </c>
     </row>
-    <row r="6" spans="1:75" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:76" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A6" s="16">
         <v>4</v>
       </c>
@@ -3125,11 +3285,14 @@
         <f t="shared" si="43"/>
         <v>Excellent</v>
       </c>
-      <c r="BW6" s="96" t="s">
+      <c r="BW6" s="111" t="s">
         <v>157</v>
       </c>
+      <c r="BX6" s="114" t="s">
+        <v>252</v>
+      </c>
     </row>
-    <row r="7" spans="1:75" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:76" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A7" s="16">
         <v>5</v>
       </c>
@@ -3397,11 +3560,14 @@
         <f t="shared" si="43"/>
         <v>Excellent</v>
       </c>
-      <c r="BW7" s="95" t="s">
+      <c r="BW7" s="111" t="s">
         <v>158</v>
       </c>
+      <c r="BX7" s="114" t="s">
+        <v>253</v>
+      </c>
     </row>
-    <row r="8" spans="1:75" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:76" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A8" s="16">
         <v>6</v>
       </c>
@@ -3669,11 +3835,14 @@
         <f t="shared" si="43"/>
         <v>Highly Satisfactory</v>
       </c>
-      <c r="BW8" s="95" t="s">
+      <c r="BW8" s="111" t="s">
         <v>159</v>
       </c>
+      <c r="BX8" s="114" t="s">
+        <v>254</v>
+      </c>
     </row>
-    <row r="9" spans="1:75" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:76" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A9" s="16">
         <v>7</v>
       </c>
@@ -3941,11 +4110,14 @@
         <f t="shared" si="43"/>
         <v>Excellent</v>
       </c>
-      <c r="BW9" s="95" t="s">
+      <c r="BW9" s="111" t="s">
         <v>160</v>
       </c>
+      <c r="BX9" s="114" t="s">
+        <v>255</v>
+      </c>
     </row>
-    <row r="10" spans="1:75" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:76" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A10" s="16">
         <v>8</v>
       </c>
@@ -4213,11 +4385,14 @@
         <f t="shared" si="43"/>
         <v>Highly Satisfactory</v>
       </c>
-      <c r="BW10" s="95" t="s">
+      <c r="BW10" s="111" t="s">
         <v>192</v>
       </c>
+      <c r="BX10" s="114" t="s">
+        <v>256</v>
+      </c>
     </row>
-    <row r="11" spans="1:75" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:76" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A11" s="16">
         <v>9</v>
       </c>
@@ -4485,11 +4660,14 @@
         <f t="shared" si="43"/>
         <v>Highly Satisfactory</v>
       </c>
-      <c r="BW11" s="95" t="s">
+      <c r="BW11" s="111" t="s">
         <v>161</v>
       </c>
+      <c r="BX11" s="114" t="s">
+        <v>257</v>
+      </c>
     </row>
-    <row r="12" spans="1:75" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:76" x14ac:dyDescent="0.25">
       <c r="A12" s="16">
         <v>10</v>
       </c>
@@ -4757,11 +4935,14 @@
         <f t="shared" si="43"/>
         <v>Highly Satisfactory</v>
       </c>
-      <c r="BW12" s="95" t="s">
+      <c r="BW12" s="111" t="s">
         <v>162</v>
       </c>
+      <c r="BX12" s="114" t="s">
+        <v>258</v>
+      </c>
     </row>
-    <row r="13" spans="1:75" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:76" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A13" s="16">
         <v>11</v>
       </c>
@@ -5029,11 +5210,14 @@
         <f t="shared" si="43"/>
         <v>Highly Satisfactory</v>
       </c>
-      <c r="BW13" s="95" t="s">
+      <c r="BW13" s="111" t="s">
         <v>163</v>
       </c>
+      <c r="BX13" s="114" t="s">
+        <v>259</v>
+      </c>
     </row>
-    <row r="14" spans="1:75" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:76" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A14" s="16">
         <v>12</v>
       </c>
@@ -5301,11 +5485,14 @@
         <f t="shared" si="43"/>
         <v>Highly Satisfactory</v>
       </c>
-      <c r="BW14" s="95" t="s">
+      <c r="BW14" s="111" t="s">
         <v>164</v>
       </c>
+      <c r="BX14" s="114" t="s">
+        <v>260</v>
+      </c>
     </row>
-    <row r="15" spans="1:75" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:76" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A15" s="16">
         <v>13</v>
       </c>
@@ -5573,11 +5760,14 @@
         <f t="shared" si="43"/>
         <v>Excellent</v>
       </c>
-      <c r="BW15" s="95" t="s">
+      <c r="BW15" s="111" t="s">
         <v>165</v>
       </c>
+      <c r="BX15" s="114" t="s">
+        <v>261</v>
+      </c>
     </row>
-    <row r="16" spans="1:75" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:76" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A16" s="16">
         <v>14</v>
       </c>
@@ -5845,11 +6035,14 @@
         <f t="shared" si="43"/>
         <v>Highly Satisfactory</v>
       </c>
-      <c r="BW16" s="97" t="s">
+      <c r="BW16" s="112" t="s">
         <v>166</v>
       </c>
+      <c r="BX16" s="114" t="s">
+        <v>262</v>
+      </c>
     </row>
-    <row r="17" spans="1:75" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:76" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A17" s="16">
         <v>15</v>
       </c>
@@ -6117,11 +6310,14 @@
         <f t="shared" si="43"/>
         <v>Highly Satisfactory</v>
       </c>
-      <c r="BW17" s="95" t="s">
+      <c r="BW17" s="111" t="s">
         <v>167</v>
       </c>
+      <c r="BX17" s="114" t="s">
+        <v>263</v>
+      </c>
     </row>
-    <row r="18" spans="1:75" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:76" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A18" s="16">
         <v>16</v>
       </c>
@@ -6389,11 +6585,14 @@
         <f t="shared" si="43"/>
         <v>Highly Satisfactory</v>
       </c>
-      <c r="BW18" s="95" t="s">
+      <c r="BW18" s="111" t="s">
         <v>168</v>
       </c>
+      <c r="BX18" s="114" t="s">
+        <v>264</v>
+      </c>
     </row>
-    <row r="19" spans="1:75" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:76" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A19" s="16">
         <v>17</v>
       </c>
@@ -6661,11 +6860,14 @@
         <f t="shared" si="43"/>
         <v>Highly Satisfactory</v>
       </c>
-      <c r="BW19" s="95" t="s">
+      <c r="BW19" s="111" t="s">
         <v>195</v>
       </c>
+      <c r="BX19" s="114" t="s">
+        <v>265</v>
+      </c>
     </row>
-    <row r="20" spans="1:75" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:76" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A20" s="16">
         <v>18</v>
       </c>
@@ -6933,11 +7135,14 @@
         <f t="shared" si="43"/>
         <v>Highly Satisfactory</v>
       </c>
-      <c r="BW20" s="95" t="s">
+      <c r="BW20" s="111" t="s">
         <v>169</v>
       </c>
+      <c r="BX20" s="114" t="s">
+        <v>266</v>
+      </c>
     </row>
-    <row r="21" spans="1:75" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:76" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A21" s="16">
         <v>19</v>
       </c>
@@ -7205,11 +7410,14 @@
         <f t="shared" si="43"/>
         <v>Highly Satisfactory</v>
       </c>
-      <c r="BW21" s="97" t="s">
+      <c r="BW21" s="112" t="s">
         <v>170</v>
       </c>
+      <c r="BX21" s="114" t="s">
+        <v>267</v>
+      </c>
     </row>
-    <row r="22" spans="1:75" ht="21.95" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:76" ht="21.95" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A22" s="16">
         <v>34</v>
       </c>
@@ -7477,11 +7685,14 @@
         <f t="shared" si="43"/>
         <v>Excellent</v>
       </c>
-      <c r="BW22" s="95" t="s">
+      <c r="BW22" s="111" t="s">
         <v>171</v>
       </c>
+      <c r="BX22" s="114" t="s">
+        <v>268</v>
+      </c>
     </row>
-    <row r="23" spans="1:75" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:76" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A23" s="16">
         <v>20</v>
       </c>
@@ -7749,11 +7960,14 @@
         <f t="shared" si="43"/>
         <v>Highly Satisfactory</v>
       </c>
-      <c r="BW23" s="95" t="s">
+      <c r="BW23" s="111" t="s">
         <v>172</v>
       </c>
+      <c r="BX23" s="114" t="s">
+        <v>269</v>
+      </c>
     </row>
-    <row r="24" spans="1:75" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:76" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A24" s="16">
         <v>21</v>
       </c>
@@ -8021,11 +8235,14 @@
         <f t="shared" si="43"/>
         <v>Highly Satisfactory</v>
       </c>
-      <c r="BW24" s="95" t="s">
+      <c r="BW24" s="111" t="s">
         <v>173</v>
       </c>
+      <c r="BX24" s="114" t="s">
+        <v>270</v>
+      </c>
     </row>
-    <row r="25" spans="1:75" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:76" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A25" s="16">
         <v>22</v>
       </c>
@@ -8293,11 +8510,14 @@
         <f t="shared" si="43"/>
         <v>Excellent</v>
       </c>
-      <c r="BW25" s="95" t="s">
+      <c r="BW25" s="111" t="s">
         <v>174</v>
       </c>
+      <c r="BX25" s="114" t="s">
+        <v>271</v>
+      </c>
     </row>
-    <row r="26" spans="1:75" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:76" x14ac:dyDescent="0.25">
       <c r="A26" s="16">
         <v>23</v>
       </c>
@@ -8565,11 +8785,14 @@
         <f t="shared" si="43"/>
         <v>Highly Satisfactory</v>
       </c>
-      <c r="BW26" s="95" t="s">
+      <c r="BW26" s="111" t="s">
         <v>175</v>
       </c>
+      <c r="BX26" s="114" t="s">
+        <v>272</v>
+      </c>
     </row>
-    <row r="27" spans="1:75" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:76" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A27" s="16">
         <v>24</v>
       </c>
@@ -8837,11 +9060,14 @@
         <f t="shared" si="43"/>
         <v>Excellent</v>
       </c>
-      <c r="BW27" s="95" t="s">
+      <c r="BW27" s="111" t="s">
         <v>176</v>
       </c>
+      <c r="BX27" s="114" t="s">
+        <v>273</v>
+      </c>
     </row>
-    <row r="28" spans="1:75" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:76" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A28" s="16">
         <v>25</v>
       </c>
@@ -9109,11 +9335,14 @@
         <f t="shared" si="43"/>
         <v>Highly Satisfactory</v>
       </c>
-      <c r="BW28" s="95" t="s">
+      <c r="BW28" s="111" t="s">
         <v>177</v>
       </c>
+      <c r="BX28" s="114" t="s">
+        <v>274</v>
+      </c>
     </row>
-    <row r="29" spans="1:75" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:76" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A29" s="16">
         <v>26</v>
       </c>
@@ -9381,15 +9610,18 @@
         <f t="shared" si="43"/>
         <v>Excellent</v>
       </c>
-      <c r="BW29" s="95" t="s">
+      <c r="BW29" s="111" t="s">
         <v>178</v>
       </c>
+      <c r="BX29" s="114" t="s">
+        <v>275</v>
+      </c>
     </row>
-    <row r="30" spans="1:75" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:76" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A30" s="16">
         <v>27</v>
       </c>
-      <c r="B30" s="113" t="s">
+      <c r="B30" s="16" t="s">
         <v>54</v>
       </c>
       <c r="C30" s="16">
@@ -9653,11 +9885,14 @@
         <f t="shared" si="43"/>
         <v>Highly Satisfactory</v>
       </c>
-      <c r="BW30" s="95" t="s">
+      <c r="BW30" s="111" t="s">
         <v>196</v>
       </c>
+      <c r="BX30" s="114" t="s">
+        <v>276</v>
+      </c>
     </row>
-    <row r="31" spans="1:75" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:76" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A31" s="16">
         <v>28</v>
       </c>
@@ -9925,15 +10160,18 @@
         <f t="shared" si="43"/>
         <v>Highly Satisfactory</v>
       </c>
-      <c r="BW31" s="95" t="s">
+      <c r="BW31" s="111" t="s">
         <v>179</v>
       </c>
+      <c r="BX31" s="114" t="s">
+        <v>277</v>
+      </c>
     </row>
-    <row r="32" spans="1:75" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:76" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A32" s="16">
         <v>29</v>
       </c>
-      <c r="B32" s="113" t="s">
+      <c r="B32" s="16" t="s">
         <v>56</v>
       </c>
       <c r="C32" s="16">
@@ -10197,11 +10435,14 @@
         <f t="shared" si="43"/>
         <v>Highly Satisfactory</v>
       </c>
-      <c r="BW32" s="95" t="s">
+      <c r="BW32" s="111" t="s">
         <v>245</v>
       </c>
+      <c r="BX32" s="114" t="s">
+        <v>278</v>
+      </c>
     </row>
-    <row r="33" spans="1:75" x14ac:dyDescent="0.25">
+    <row r="33" spans="1:76" x14ac:dyDescent="0.25">
       <c r="A33" s="16">
         <v>30</v>
       </c>
@@ -10469,11 +10710,14 @@
         <f t="shared" si="43"/>
         <v>Excellent</v>
       </c>
-      <c r="BW33" s="95" t="s">
+      <c r="BW33" s="111" t="s">
         <v>180</v>
       </c>
+      <c r="BX33" s="114" t="s">
+        <v>279</v>
+      </c>
     </row>
-    <row r="34" spans="1:75" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="34" spans="1:76" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A34" s="16">
         <v>31</v>
       </c>
@@ -10741,11 +10985,14 @@
         <f t="shared" si="43"/>
         <v>Highly Satisfactory</v>
       </c>
-      <c r="BW34" s="95" t="s">
+      <c r="BW34" s="111" t="s">
         <v>181</v>
       </c>
+      <c r="BX34" s="114" t="s">
+        <v>280</v>
+      </c>
     </row>
-    <row r="35" spans="1:75" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="35" spans="1:76" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A35" s="16">
         <v>32</v>
       </c>
@@ -11013,11 +11260,14 @@
         <f t="shared" si="43"/>
         <v>Excellent</v>
       </c>
-      <c r="BW35" s="97" t="s">
+      <c r="BW35" s="112" t="s">
         <v>182</v>
       </c>
+      <c r="BX35" s="114" t="s">
+        <v>281</v>
+      </c>
     </row>
-    <row r="36" spans="1:75" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="36" spans="1:76" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A36" s="16">
         <v>33</v>
       </c>
@@ -11285,11 +11535,14 @@
         <f t="shared" si="43"/>
         <v>Excellent</v>
       </c>
-      <c r="BW36" s="95" t="s">
+      <c r="BW36" s="111" t="s">
         <v>246</v>
       </c>
+      <c r="BX36" s="114" t="s">
+        <v>282</v>
+      </c>
     </row>
-    <row r="37" spans="1:75" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="37" spans="1:76" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A37" s="16">
         <v>34</v>
       </c>
@@ -11557,11 +11810,14 @@
         <f t="shared" si="43"/>
         <v>Excellent</v>
       </c>
-      <c r="BW37" s="97" t="s">
+      <c r="BW37" s="112" t="s">
         <v>183</v>
       </c>
+      <c r="BX37" s="114" t="s">
+        <v>283</v>
+      </c>
     </row>
-    <row r="38" spans="1:75" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="38" spans="1:76" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A38" s="16">
         <v>35</v>
       </c>
@@ -11829,11 +12085,14 @@
         <f t="shared" si="43"/>
         <v>Excellent</v>
       </c>
-      <c r="BW38" s="95" t="s">
+      <c r="BW38" s="111" t="s">
         <v>184</v>
       </c>
+      <c r="BX38" s="114" t="s">
+        <v>284</v>
+      </c>
     </row>
-    <row r="39" spans="1:75" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="39" spans="1:76" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A39" s="16">
         <v>36</v>
       </c>
@@ -12101,11 +12360,14 @@
         <f t="shared" si="43"/>
         <v>Highly Satisfactory</v>
       </c>
-      <c r="BW39" s="95" t="s">
+      <c r="BW39" s="111" t="s">
         <v>185</v>
       </c>
+      <c r="BX39" s="114" t="s">
+        <v>285</v>
+      </c>
     </row>
-    <row r="40" spans="1:75" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="40" spans="1:76" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A40" s="16">
         <v>37</v>
       </c>
@@ -12372,11 +12634,14 @@
         <f t="shared" si="43"/>
         <v>Highly Satisfactory</v>
       </c>
-      <c r="BW40" s="95" t="s">
+      <c r="BW40" s="111" t="s">
         <v>194</v>
       </c>
+      <c r="BX40" s="114" t="s">
+        <v>286</v>
+      </c>
     </row>
-    <row r="41" spans="1:75" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="41" spans="1:76" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A41" s="16">
         <v>38</v>
       </c>
@@ -12644,11 +12909,14 @@
         <f t="shared" si="43"/>
         <v>Excellent</v>
       </c>
-      <c r="BW41" s="95" t="s">
+      <c r="BW41" s="111" t="s">
         <v>186</v>
       </c>
+      <c r="BX41" s="114" t="s">
+        <v>287</v>
+      </c>
     </row>
-    <row r="42" spans="1:75" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="42" spans="1:76" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A42" s="16">
         <v>39</v>
       </c>
@@ -12916,11 +13184,14 @@
         <f t="shared" si="43"/>
         <v>Excellent</v>
       </c>
-      <c r="BW42" s="95" t="s">
+      <c r="BW42" s="111" t="s">
         <v>187</v>
       </c>
+      <c r="BX42" s="114" t="s">
+        <v>288</v>
+      </c>
     </row>
-    <row r="43" spans="1:75" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="43" spans="1:76" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A43" s="16">
         <v>40</v>
       </c>
@@ -13188,11 +13459,14 @@
         <f t="shared" si="43"/>
         <v>Excellent</v>
       </c>
-      <c r="BW43" s="95" t="s">
+      <c r="BW43" s="111" t="s">
         <v>188</v>
       </c>
+      <c r="BX43" s="114" t="s">
+        <v>289</v>
+      </c>
     </row>
-    <row r="44" spans="1:75" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="44" spans="1:76" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A44" s="16">
         <v>41</v>
       </c>
@@ -13460,11 +13734,14 @@
         <f t="shared" si="43"/>
         <v>Highly Satisfactory</v>
       </c>
-      <c r="BW44" s="95" t="s">
+      <c r="BW44" s="111" t="s">
         <v>247</v>
       </c>
+      <c r="BX44" s="114" t="s">
+        <v>290</v>
+      </c>
     </row>
-    <row r="45" spans="1:75" x14ac:dyDescent="0.25">
+    <row r="45" spans="1:76" x14ac:dyDescent="0.25">
       <c r="A45" s="16">
         <v>42</v>
       </c>
@@ -13732,11 +14009,14 @@
         <f t="shared" si="43"/>
         <v>Excellent</v>
       </c>
-      <c r="BW45" s="95" t="s">
+      <c r="BW45" s="111" t="s">
         <v>189</v>
       </c>
+      <c r="BX45" s="114" t="s">
+        <v>291</v>
+      </c>
     </row>
-    <row r="46" spans="1:75" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="46" spans="1:76" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A46" s="16">
         <v>43</v>
       </c>
@@ -14004,11 +14284,14 @@
         <f t="shared" si="43"/>
         <v>Excellent</v>
       </c>
-      <c r="BW46" s="95" t="s">
+      <c r="BW46" s="111" t="s">
         <v>190</v>
       </c>
+      <c r="BX46" s="114" t="s">
+        <v>292</v>
+      </c>
     </row>
-    <row r="47" spans="1:75" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="47" spans="1:76" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A47" s="16">
         <v>44</v>
       </c>
@@ -14276,12 +14559,35 @@
         <f t="shared" si="43"/>
         <v>Highly Satisfactory</v>
       </c>
-      <c r="BW47" s="97" t="s">
+      <c r="BW47" s="112" t="s">
         <v>191</v>
+      </c>
+      <c r="BX47" s="114" t="s">
+        <v>293</v>
       </c>
     </row>
   </sheetData>
-  <mergeCells count="29">
+  <mergeCells count="30">
+    <mergeCell ref="BX1:BX2"/>
+    <mergeCell ref="BU1:BU2"/>
+    <mergeCell ref="BV1:BV2"/>
+    <mergeCell ref="BW1:BW2"/>
+    <mergeCell ref="BO1:BO2"/>
+    <mergeCell ref="BP1:BP2"/>
+    <mergeCell ref="BQ1:BQ2"/>
+    <mergeCell ref="BT1:BT2"/>
+    <mergeCell ref="S1:W1"/>
+    <mergeCell ref="X1:AB1"/>
+    <mergeCell ref="AC1:AG1"/>
+    <mergeCell ref="AH1:AL1"/>
+    <mergeCell ref="BL1:BL2"/>
+    <mergeCell ref="BN1:BN2"/>
+    <mergeCell ref="AM1:AQ1"/>
+    <mergeCell ref="AR1:AV1"/>
+    <mergeCell ref="AW1:BA1"/>
+    <mergeCell ref="BB1:BF1"/>
+    <mergeCell ref="BG1:BK1"/>
+    <mergeCell ref="BM1:BM2"/>
     <mergeCell ref="N1:R1"/>
     <mergeCell ref="A1:A2"/>
     <mergeCell ref="B1:B2"/>
@@ -14292,25 +14598,6 @@
     <mergeCell ref="F1:F2"/>
     <mergeCell ref="G1:G2"/>
     <mergeCell ref="H1:H2"/>
-    <mergeCell ref="BN1:BN2"/>
-    <mergeCell ref="AM1:AQ1"/>
-    <mergeCell ref="AR1:AV1"/>
-    <mergeCell ref="AW1:BA1"/>
-    <mergeCell ref="BB1:BF1"/>
-    <mergeCell ref="BG1:BK1"/>
-    <mergeCell ref="BM1:BM2"/>
-    <mergeCell ref="S1:W1"/>
-    <mergeCell ref="X1:AB1"/>
-    <mergeCell ref="AC1:AG1"/>
-    <mergeCell ref="AH1:AL1"/>
-    <mergeCell ref="BL1:BL2"/>
-    <mergeCell ref="BU1:BU2"/>
-    <mergeCell ref="BV1:BV2"/>
-    <mergeCell ref="BW1:BW2"/>
-    <mergeCell ref="BO1:BO2"/>
-    <mergeCell ref="BP1:BP2"/>
-    <mergeCell ref="BQ1:BQ2"/>
-    <mergeCell ref="BT1:BT2"/>
   </mergeCells>
   <phoneticPr fontId="13" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
penamabahan data yang belum
</commit_message>
<xml_diff>
--- a/Ners/2023-2024/Transkip Nilai Ners 2023-2024.xlsx
+++ b/Ners/2023-2024/Transkip Nilai Ners 2023-2024.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Nando\Documents\Stikes\Transkip Nilai 2025\Ners\2023-2024\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A03190A8-A1A0-4713-B0CB-85BB637E0513}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5C560498-2C0E-49FE-93DF-1B833AD8E499}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{435B60B8-694F-4DDA-ADD2-15262503367A}"/>
   </bookViews>
@@ -1447,34 +1447,23 @@
     <xf numFmtId="0" fontId="11" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="15" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="49" fontId="1" fillId="2" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="9" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="10" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="1" fillId="11" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="12" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="13" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="14" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="5" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -1489,19 +1478,30 @@
     <xf numFmtId="0" fontId="1" fillId="8" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="1" fillId="9" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="11" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="15" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="1" fillId="10" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="12" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="13" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="14" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="1" fillId="2" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
   </cellXfs>
   <cellStyles count="3">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -1821,10 +1821,10 @@
   <dimension ref="A1:BX47"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <pane xSplit="2" ySplit="2" topLeftCell="C24" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="2" ySplit="2" topLeftCell="C21" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="C1" sqref="C1"/>
       <selection pane="bottomLeft" activeCell="A3" sqref="A3"/>
-      <selection pane="bottomRight" activeCell="I46" sqref="I46"/>
+      <selection pane="bottomRight" activeCell="E42" sqref="E42"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1859,79 +1859,79 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:76" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A1" s="97" t="s">
+      <c r="A1" s="101" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="97" t="s">
+      <c r="B1" s="101" t="s">
         <v>1</v>
       </c>
-      <c r="C1" s="97" t="s">
+      <c r="C1" s="101" t="s">
         <v>2</v>
       </c>
-      <c r="D1" s="97" t="s">
-        <v>3</v>
-      </c>
-      <c r="E1" s="97" t="s">
+      <c r="D1" s="101" t="s">
+        <v>3</v>
+      </c>
+      <c r="E1" s="101" t="s">
         <v>73</v>
       </c>
-      <c r="F1" s="99" t="s">
+      <c r="F1" s="114" t="s">
         <v>74</v>
       </c>
-      <c r="G1" s="99" t="s">
+      <c r="G1" s="114" t="s">
         <v>75</v>
       </c>
-      <c r="H1" s="97" t="s">
+      <c r="H1" s="101" t="s">
         <v>76</v>
       </c>
-      <c r="I1" s="98" t="s">
-        <v>4</v>
-      </c>
-      <c r="J1" s="98"/>
-      <c r="K1" s="98"/>
-      <c r="L1" s="98"/>
-      <c r="M1" s="98"/>
-      <c r="N1" s="96" t="s">
+      <c r="I1" s="113" t="s">
+        <v>4</v>
+      </c>
+      <c r="J1" s="113"/>
+      <c r="K1" s="113"/>
+      <c r="L1" s="113"/>
+      <c r="M1" s="113"/>
+      <c r="N1" s="112" t="s">
         <v>5</v>
       </c>
-      <c r="O1" s="96"/>
-      <c r="P1" s="96"/>
-      <c r="Q1" s="96"/>
-      <c r="R1" s="96"/>
-      <c r="S1" s="106" t="s">
+      <c r="O1" s="112"/>
+      <c r="P1" s="112"/>
+      <c r="Q1" s="112"/>
+      <c r="R1" s="112"/>
+      <c r="S1" s="103" t="s">
         <v>6</v>
       </c>
-      <c r="T1" s="106"/>
-      <c r="U1" s="106"/>
-      <c r="V1" s="106"/>
-      <c r="W1" s="106"/>
-      <c r="X1" s="107" t="s">
+      <c r="T1" s="103"/>
+      <c r="U1" s="103"/>
+      <c r="V1" s="103"/>
+      <c r="W1" s="103"/>
+      <c r="X1" s="104" t="s">
         <v>7</v>
       </c>
-      <c r="Y1" s="107"/>
-      <c r="Z1" s="107"/>
-      <c r="AA1" s="107"/>
-      <c r="AB1" s="107"/>
-      <c r="AC1" s="108" t="s">
+      <c r="Y1" s="104"/>
+      <c r="Z1" s="104"/>
+      <c r="AA1" s="104"/>
+      <c r="AB1" s="104"/>
+      <c r="AC1" s="105" t="s">
         <v>8</v>
       </c>
-      <c r="AD1" s="108"/>
-      <c r="AE1" s="108"/>
-      <c r="AF1" s="108"/>
-      <c r="AG1" s="108"/>
-      <c r="AH1" s="109" t="s">
+      <c r="AD1" s="105"/>
+      <c r="AE1" s="105"/>
+      <c r="AF1" s="105"/>
+      <c r="AG1" s="105"/>
+      <c r="AH1" s="106" t="s">
         <v>9</v>
       </c>
-      <c r="AI1" s="109"/>
-      <c r="AJ1" s="109"/>
-      <c r="AK1" s="109"/>
-      <c r="AL1" s="109"/>
-      <c r="AM1" s="101" t="s">
+      <c r="AI1" s="106"/>
+      <c r="AJ1" s="106"/>
+      <c r="AK1" s="106"/>
+      <c r="AL1" s="106"/>
+      <c r="AM1" s="108" t="s">
         <v>13</v>
       </c>
-      <c r="AN1" s="101"/>
-      <c r="AO1" s="101"/>
-      <c r="AP1" s="101"/>
-      <c r="AQ1" s="101"/>
+      <c r="AN1" s="108"/>
+      <c r="AO1" s="108"/>
+      <c r="AP1" s="108"/>
+      <c r="AQ1" s="108"/>
       <c r="AR1" s="102" t="s">
         <v>14</v>
       </c>
@@ -1939,43 +1939,43 @@
       <c r="AT1" s="102"/>
       <c r="AU1" s="102"/>
       <c r="AV1" s="102"/>
-      <c r="AW1" s="103" t="s">
+      <c r="AW1" s="109" t="s">
         <v>15</v>
       </c>
-      <c r="AX1" s="103"/>
-      <c r="AY1" s="103"/>
-      <c r="AZ1" s="103"/>
-      <c r="BA1" s="103"/>
-      <c r="BB1" s="104" t="s">
+      <c r="AX1" s="109"/>
+      <c r="AY1" s="109"/>
+      <c r="AZ1" s="109"/>
+      <c r="BA1" s="109"/>
+      <c r="BB1" s="110" t="s">
         <v>16</v>
       </c>
-      <c r="BC1" s="104"/>
-      <c r="BD1" s="104"/>
-      <c r="BE1" s="104"/>
-      <c r="BF1" s="104"/>
-      <c r="BG1" s="105" t="s">
+      <c r="BC1" s="110"/>
+      <c r="BD1" s="110"/>
+      <c r="BE1" s="110"/>
+      <c r="BF1" s="110"/>
+      <c r="BG1" s="111" t="s">
         <v>17</v>
       </c>
-      <c r="BH1" s="105"/>
-      <c r="BI1" s="105"/>
-      <c r="BJ1" s="105"/>
-      <c r="BK1" s="105"/>
-      <c r="BL1" s="100" t="s">
+      <c r="BH1" s="111"/>
+      <c r="BI1" s="111"/>
+      <c r="BJ1" s="111"/>
+      <c r="BK1" s="111"/>
+      <c r="BL1" s="107" t="s">
         <v>10</v>
       </c>
-      <c r="BM1" s="100" t="s">
+      <c r="BM1" s="107" t="s">
         <v>11</v>
       </c>
-      <c r="BN1" s="100" t="s">
+      <c r="BN1" s="107" t="s">
         <v>12</v>
       </c>
-      <c r="BO1" s="97" t="s">
+      <c r="BO1" s="101" t="s">
         <v>10</v>
       </c>
-      <c r="BP1" s="97" t="s">
+      <c r="BP1" s="101" t="s">
         <v>11</v>
       </c>
-      <c r="BQ1" s="97" t="s">
+      <c r="BQ1" s="101" t="s">
         <v>12</v>
       </c>
       <c r="BR1" s="2" t="s">
@@ -1987,28 +1987,28 @@
       <c r="BT1" s="102" t="s">
         <v>19</v>
       </c>
-      <c r="BU1" s="110" t="s">
+      <c r="BU1" s="100" t="s">
         <v>77</v>
       </c>
-      <c r="BV1" s="110" t="s">
+      <c r="BV1" s="100" t="s">
         <v>78</v>
       </c>
-      <c r="BW1" s="110" t="s">
+      <c r="BW1" s="100" t="s">
         <v>79</v>
       </c>
-      <c r="BX1" s="113" t="s">
+      <c r="BX1" s="99" t="s">
         <v>248</v>
       </c>
     </row>
     <row r="2" spans="1:76" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A2" s="97"/>
-      <c r="B2" s="97"/>
-      <c r="C2" s="97"/>
-      <c r="D2" s="97"/>
-      <c r="E2" s="97"/>
-      <c r="F2" s="99"/>
-      <c r="G2" s="99"/>
-      <c r="H2" s="97"/>
+      <c r="A2" s="101"/>
+      <c r="B2" s="101"/>
+      <c r="C2" s="101"/>
+      <c r="D2" s="101"/>
+      <c r="E2" s="101"/>
+      <c r="F2" s="114"/>
+      <c r="G2" s="114"/>
+      <c r="H2" s="101"/>
       <c r="I2" s="7" t="s">
         <v>20</v>
       </c>
@@ -2174,12 +2174,12 @@
       <c r="BK2" s="5" t="s">
         <v>24</v>
       </c>
-      <c r="BL2" s="100"/>
-      <c r="BM2" s="100"/>
-      <c r="BN2" s="100"/>
-      <c r="BO2" s="97"/>
-      <c r="BP2" s="97"/>
-      <c r="BQ2" s="97"/>
+      <c r="BL2" s="107"/>
+      <c r="BM2" s="107"/>
+      <c r="BN2" s="107"/>
+      <c r="BO2" s="101"/>
+      <c r="BP2" s="101"/>
+      <c r="BQ2" s="101"/>
       <c r="BR2" s="2" t="s">
         <v>20</v>
       </c>
@@ -2187,10 +2187,10 @@
         <v>25</v>
       </c>
       <c r="BT2" s="102"/>
-      <c r="BU2" s="110"/>
-      <c r="BV2" s="110"/>
-      <c r="BW2" s="110"/>
-      <c r="BX2" s="113"/>
+      <c r="BU2" s="100"/>
+      <c r="BV2" s="100"/>
+      <c r="BW2" s="100"/>
+      <c r="BX2" s="99"/>
     </row>
     <row r="3" spans="1:76" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A3" s="16">
@@ -2460,10 +2460,10 @@
         <f>IF(BT3&gt;=3.51,"Excellent",(IF(BT3&gt;=2.75,"Highly Satisfactory",(IF(BT3&gt;=2,"Satisfactory","FAILED")))))</f>
         <v>Highly Satisfactory</v>
       </c>
-      <c r="BW3" s="111" t="s">
+      <c r="BW3" s="96" t="s">
         <v>155</v>
       </c>
-      <c r="BX3" s="114" t="s">
+      <c r="BX3" s="98" t="s">
         <v>249</v>
       </c>
     </row>
@@ -2735,10 +2735,10 @@
         <f t="shared" ref="BV4:BV47" si="43">IF(BT4&gt;=3.51,"Excellent",(IF(BT4&gt;=2.75,"Highly Satisfactory",(IF(BT4&gt;=2,"Satisfactory","FAILED")))))</f>
         <v>Highly Satisfactory</v>
       </c>
-      <c r="BW4" s="111" t="s">
+      <c r="BW4" s="96" t="s">
         <v>156</v>
       </c>
-      <c r="BX4" s="114" t="s">
+      <c r="BX4" s="98" t="s">
         <v>250</v>
       </c>
     </row>
@@ -3010,10 +3010,10 @@
         <f t="shared" si="43"/>
         <v>Excellent</v>
       </c>
-      <c r="BW5" s="111" t="s">
+      <c r="BW5" s="96" t="s">
         <v>199</v>
       </c>
-      <c r="BX5" s="114" t="s">
+      <c r="BX5" s="98" t="s">
         <v>251</v>
       </c>
     </row>
@@ -3285,10 +3285,10 @@
         <f t="shared" si="43"/>
         <v>Excellent</v>
       </c>
-      <c r="BW6" s="111" t="s">
+      <c r="BW6" s="96" t="s">
         <v>157</v>
       </c>
-      <c r="BX6" s="114" t="s">
+      <c r="BX6" s="98" t="s">
         <v>252</v>
       </c>
     </row>
@@ -3560,10 +3560,10 @@
         <f t="shared" si="43"/>
         <v>Excellent</v>
       </c>
-      <c r="BW7" s="111" t="s">
+      <c r="BW7" s="96" t="s">
         <v>158</v>
       </c>
-      <c r="BX7" s="114" t="s">
+      <c r="BX7" s="98" t="s">
         <v>253</v>
       </c>
     </row>
@@ -3835,10 +3835,10 @@
         <f t="shared" si="43"/>
         <v>Highly Satisfactory</v>
       </c>
-      <c r="BW8" s="111" t="s">
+      <c r="BW8" s="96" t="s">
         <v>159</v>
       </c>
-      <c r="BX8" s="114" t="s">
+      <c r="BX8" s="98" t="s">
         <v>254</v>
       </c>
     </row>
@@ -4110,10 +4110,10 @@
         <f t="shared" si="43"/>
         <v>Excellent</v>
       </c>
-      <c r="BW9" s="111" t="s">
+      <c r="BW9" s="96" t="s">
         <v>160</v>
       </c>
-      <c r="BX9" s="114" t="s">
+      <c r="BX9" s="98" t="s">
         <v>255</v>
       </c>
     </row>
@@ -4385,10 +4385,10 @@
         <f t="shared" si="43"/>
         <v>Highly Satisfactory</v>
       </c>
-      <c r="BW10" s="111" t="s">
+      <c r="BW10" s="96" t="s">
         <v>192</v>
       </c>
-      <c r="BX10" s="114" t="s">
+      <c r="BX10" s="98" t="s">
         <v>256</v>
       </c>
     </row>
@@ -4660,10 +4660,10 @@
         <f t="shared" si="43"/>
         <v>Highly Satisfactory</v>
       </c>
-      <c r="BW11" s="111" t="s">
+      <c r="BW11" s="96" t="s">
         <v>161</v>
       </c>
-      <c r="BX11" s="114" t="s">
+      <c r="BX11" s="98" t="s">
         <v>257</v>
       </c>
     </row>
@@ -4935,10 +4935,10 @@
         <f t="shared" si="43"/>
         <v>Highly Satisfactory</v>
       </c>
-      <c r="BW12" s="111" t="s">
+      <c r="BW12" s="96" t="s">
         <v>162</v>
       </c>
-      <c r="BX12" s="114" t="s">
+      <c r="BX12" s="98" t="s">
         <v>258</v>
       </c>
     </row>
@@ -5210,10 +5210,10 @@
         <f t="shared" si="43"/>
         <v>Highly Satisfactory</v>
       </c>
-      <c r="BW13" s="111" t="s">
+      <c r="BW13" s="96" t="s">
         <v>163</v>
       </c>
-      <c r="BX13" s="114" t="s">
+      <c r="BX13" s="98" t="s">
         <v>259</v>
       </c>
     </row>
@@ -5485,10 +5485,10 @@
         <f t="shared" si="43"/>
         <v>Highly Satisfactory</v>
       </c>
-      <c r="BW14" s="111" t="s">
+      <c r="BW14" s="96" t="s">
         <v>164</v>
       </c>
-      <c r="BX14" s="114" t="s">
+      <c r="BX14" s="98" t="s">
         <v>260</v>
       </c>
     </row>
@@ -5760,10 +5760,10 @@
         <f t="shared" si="43"/>
         <v>Excellent</v>
       </c>
-      <c r="BW15" s="111" t="s">
+      <c r="BW15" s="96" t="s">
         <v>165</v>
       </c>
-      <c r="BX15" s="114" t="s">
+      <c r="BX15" s="98" t="s">
         <v>261</v>
       </c>
     </row>
@@ -6035,10 +6035,10 @@
         <f t="shared" si="43"/>
         <v>Highly Satisfactory</v>
       </c>
-      <c r="BW16" s="112" t="s">
+      <c r="BW16" s="97" t="s">
         <v>166</v>
       </c>
-      <c r="BX16" s="114" t="s">
+      <c r="BX16" s="98" t="s">
         <v>262</v>
       </c>
     </row>
@@ -6310,10 +6310,10 @@
         <f t="shared" si="43"/>
         <v>Highly Satisfactory</v>
       </c>
-      <c r="BW17" s="111" t="s">
+      <c r="BW17" s="96" t="s">
         <v>167</v>
       </c>
-      <c r="BX17" s="114" t="s">
+      <c r="BX17" s="98" t="s">
         <v>263</v>
       </c>
     </row>
@@ -6585,10 +6585,10 @@
         <f t="shared" si="43"/>
         <v>Highly Satisfactory</v>
       </c>
-      <c r="BW18" s="111" t="s">
+      <c r="BW18" s="96" t="s">
         <v>168</v>
       </c>
-      <c r="BX18" s="114" t="s">
+      <c r="BX18" s="98" t="s">
         <v>264</v>
       </c>
     </row>
@@ -6860,10 +6860,10 @@
         <f t="shared" si="43"/>
         <v>Highly Satisfactory</v>
       </c>
-      <c r="BW19" s="111" t="s">
+      <c r="BW19" s="96" t="s">
         <v>195</v>
       </c>
-      <c r="BX19" s="114" t="s">
+      <c r="BX19" s="98" t="s">
         <v>265</v>
       </c>
     </row>
@@ -7135,10 +7135,10 @@
         <f t="shared" si="43"/>
         <v>Highly Satisfactory</v>
       </c>
-      <c r="BW20" s="111" t="s">
+      <c r="BW20" s="96" t="s">
         <v>169</v>
       </c>
-      <c r="BX20" s="114" t="s">
+      <c r="BX20" s="98" t="s">
         <v>266</v>
       </c>
     </row>
@@ -7410,10 +7410,10 @@
         <f t="shared" si="43"/>
         <v>Highly Satisfactory</v>
       </c>
-      <c r="BW21" s="112" t="s">
+      <c r="BW21" s="97" t="s">
         <v>170</v>
       </c>
-      <c r="BX21" s="114" t="s">
+      <c r="BX21" s="98" t="s">
         <v>267</v>
       </c>
     </row>
@@ -7685,10 +7685,10 @@
         <f t="shared" si="43"/>
         <v>Excellent</v>
       </c>
-      <c r="BW22" s="111" t="s">
+      <c r="BW22" s="96" t="s">
         <v>171</v>
       </c>
-      <c r="BX22" s="114" t="s">
+      <c r="BX22" s="98" t="s">
         <v>268</v>
       </c>
     </row>
@@ -7960,10 +7960,10 @@
         <f t="shared" si="43"/>
         <v>Highly Satisfactory</v>
       </c>
-      <c r="BW23" s="111" t="s">
+      <c r="BW23" s="96" t="s">
         <v>172</v>
       </c>
-      <c r="BX23" s="114" t="s">
+      <c r="BX23" s="98" t="s">
         <v>269</v>
       </c>
     </row>
@@ -8235,10 +8235,10 @@
         <f t="shared" si="43"/>
         <v>Highly Satisfactory</v>
       </c>
-      <c r="BW24" s="111" t="s">
+      <c r="BW24" s="96" t="s">
         <v>173</v>
       </c>
-      <c r="BX24" s="114" t="s">
+      <c r="BX24" s="98" t="s">
         <v>270</v>
       </c>
     </row>
@@ -8510,10 +8510,10 @@
         <f t="shared" si="43"/>
         <v>Excellent</v>
       </c>
-      <c r="BW25" s="111" t="s">
+      <c r="BW25" s="96" t="s">
         <v>174</v>
       </c>
-      <c r="BX25" s="114" t="s">
+      <c r="BX25" s="98" t="s">
         <v>271</v>
       </c>
     </row>
@@ -8785,10 +8785,10 @@
         <f t="shared" si="43"/>
         <v>Highly Satisfactory</v>
       </c>
-      <c r="BW26" s="111" t="s">
+      <c r="BW26" s="96" t="s">
         <v>175</v>
       </c>
-      <c r="BX26" s="114" t="s">
+      <c r="BX26" s="98" t="s">
         <v>272</v>
       </c>
     </row>
@@ -9060,10 +9060,10 @@
         <f t="shared" si="43"/>
         <v>Excellent</v>
       </c>
-      <c r="BW27" s="111" t="s">
+      <c r="BW27" s="96" t="s">
         <v>176</v>
       </c>
-      <c r="BX27" s="114" t="s">
+      <c r="BX27" s="98" t="s">
         <v>273</v>
       </c>
     </row>
@@ -9335,10 +9335,10 @@
         <f t="shared" si="43"/>
         <v>Highly Satisfactory</v>
       </c>
-      <c r="BW28" s="111" t="s">
+      <c r="BW28" s="96" t="s">
         <v>177</v>
       </c>
-      <c r="BX28" s="114" t="s">
+      <c r="BX28" s="98" t="s">
         <v>274</v>
       </c>
     </row>
@@ -9610,10 +9610,10 @@
         <f t="shared" si="43"/>
         <v>Excellent</v>
       </c>
-      <c r="BW29" s="111" t="s">
+      <c r="BW29" s="96" t="s">
         <v>178</v>
       </c>
-      <c r="BX29" s="114" t="s">
+      <c r="BX29" s="98" t="s">
         <v>275</v>
       </c>
     </row>
@@ -9885,10 +9885,10 @@
         <f t="shared" si="43"/>
         <v>Highly Satisfactory</v>
       </c>
-      <c r="BW30" s="111" t="s">
+      <c r="BW30" s="96" t="s">
         <v>196</v>
       </c>
-      <c r="BX30" s="114" t="s">
+      <c r="BX30" s="98" t="s">
         <v>276</v>
       </c>
     </row>
@@ -10160,10 +10160,10 @@
         <f t="shared" si="43"/>
         <v>Highly Satisfactory</v>
       </c>
-      <c r="BW31" s="111" t="s">
+      <c r="BW31" s="96" t="s">
         <v>179</v>
       </c>
-      <c r="BX31" s="114" t="s">
+      <c r="BX31" s="98" t="s">
         <v>277</v>
       </c>
     </row>
@@ -10435,10 +10435,10 @@
         <f t="shared" si="43"/>
         <v>Highly Satisfactory</v>
       </c>
-      <c r="BW32" s="111" t="s">
+      <c r="BW32" s="96" t="s">
         <v>245</v>
       </c>
-      <c r="BX32" s="114" t="s">
+      <c r="BX32" s="98" t="s">
         <v>278</v>
       </c>
     </row>
@@ -10710,10 +10710,10 @@
         <f t="shared" si="43"/>
         <v>Excellent</v>
       </c>
-      <c r="BW33" s="111" t="s">
+      <c r="BW33" s="96" t="s">
         <v>180</v>
       </c>
-      <c r="BX33" s="114" t="s">
+      <c r="BX33" s="98" t="s">
         <v>279</v>
       </c>
     </row>
@@ -10985,10 +10985,10 @@
         <f t="shared" si="43"/>
         <v>Highly Satisfactory</v>
       </c>
-      <c r="BW34" s="111" t="s">
+      <c r="BW34" s="96" t="s">
         <v>181</v>
       </c>
-      <c r="BX34" s="114" t="s">
+      <c r="BX34" s="98" t="s">
         <v>280</v>
       </c>
     </row>
@@ -11260,10 +11260,10 @@
         <f t="shared" si="43"/>
         <v>Excellent</v>
       </c>
-      <c r="BW35" s="112" t="s">
+      <c r="BW35" s="97" t="s">
         <v>182</v>
       </c>
-      <c r="BX35" s="114" t="s">
+      <c r="BX35" s="98" t="s">
         <v>281</v>
       </c>
     </row>
@@ -11535,10 +11535,10 @@
         <f t="shared" si="43"/>
         <v>Excellent</v>
       </c>
-      <c r="BW36" s="111" t="s">
+      <c r="BW36" s="96" t="s">
         <v>246</v>
       </c>
-      <c r="BX36" s="114" t="s">
+      <c r="BX36" s="98" t="s">
         <v>282</v>
       </c>
     </row>
@@ -11810,10 +11810,10 @@
         <f t="shared" si="43"/>
         <v>Excellent</v>
       </c>
-      <c r="BW37" s="112" t="s">
+      <c r="BW37" s="97" t="s">
         <v>183</v>
       </c>
-      <c r="BX37" s="114" t="s">
+      <c r="BX37" s="98" t="s">
         <v>283</v>
       </c>
     </row>
@@ -12085,10 +12085,10 @@
         <f t="shared" si="43"/>
         <v>Excellent</v>
       </c>
-      <c r="BW38" s="111" t="s">
+      <c r="BW38" s="96" t="s">
         <v>184</v>
       </c>
-      <c r="BX38" s="114" t="s">
+      <c r="BX38" s="98" t="s">
         <v>284</v>
       </c>
     </row>
@@ -12360,10 +12360,10 @@
         <f t="shared" si="43"/>
         <v>Highly Satisfactory</v>
       </c>
-      <c r="BW39" s="111" t="s">
+      <c r="BW39" s="96" t="s">
         <v>185</v>
       </c>
-      <c r="BX39" s="114" t="s">
+      <c r="BX39" s="98" t="s">
         <v>285</v>
       </c>
     </row>
@@ -12634,10 +12634,10 @@
         <f t="shared" si="43"/>
         <v>Highly Satisfactory</v>
       </c>
-      <c r="BW40" s="111" t="s">
+      <c r="BW40" s="96" t="s">
         <v>194</v>
       </c>
-      <c r="BX40" s="114" t="s">
+      <c r="BX40" s="98" t="s">
         <v>286</v>
       </c>
     </row>
@@ -12909,10 +12909,10 @@
         <f t="shared" si="43"/>
         <v>Excellent</v>
       </c>
-      <c r="BW41" s="111" t="s">
+      <c r="BW41" s="96" t="s">
         <v>186</v>
       </c>
-      <c r="BX41" s="114" t="s">
+      <c r="BX41" s="98" t="s">
         <v>287</v>
       </c>
     </row>
@@ -13184,10 +13184,10 @@
         <f t="shared" si="43"/>
         <v>Excellent</v>
       </c>
-      <c r="BW42" s="111" t="s">
+      <c r="BW42" s="96" t="s">
         <v>187</v>
       </c>
-      <c r="BX42" s="114" t="s">
+      <c r="BX42" s="98" t="s">
         <v>288</v>
       </c>
     </row>
@@ -13459,10 +13459,10 @@
         <f t="shared" si="43"/>
         <v>Excellent</v>
       </c>
-      <c r="BW43" s="111" t="s">
+      <c r="BW43" s="96" t="s">
         <v>188</v>
       </c>
-      <c r="BX43" s="114" t="s">
+      <c r="BX43" s="98" t="s">
         <v>289</v>
       </c>
     </row>
@@ -13734,10 +13734,10 @@
         <f t="shared" si="43"/>
         <v>Highly Satisfactory</v>
       </c>
-      <c r="BW44" s="111" t="s">
+      <c r="BW44" s="96" t="s">
         <v>247</v>
       </c>
-      <c r="BX44" s="114" t="s">
+      <c r="BX44" s="98" t="s">
         <v>290</v>
       </c>
     </row>
@@ -14009,10 +14009,10 @@
         <f t="shared" si="43"/>
         <v>Excellent</v>
       </c>
-      <c r="BW45" s="111" t="s">
+      <c r="BW45" s="96" t="s">
         <v>189</v>
       </c>
-      <c r="BX45" s="114" t="s">
+      <c r="BX45" s="98" t="s">
         <v>291</v>
       </c>
     </row>
@@ -14284,10 +14284,10 @@
         <f t="shared" si="43"/>
         <v>Excellent</v>
       </c>
-      <c r="BW46" s="111" t="s">
+      <c r="BW46" s="96" t="s">
         <v>190</v>
       </c>
-      <c r="BX46" s="114" t="s">
+      <c r="BX46" s="98" t="s">
         <v>292</v>
       </c>
     </row>
@@ -14559,35 +14559,15 @@
         <f t="shared" si="43"/>
         <v>Highly Satisfactory</v>
       </c>
-      <c r="BW47" s="112" t="s">
+      <c r="BW47" s="97" t="s">
         <v>191</v>
       </c>
-      <c r="BX47" s="114" t="s">
+      <c r="BX47" s="98" t="s">
         <v>293</v>
       </c>
     </row>
   </sheetData>
   <mergeCells count="30">
-    <mergeCell ref="BX1:BX2"/>
-    <mergeCell ref="BU1:BU2"/>
-    <mergeCell ref="BV1:BV2"/>
-    <mergeCell ref="BW1:BW2"/>
-    <mergeCell ref="BO1:BO2"/>
-    <mergeCell ref="BP1:BP2"/>
-    <mergeCell ref="BQ1:BQ2"/>
-    <mergeCell ref="BT1:BT2"/>
-    <mergeCell ref="S1:W1"/>
-    <mergeCell ref="X1:AB1"/>
-    <mergeCell ref="AC1:AG1"/>
-    <mergeCell ref="AH1:AL1"/>
-    <mergeCell ref="BL1:BL2"/>
-    <mergeCell ref="BN1:BN2"/>
-    <mergeCell ref="AM1:AQ1"/>
-    <mergeCell ref="AR1:AV1"/>
-    <mergeCell ref="AW1:BA1"/>
-    <mergeCell ref="BB1:BF1"/>
-    <mergeCell ref="BG1:BK1"/>
-    <mergeCell ref="BM1:BM2"/>
     <mergeCell ref="N1:R1"/>
     <mergeCell ref="A1:A2"/>
     <mergeCell ref="B1:B2"/>
@@ -14598,6 +14578,26 @@
     <mergeCell ref="F1:F2"/>
     <mergeCell ref="G1:G2"/>
     <mergeCell ref="H1:H2"/>
+    <mergeCell ref="BN1:BN2"/>
+    <mergeCell ref="AM1:AQ1"/>
+    <mergeCell ref="AR1:AV1"/>
+    <mergeCell ref="AW1:BA1"/>
+    <mergeCell ref="BB1:BF1"/>
+    <mergeCell ref="BG1:BK1"/>
+    <mergeCell ref="BM1:BM2"/>
+    <mergeCell ref="S1:W1"/>
+    <mergeCell ref="X1:AB1"/>
+    <mergeCell ref="AC1:AG1"/>
+    <mergeCell ref="AH1:AL1"/>
+    <mergeCell ref="BL1:BL2"/>
+    <mergeCell ref="BX1:BX2"/>
+    <mergeCell ref="BU1:BU2"/>
+    <mergeCell ref="BV1:BV2"/>
+    <mergeCell ref="BW1:BW2"/>
+    <mergeCell ref="BO1:BO2"/>
+    <mergeCell ref="BP1:BP2"/>
+    <mergeCell ref="BQ1:BQ2"/>
+    <mergeCell ref="BT1:BT2"/>
   </mergeCells>
   <phoneticPr fontId="13" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>